<commit_message>
Fixed MD2, Oracle 11g/12c & Snefru-256 regex
Fixed regex for:
* MD2
* Oracle 11g/12c
* Snefru-256
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="709">
   <si>
     <t>Hash</t>
   </si>
@@ -1028,6 +1028,9 @@
     <t>MD2</t>
   </si>
   <si>
+    <t>^(\$md2\$)?[a-f0-9]{32}$/i</t>
+  </si>
+  <si>
     <t>8350e5a3e24c153df2275c9f80692773</t>
   </si>
   <si>
@@ -1349,7 +1352,7 @@
     <t>Oracle 11g/12c</t>
   </si>
   <si>
-    <t>^S:[a-f0-9]{60}$/i</t>
+    <t>^(S:)?[a-f0-9]{40}(:)?[a-f0-9]{20}$/i</t>
   </si>
   <si>
     <t>oracle11</t>
@@ -1947,6 +1950,9 @@
   </si>
   <si>
     <t>Snefru-256</t>
+  </si>
+  <si>
+    <t>^(\$snefru\$)?[a-f0-9]{64}$/i</t>
   </si>
   <si>
     <t>snefru-256</t>
@@ -2320,7 +2326,7 @@
   <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="B105" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4041,20 +4047,20 @@
         <v>336</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>178</v>
+        <v>337</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
       <c r="E94" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>178</v>
@@ -4063,38 +4069,38 @@
         <v>900</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>178</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>79</v>
@@ -4104,15 +4110,15 @@
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>45</v>
@@ -4130,7 +4136,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>277</v>
@@ -4150,209 +4156,209 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="10"/>
       <c r="E101" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C102" s="5" t="n">
         <v>9700</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E102" s="15" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="13" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C103" s="5" t="n">
         <v>9800</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C104" s="5" t="n">
         <v>9400</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C105" s="5" t="n">
         <v>9500</v>
       </c>
       <c r="E105" s="16" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C106" s="5" t="n">
         <v>9600</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="10"/>
       <c r="E107" s="7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="10"/>
       <c r="E108" s="7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C109" s="7" t="n">
         <v>131</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="9" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C110" s="7" t="n">
         <v>132</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="9" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C111" s="10" t="n">
         <v>132</v>
@@ -4365,19 +4371,19 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C112" s="7" t="n">
         <v>1731</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G112" s="8" t="s">
         <v>18</v>
@@ -4385,46 +4391,46 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C113" s="7" t="n">
         <v>1731</v>
       </c>
       <c r="D113" s="7" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="G113" s="8"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="9" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C114" s="7" t="n">
         <v>2811</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="9" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>110</v>
@@ -4433,50 +4439,50 @@
         <v>200</v>
       </c>
       <c r="D115" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="12" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C116" s="7" t="n">
         <v>300</v>
       </c>
       <c r="D116" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C117" s="7" t="n">
         <v>300</v>
       </c>
       <c r="D117" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F117" s="7"/>
       <c r="G117" s="8" t="s">
@@ -4485,17 +4491,17 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C118" s="7" t="n">
         <v>5500</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G118" s="8" t="s">
         <v>18</v>
@@ -4503,17 +4509,17 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="9" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C119" s="7" t="n">
         <v>5600</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G119" s="8" t="s">
         <v>18</v>
@@ -4521,19 +4527,19 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C120" s="7" t="n">
         <v>101</v>
       </c>
       <c r="D120" s="7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G120" s="8" t="s">
         <v>18</v>
@@ -4541,19 +4547,19 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C121" s="7" t="n">
         <v>111</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G121" s="8" t="s">
         <v>18</v>
@@ -4561,35 +4567,35 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C122" s="10"/>
       <c r="D122" s="10"/>
       <c r="E122" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C123" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G123" s="8" t="s">
         <v>18</v>
@@ -4597,27 +4603,27 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="9" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C124" s="7" t="n">
         <v>112</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="9" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B125" s="7" t="s">
         <v>110</v>
@@ -4627,33 +4633,33 @@
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F125" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C126" s="7" t="n">
         <v>21</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="9" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B127" s="7" t="s">
         <v>250</v>
@@ -4662,10 +4668,10 @@
         <v>122</v>
       </c>
       <c r="D127" s="7" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G127" s="8" t="s">
         <v>18</v>
@@ -4673,17 +4679,17 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="9" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C128" s="7" t="n">
         <v>1722</v>
       </c>
       <c r="D128" s="7"/>
       <c r="E128" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="G128" s="8" t="s">
         <v>18</v>
@@ -4691,17 +4697,17 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C129" s="7" t="n">
         <v>7100</v>
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="7" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="G129" s="8" t="s">
         <v>18</v>
@@ -4709,15 +4715,15 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10"/>
       <c r="E130" s="7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="F130" s="7"/>
       <c r="G130" s="8" t="s">
@@ -4726,89 +4732,89 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="9" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C131" s="6"/>
       <c r="E131" s="7" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="9" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C132" s="10"/>
       <c r="D132" s="10"/>
       <c r="E132" s="7" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10"/>
       <c r="E133" s="7" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F133" s="7" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C134" s="10"/>
       <c r="D134" s="10" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C135" s="5" t="n">
         <v>133</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="9" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>288</v>
@@ -4817,30 +4823,30 @@
         <v>400</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F136" s="7" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C137" s="7" t="n">
         <v>400</v>
       </c>
       <c r="D137" s="7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F137" s="7"/>
       <c r="G137" s="8" t="s">
@@ -4849,74 +4855,74 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C138" s="5" t="n">
         <v>2612</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C139" s="6"/>
       <c r="E139" s="7" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="9" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E140" s="7" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="9" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D141" s="10" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E141" s="7" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F141" s="7"/>
       <c r="G141" s="8" t="s">
@@ -4925,35 +4931,35 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="9" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C142" s="7" t="n">
         <v>7600</v>
       </c>
       <c r="D142" s="7"/>
       <c r="E142" s="7" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="9" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B143" s="7" t="s">
         <v>178</v>
       </c>
       <c r="C143" s="10"/>
       <c r="D143" s="10" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E143" s="7" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="F143" s="7"/>
       <c r="G143" s="8" t="s">
@@ -4962,7 +4968,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="9" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>181</v>
@@ -4971,10 +4977,10 @@
         <v>6000</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F144" s="7"/>
       <c r="G144" s="8" t="s">
@@ -4983,7 +4989,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="9" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B145" s="7" t="s">
         <v>231</v>
@@ -4991,7 +4997,7 @@
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
       <c r="E145" s="7" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F145" s="7"/>
       <c r="G145" s="8" t="s">
@@ -5000,15 +5006,15 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="9" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
       <c r="E146" s="7" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="F146" s="7"/>
       <c r="G146" s="8" t="s">
@@ -5017,120 +5023,120 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C147" s="10"/>
       <c r="D147" s="10"/>
       <c r="E147" s="7" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F147" s="7" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C148" s="10"/>
       <c r="D148" s="10"/>
       <c r="E148" s="7" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
       <c r="E149" s="7" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F149" s="7" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="9" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C150" s="7" t="n">
         <v>7700</v>
       </c>
       <c r="D150" s="7" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F150" s="7" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="9" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C151" s="7" t="n">
         <v>7800</v>
       </c>
       <c r="D151" s="7" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E151" s="7" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F151" s="7" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="9" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C152" s="10"/>
       <c r="D152" s="10"/>
       <c r="E152" s="7" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F152" s="7" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C153" s="5" t="n">
         <v>8900</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="G153" s="8" t="s">
         <v>11</v>
@@ -5138,7 +5144,7 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="9" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B154" s="7" t="s">
         <v>181</v>
@@ -5147,46 +5153,46 @@
         <v>100</v>
       </c>
       <c r="D154" s="10" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E154" s="7" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F154" s="7" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="9" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C155" s="10"/>
       <c r="D155" s="10" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="9" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C156" s="7" t="n">
         <v>101</v>
       </c>
       <c r="D156" s="7"/>
       <c r="E156" s="7" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G156" s="8" t="s">
         <v>18</v>
@@ -5194,7 +5200,7 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="9" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B157" s="7" t="s">
         <v>250</v>
@@ -5202,7 +5208,7 @@
       <c r="C157" s="10"/>
       <c r="D157" s="10"/>
       <c r="E157" s="7" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F157" s="7"/>
       <c r="G157" s="8" t="s">
@@ -5211,17 +5217,17 @@
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="9" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B158" s="7" t="s">
         <v>253</v>
       </c>
       <c r="C158" s="10"/>
       <c r="D158" s="10" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F158" s="7"/>
       <c r="G158" s="8" t="s">
@@ -5230,7 +5236,7 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="9" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B159" s="7" t="s">
         <v>231</v>
@@ -5239,10 +5245,10 @@
         <v>1400</v>
       </c>
       <c r="D159" s="7" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="F159" s="7"/>
       <c r="G159" s="8" t="s">
@@ -5251,37 +5257,37 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C160" s="7" t="n">
         <v>7400</v>
       </c>
       <c r="D160" s="7" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E160" s="7" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F160" s="7" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="9" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C161" s="10"/>
       <c r="D161" s="10" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E161" s="7" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="F161" s="7"/>
       <c r="G161" s="8" t="s">
@@ -5290,19 +5296,19 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="9" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C162" s="7" t="n">
         <v>1700</v>
       </c>
       <c r="D162" s="7" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E162" s="7" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F162" s="7"/>
       <c r="G162" s="8" t="s">
@@ -5311,27 +5317,27 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="9" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C163" s="7" t="n">
         <v>1800</v>
       </c>
       <c r="D163" s="7" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E163" s="7" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="9" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B164" s="7" t="s">
         <v>253</v>
@@ -5339,77 +5345,77 @@
       <c r="C164" s="6"/>
       <c r="D164" s="6"/>
       <c r="E164" s="7" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="F164" s="7" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="9" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B165" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D165" s="10" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="E165" s="7" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F165" s="7" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="9" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
       <c r="E166" s="7" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F166" s="7" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="9" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C167" s="10"/>
       <c r="D167" s="10" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="E167" s="7" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="F167" s="7" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="9" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C168" s="10"/>
       <c r="D168" s="10"/>
       <c r="E168" s="7" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="F168" s="7"/>
       <c r="G168" s="8" t="s">
@@ -5418,15 +5424,15 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="9" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C169" s="10"/>
       <c r="D169" s="10"/>
       <c r="E169" s="7" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F169" s="7"/>
       <c r="G169" s="8" t="s">
@@ -5435,15 +5441,15 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="9" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C170" s="10"/>
       <c r="D170" s="10"/>
       <c r="E170" s="7" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="F170" s="7"/>
       <c r="G170" s="8" t="s">
@@ -5452,17 +5458,17 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="9" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B171" s="7" t="s">
         <v>231</v>
       </c>
       <c r="C171" s="10"/>
       <c r="D171" s="10" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E171" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F171" s="7"/>
       <c r="G171" s="8" t="s">
@@ -5471,7 +5477,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="9" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B172" s="7" t="s">
         <v>178</v>
@@ -5479,7 +5485,7 @@
       <c r="C172" s="10"/>
       <c r="D172" s="10"/>
       <c r="E172" s="7" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F172" s="7"/>
       <c r="G172" s="8" t="s">
@@ -5488,7 +5494,7 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="9" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B173" s="7" t="s">
         <v>181</v>
@@ -5496,7 +5502,7 @@
       <c r="C173" s="10"/>
       <c r="D173" s="10"/>
       <c r="E173" s="7" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F173" s="7"/>
       <c r="G173" s="8" t="s">
@@ -5505,7 +5511,7 @@
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="9" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B174" s="7" t="s">
         <v>253</v>
@@ -5513,7 +5519,7 @@
       <c r="C174" s="10"/>
       <c r="D174" s="10"/>
       <c r="E174" s="7" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F174" s="7"/>
       <c r="G174" s="8" t="s">
@@ -5522,17 +5528,17 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="9" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C175" s="10"/>
       <c r="D175" s="10" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="E175" s="7" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F175" s="7"/>
       <c r="G175" s="8" t="s">
@@ -5541,7 +5547,7 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="9" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B176" s="7" t="s">
         <v>178</v>
@@ -5549,7 +5555,7 @@
       <c r="C176" s="10"/>
       <c r="D176" s="10"/>
       <c r="E176" s="7" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F176" s="7"/>
       <c r="G176" s="8" t="s">
@@ -5558,7 +5564,7 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="9" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B177" s="7" t="s">
         <v>181</v>
@@ -5566,7 +5572,7 @@
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
       <c r="E177" s="7" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F177" s="7"/>
       <c r="G177" s="8" t="s">
@@ -5575,7 +5581,7 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="9" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B178" s="7" t="s">
         <v>253</v>
@@ -5583,7 +5589,7 @@
       <c r="C178" s="10"/>
       <c r="D178" s="10"/>
       <c r="E178" s="7" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="F178" s="7"/>
       <c r="G178" s="8" t="s">
@@ -5592,7 +5598,7 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="9" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B179" s="7" t="s">
         <v>231</v>
@@ -5600,7 +5606,7 @@
       <c r="C179" s="10"/>
       <c r="D179" s="10"/>
       <c r="E179" s="7" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F179" s="7"/>
       <c r="G179" s="8" t="s">
@@ -5609,15 +5615,15 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="9" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C180" s="10"/>
       <c r="D180" s="10"/>
       <c r="E180" s="7" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F180" s="7"/>
       <c r="G180" s="8" t="s">
@@ -5626,34 +5632,34 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C181" s="5" t="n">
         <v>23</v>
       </c>
       <c r="E181" s="7" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F181" s="5" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="9" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C182" s="7" t="n">
         <v>121</v>
       </c>
       <c r="D182" s="7"/>
       <c r="E182" s="7" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="G182" s="8" t="s">
         <v>18</v>
@@ -5661,17 +5667,17 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="9" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B183" s="7" t="s">
         <v>178</v>
       </c>
       <c r="C183" s="10"/>
       <c r="D183" s="10" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E183" s="7" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F183" s="7"/>
       <c r="G183" s="8" t="s">
@@ -5680,17 +5686,17 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="9" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>231</v>
+        <v>645</v>
       </c>
       <c r="C184" s="10"/>
       <c r="D184" s="10" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="E184" s="7" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="F184" s="7"/>
       <c r="G184" s="8" t="s">
@@ -5699,17 +5705,17 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="9" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C185" s="7" t="n">
         <v>111</v>
       </c>
       <c r="D185" s="7"/>
       <c r="E185" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="G185" s="8" t="s">
         <v>18</v>
@@ -5717,7 +5723,7 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="9" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="B186" s="7" t="s">
         <v>306</v>
@@ -5726,7 +5732,7 @@
         <v>1711</v>
       </c>
       <c r="D186" s="7" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="E186" s="7" t="s">
         <v>307</v>
@@ -5737,47 +5743,47 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="C187" s="7" t="n">
         <v>3300</v>
       </c>
       <c r="D187" s="7" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="E187" s="7" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="F187" s="7" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="9" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="C188" s="7" t="n">
         <v>8000</v>
       </c>
       <c r="D188" s="7" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="E188" s="7" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="F188" s="7" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="9" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B189" s="7" t="s">
         <v>178</v>
@@ -5785,7 +5791,7 @@
       <c r="C189" s="10"/>
       <c r="D189" s="10"/>
       <c r="E189" s="7" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="F189" s="7"/>
       <c r="G189" s="8" t="s">
@@ -5794,7 +5800,7 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="9" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B190" s="7" t="s">
         <v>181</v>
@@ -5802,7 +5808,7 @@
       <c r="C190" s="10"/>
       <c r="D190" s="10"/>
       <c r="E190" s="7" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="F190" s="7"/>
       <c r="G190" s="8" t="s">
@@ -5811,17 +5817,17 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="9" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B191" s="7" t="s">
         <v>250</v>
       </c>
       <c r="C191" s="10"/>
       <c r="D191" s="10" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="E191" s="7" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="F191" s="7"/>
       <c r="G191" s="8" t="s">
@@ -5830,7 +5836,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="9" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B192" s="7" t="s">
         <v>129</v>
@@ -5839,10 +5845,10 @@
         <v>1500</v>
       </c>
       <c r="D192" s="7" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="E192" s="7" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="F192" s="7" t="s">
         <v>132</v>
@@ -5850,17 +5856,17 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="9" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="C193" s="7" t="n">
         <v>2611</v>
       </c>
       <c r="D193" s="7"/>
       <c r="E193" s="7" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="G193" s="8" t="s">
         <v>18</v>
@@ -5868,17 +5874,17 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="9" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="C194" s="7" t="n">
         <v>2711</v>
       </c>
       <c r="D194" s="7"/>
       <c r="E194" s="7" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="G194" s="8" t="s">
         <v>18</v>
@@ -5886,7 +5892,7 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="9" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="B195" s="7" t="s">
         <v>231</v>
@@ -5894,7 +5900,7 @@
       <c r="C195" s="10"/>
       <c r="D195" s="10"/>
       <c r="E195" s="7" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="F195" s="7"/>
       <c r="G195" s="8" t="s">
@@ -5903,55 +5909,55 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="9" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="C196" s="10"/>
       <c r="D196" s="10" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E196" s="7" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="F196" s="7" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="9" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C197" s="7" t="n">
         <v>3721</v>
       </c>
       <c r="D197" s="7"/>
       <c r="E197" s="7" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="F197" s="7" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="9" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C198" s="7" t="n">
         <v>6100</v>
       </c>
       <c r="D198" s="7" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="E198" s="7" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="F198" s="7"/>
       <c r="G198" s="8" t="s">
@@ -5960,25 +5966,25 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="9" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="C199" s="10" t="n">
         <v>8400</v>
       </c>
       <c r="D199" s="10"/>
       <c r="E199" s="7" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="F199" s="7" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="9" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B200" s="7" t="s">
         <v>54</v>
@@ -5986,15 +5992,15 @@
       <c r="C200" s="6"/>
       <c r="D200" s="6"/>
       <c r="E200" s="7" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="F200" s="7" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B201" s="7" t="s">
         <v>288</v>
@@ -6004,7 +6010,7 @@
       </c>
       <c r="D201" s="7"/>
       <c r="E201" s="7" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="F201" s="7"/>
       <c r="G201" s="8" t="s">
@@ -6013,19 +6019,19 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C202" s="7" t="n">
         <v>400</v>
       </c>
       <c r="D202" s="7" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E202" s="7" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="F202" s="7"/>
       <c r="G202" s="8" t="s">
@@ -6034,7 +6040,7 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="9" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="B203" s="7" t="s">
         <v>16</v>
@@ -6042,7 +6048,7 @@
       <c r="C203" s="10"/>
       <c r="D203" s="10"/>
       <c r="E203" s="7" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="F203" s="7"/>
       <c r="G203" s="8" t="s">
@@ -6051,17 +6057,17 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="9" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C204" s="7" t="n">
         <v>21</v>
       </c>
       <c r="D204" s="7"/>
       <c r="E204" s="7" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="G204" s="8" t="s">
         <v>18</v>
@@ -6069,13 +6075,13 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="B205" s="7" t="s">
         <v>178</v>
       </c>
       <c r="E205" s="7" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="F205" s="7"/>
     </row>

</xml_diff>

<commit_message>
Add SipHash. Closes #18
Added SipHash and hashcat mode
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="743">
   <si>
     <t>Hash</t>
   </si>
@@ -1908,6 +1908,15 @@
   </si>
   <si>
     <t>2d7421aeb3bae997944090ba7e1c1df448dd92af995af28fa58737d2cc0b0ecc955a9c747cd701e70edfe41e8e3d76740700df60926886c540a80cfa76854da5</t>
+  </si>
+  <si>
+    <t>SipHash</t>
+  </si>
+  <si>
+    <t>^[a-f0-9]{16}:2:4:[a-f0-9]{32}$/i</t>
+  </si>
+  <si>
+    <t>ad61d78c06037cd9:2:4:81533218127174468417660201434054</t>
   </si>
   <si>
     <t>Skein-1024</t>
@@ -2424,10 +2433,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G207"/>
+  <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A184" activeCellId="0" sqref="A1:G207"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B175" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2790,7 +2799,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
         <v>78</v>
       </c>
@@ -2810,7 +2819,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
         <v>83</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
         <v>96</v>
       </c>
@@ -2884,7 +2893,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>99</v>
       </c>
@@ -3291,7 +3300,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>185</v>
       </c>
@@ -3309,7 +3318,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>188</v>
       </c>
@@ -3543,7 +3552,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="11" t="s">
         <v>232</v>
       </c>
@@ -3563,7 +3572,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="11" t="s">
         <v>236</v>
       </c>
@@ -3833,7 +3842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
         <v>283</v>
       </c>
@@ -3851,7 +3860,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>286</v>
       </c>
@@ -4077,7 +4086,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
         <v>335</v>
       </c>
@@ -4097,7 +4106,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
         <v>339</v>
       </c>
@@ -4463,7 +4472,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="11" t="s">
         <v>415</v>
       </c>
@@ -4479,7 +4488,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="11" t="s">
         <v>416</v>
       </c>
@@ -4598,7 +4607,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="11" t="s">
         <v>438</v>
       </c>
@@ -4616,7 +4625,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="11" t="s">
         <v>441</v>
       </c>
@@ -4636,7 +4645,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="11" t="s">
         <v>445</v>
       </c>
@@ -4656,7 +4665,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="11" t="s">
         <v>449</v>
       </c>
@@ -4692,7 +4701,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="11" t="s">
         <v>457</v>
       </c>
@@ -4768,7 +4777,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="11" t="s">
         <v>472</v>
       </c>
@@ -4788,7 +4797,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="11" t="s">
         <v>475</v>
       </c>
@@ -4808,7 +4817,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="11" t="s">
         <v>479</v>
       </c>
@@ -5256,7 +5265,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
         <v>580</v>
       </c>
@@ -5266,7 +5275,6 @@
       <c r="C155" s="10" t="n">
         <v>8900</v>
       </c>
-      <c r="D155" s="1"/>
       <c r="E155" s="9" t="s">
         <v>582</v>
       </c>
@@ -5312,7 +5320,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="11" t="s">
         <v>592</v>
       </c>
@@ -5534,28 +5542,29 @@
         <v>621</v>
       </c>
     </row>
-    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="11" t="s">
+    <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="B170" s="9" t="s">
+      <c r="B170" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="C170" s="12"/>
-      <c r="D170" s="12"/>
-      <c r="E170" s="9" t="s">
+      <c r="C170" s="15" t="n">
+        <v>10100</v>
+      </c>
+      <c r="E170" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="F170" s="9" t="s">
-        <v>634</v>
+      <c r="G170" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="B171" s="9" t="s">
         <v>635</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>608</v>
       </c>
       <c r="C171" s="12"/>
       <c r="D171" s="12"/>
@@ -5563,41 +5572,39 @@
         <v>636</v>
       </c>
       <c r="F171" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="11" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>552</v>
+        <v>608</v>
       </c>
       <c r="C172" s="12"/>
       <c r="D172" s="12"/>
       <c r="E172" s="9" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F172" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="11" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>242</v>
+        <v>552</v>
       </c>
       <c r="C173" s="12"/>
-      <c r="D173" s="12" t="s">
-        <v>640</v>
-      </c>
+      <c r="D173" s="12"/>
       <c r="E173" s="9" t="s">
         <v>641</v>
       </c>
       <c r="F173" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5605,65 +5612,65 @@
         <v>642</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="C174" s="12"/>
-      <c r="D174" s="12"/>
+      <c r="D174" s="12" t="s">
+        <v>643</v>
+      </c>
       <c r="E174" s="9" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="F174" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="11" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C175" s="12"/>
       <c r="D175" s="12"/>
       <c r="E175" s="9" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F175" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="11" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>266</v>
+        <v>189</v>
       </c>
       <c r="C176" s="12"/>
       <c r="D176" s="12"/>
       <c r="E176" s="9" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F176" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="11" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>552</v>
+        <v>266</v>
       </c>
       <c r="C177" s="12"/>
-      <c r="D177" s="12" t="s">
-        <v>649</v>
-      </c>
+      <c r="D177" s="12"/>
       <c r="E177" s="9" t="s">
         <v>650</v>
       </c>
       <c r="F177" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5671,114 +5678,114 @@
         <v>651</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>186</v>
+        <v>552</v>
       </c>
       <c r="C178" s="12"/>
-      <c r="D178" s="12"/>
+      <c r="D178" s="12" t="s">
+        <v>652</v>
+      </c>
       <c r="E178" s="9" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F178" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="11" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C179" s="12"/>
       <c r="D179" s="12"/>
       <c r="E179" s="9" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="11" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>266</v>
+        <v>189</v>
       </c>
       <c r="C180" s="12"/>
       <c r="D180" s="12"/>
       <c r="E180" s="9" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F180" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="11" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="C181" s="12"/>
       <c r="D181" s="12"/>
       <c r="E181" s="9" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F181" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="11" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>608</v>
+        <v>242</v>
       </c>
       <c r="C182" s="12"/>
       <c r="D182" s="12"/>
       <c r="E182" s="9" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F182" s="9" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="s">
-        <v>661</v>
+      <c r="A183" s="11" t="s">
+        <v>662</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>662</v>
-      </c>
-      <c r="C183" s="10" t="n">
-        <v>23</v>
-      </c>
+        <v>608</v>
+      </c>
+      <c r="C183" s="12"/>
+      <c r="D183" s="12"/>
       <c r="E183" s="9" t="s">
         <v>663</v>
       </c>
-      <c r="F183" s="10" t="s">
+      <c r="F183" s="9" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="11" t="s">
+      <c r="B184" s="9" t="s">
         <v>665</v>
       </c>
-      <c r="B184" s="9" t="s">
+      <c r="C184" s="10" t="n">
+        <v>23</v>
+      </c>
+      <c r="E184" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="C184" s="9" t="n">
-        <v>121</v>
-      </c>
-      <c r="D184" s="9"/>
-      <c r="E184" s="9" t="s">
+      <c r="F184" s="10" t="s">
         <v>667</v>
-      </c>
-      <c r="G184" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5786,124 +5793,126 @@
         <v>668</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C185" s="12"/>
-      <c r="D185" s="12" t="s">
         <v>669</v>
       </c>
+      <c r="C185" s="9" t="n">
+        <v>121</v>
+      </c>
+      <c r="D185" s="9"/>
       <c r="E185" s="9" t="s">
         <v>670</v>
       </c>
-      <c r="F185" s="9" t="s">
-        <v>671</v>
+      <c r="G185" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>673</v>
+        <v>186</v>
       </c>
       <c r="C186" s="12"/>
       <c r="D186" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="E186" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="F186" s="9" t="s">
         <v>674</v>
       </c>
-      <c r="E186" s="9" t="s">
+    </row>
+    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="11" t="s">
         <v>675</v>
       </c>
-      <c r="F186" s="9" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="11" t="s">
+      <c r="B187" s="9" t="s">
         <v>676</v>
       </c>
-      <c r="B187" s="9" t="s">
+      <c r="C187" s="12"/>
+      <c r="D187" s="12" t="s">
         <v>677</v>
       </c>
-      <c r="C187" s="9" t="n">
-        <v>111</v>
-      </c>
-      <c r="D187" s="9"/>
       <c r="E187" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="G187" s="4" t="s">
-        <v>82</v>
+        <v>678</v>
+      </c>
+      <c r="F187" s="9" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="11" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B188" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="C188" s="9" t="n">
+        <v>111</v>
+      </c>
+      <c r="D188" s="9"/>
+      <c r="E188" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="G188" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="11" t="s">
+        <v>681</v>
+      </c>
+      <c r="B189" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="C188" s="9" t="n">
+      <c r="C189" s="9" t="n">
         <v>1711</v>
-      </c>
-      <c r="D188" s="9" t="s">
-        <v>679</v>
-      </c>
-      <c r="E188" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="F188" s="9" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="B189" s="9" t="s">
-        <v>681</v>
-      </c>
-      <c r="C189" s="9" t="n">
-        <v>3300</v>
       </c>
       <c r="D189" s="9" t="s">
         <v>682</v>
       </c>
       <c r="E189" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="F189" s="9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="F189" s="9" t="s">
+      <c r="B190" s="9" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="11" t="s">
+      <c r="C190" s="9" t="n">
+        <v>3300</v>
+      </c>
+      <c r="D190" s="9" t="s">
         <v>685</v>
       </c>
-      <c r="B190" s="9" t="s">
+      <c r="E190" s="9" t="s">
         <v>686</v>
       </c>
-      <c r="C190" s="9" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D190" s="9" t="s">
+      <c r="F190" s="9" t="s">
         <v>687</v>
-      </c>
-      <c r="E190" s="9" t="s">
-        <v>688</v>
-      </c>
-      <c r="F190" s="9" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="11" t="s">
+        <v>688</v>
+      </c>
+      <c r="B191" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="C191" s="9" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D191" s="9" t="s">
         <v>690</v>
       </c>
-      <c r="B191" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C191" s="12"/>
-      <c r="D191" s="12"/>
       <c r="E191" s="9" t="s">
         <v>691</v>
       </c>
@@ -5916,7 +5925,7 @@
         <v>693</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C192" s="12"/>
       <c r="D192" s="12"/>
@@ -5924,66 +5933,64 @@
         <v>694</v>
       </c>
       <c r="F192" s="9" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="11" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>263</v>
+        <v>189</v>
       </c>
       <c r="C193" s="12"/>
-      <c r="D193" s="12" t="s">
-        <v>696</v>
-      </c>
+      <c r="D193" s="12"/>
       <c r="E193" s="9" t="s">
         <v>697</v>
       </c>
       <c r="F193" s="9" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="194" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="11" t="s">
         <v>698</v>
       </c>
       <c r="B194" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C194" s="12"/>
+      <c r="D194" s="12" t="s">
+        <v>699</v>
+      </c>
+      <c r="E194" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="F194" s="9" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="195" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="B195" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C194" s="9" t="n">
+      <c r="C195" s="9" t="n">
         <v>1500</v>
       </c>
-      <c r="D194" s="13" t="s">
+      <c r="D195" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E194" s="9" t="s">
-        <v>699</v>
-      </c>
-      <c r="F194" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="11" t="s">
-        <v>700</v>
-      </c>
-      <c r="B195" s="9" t="s">
-        <v>701</v>
-      </c>
-      <c r="C195" s="9" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D195" s="9"/>
       <c r="E195" s="9" t="s">
         <v>702</v>
       </c>
-      <c r="G195" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F195" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="11" t="s">
         <v>703</v>
       </c>
@@ -5991,7 +5998,7 @@
         <v>704</v>
       </c>
       <c r="C196" s="9" t="n">
-        <v>2711</v>
+        <v>2611</v>
       </c>
       <c r="D196" s="9"/>
       <c r="E196" s="9" t="s">
@@ -6001,107 +6008,110 @@
         <v>82</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="11" t="s">
         <v>706</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="C197" s="12"/>
-      <c r="D197" s="12"/>
+        <v>707</v>
+      </c>
+      <c r="C197" s="9" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D197" s="9"/>
       <c r="E197" s="9" t="s">
-        <v>707</v>
-      </c>
-      <c r="F197" s="9"/>
+        <v>708</v>
+      </c>
       <c r="G197" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="11" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>709</v>
+        <v>242</v>
       </c>
       <c r="C198" s="12"/>
-      <c r="D198" s="12" t="s">
+      <c r="D198" s="12"/>
+      <c r="E198" s="9" t="s">
         <v>710</v>
       </c>
-      <c r="E198" s="9" t="s">
-        <v>711</v>
-      </c>
-      <c r="F198" s="9" t="s">
-        <v>712</v>
+      <c r="F198" s="9"/>
+      <c r="G198" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="B199" s="9" t="s">
+        <v>712</v>
+      </c>
+      <c r="C199" s="12"/>
+      <c r="D199" s="12" t="s">
         <v>713</v>
       </c>
-      <c r="B199" s="9" t="s">
+      <c r="E199" s="9" t="s">
         <v>714</v>
       </c>
-      <c r="C199" s="9" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D199" s="9"/>
-      <c r="E199" s="9" t="s">
+      <c r="F199" s="9" t="s">
         <v>715</v>
-      </c>
-      <c r="F199" s="9" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="11" t="s">
+        <v>716</v>
+      </c>
+      <c r="B200" s="9" t="s">
         <v>717</v>
       </c>
-      <c r="B200" s="9" t="s">
-        <v>552</v>
-      </c>
       <c r="C200" s="9" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D200" s="9" t="s">
+        <v>3721</v>
+      </c>
+      <c r="D200" s="9"/>
+      <c r="E200" s="9" t="s">
         <v>718</v>
       </c>
-      <c r="E200" s="9" t="s">
+      <c r="F200" s="9" t="s">
         <v>719</v>
-      </c>
-      <c r="F200" s="9" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="11" t="s">
+        <v>720</v>
+      </c>
+      <c r="B201" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="C201" s="9" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D201" s="9" t="s">
         <v>721</v>
       </c>
-      <c r="B201" s="9" t="s">
+      <c r="E201" s="9" t="s">
         <v>722</v>
       </c>
-      <c r="C201" s="12" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D201" s="12" t="s">
+      <c r="F201" s="9" t="s">
         <v>723</v>
-      </c>
-      <c r="E201" s="9" t="s">
-        <v>724</v>
-      </c>
-      <c r="F201" s="9" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="11" t="s">
+        <v>724</v>
+      </c>
+      <c r="B202" s="9" t="s">
+        <v>725</v>
+      </c>
+      <c r="C202" s="12" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D202" s="12" t="s">
         <v>726</v>
       </c>
-      <c r="B202" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C202" s="3"/>
       <c r="E202" s="9" t="s">
         <v>727</v>
       </c>
@@ -6109,91 +6119,106 @@
         <v>728</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="s">
+    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="11" t="s">
         <v>729</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="C203" s="9" t="n">
-        <v>400</v>
-      </c>
-      <c r="D203" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="C203" s="3"/>
       <c r="E203" s="9" t="s">
         <v>730</v>
       </c>
-      <c r="F203" s="9"/>
-      <c r="G203" s="4" t="s">
-        <v>82</v>
+      <c r="F203" s="9" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>512</v>
+        <v>302</v>
       </c>
       <c r="C204" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="D204" s="9" t="s">
-        <v>508</v>
-      </c>
+      <c r="D204" s="9"/>
       <c r="E204" s="9" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="F204" s="9"/>
       <c r="G204" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="11" t="s">
-        <v>733</v>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>734</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C205" s="12"/>
-      <c r="D205" s="12"/>
+        <v>512</v>
+      </c>
+      <c r="C205" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D205" s="9" t="s">
+        <v>508</v>
+      </c>
       <c r="E205" s="9" t="s">
-        <v>734</v>
-      </c>
-      <c r="F205" s="9" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F205" s="9"/>
+      <c r="G205" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="11" t="s">
         <v>736</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="C206" s="9" t="n">
-        <v>21</v>
-      </c>
-      <c r="D206" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="C206" s="12"/>
+      <c r="D206" s="12"/>
       <c r="E206" s="9" t="s">
         <v>737</v>
       </c>
-      <c r="G206" s="4" t="s">
+      <c r="F206" s="9" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="11" t="s">
+        <v>739</v>
+      </c>
+      <c r="B207" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C207" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="D207" s="9"/>
+      <c r="E207" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="G207" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="B207" s="9" t="s">
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B208" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="E207" s="9" t="s">
-        <v>739</v>
-      </c>
-      <c r="F207" s="9"/>
+      <c r="E208" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="F208" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Renamed BCrypt to bcrypt
Renamed BCrypt to bcrypt
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -161,7 +161,7 @@
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.apr_md5_crypt.html</t>
   </si>
   <si>
-    <t>BCrypt(SHA-256)</t>
+    <t>bcrypt(SHA-256)</t>
   </si>
   <si>
     <t>^\$bcrypt-sha256\$(2[axy]|2)\,[0-9]+\$[a-z0-9\/.]{22}\$[a-z0-9\/.]{31}$/i</t>
@@ -443,7 +443,7 @@
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.des_crypt.html</t>
   </si>
   <si>
-    <t>Django(BCrypt)</t>
+    <t>Django(bcrypt)</t>
   </si>
   <si>
     <t>^bcrypt(\$2[axy]|\$2)\$[0-9]{0,2}?\$[a-z0-9\/.]{53}$/i</t>
@@ -1769,7 +1769,7 @@
     <t>^SCRYPT:[0-9]{1,}:[0-9]{1}:[0-9]{1}:[a-z0-9:\/+=]{1,}$/i</t>
   </si>
   <si>
-    <t>SCRYPT:1024:1:1:MDIwMzMwNTQwNDQyNQ==:5FW+zWivLxgCWj7qLiQbeC8zaNQ+qdO0NUinvqyFcfo= </t>
+    <t>SCRYPT:1024:1:1:MDIwMzMwNTQwNDQyNQ==:5FW+zWivLxgCWj7qLiQbeC8zaNQ+qdO0NUinvqyFcfo=</t>
   </si>
   <si>
     <t>SHA-1</t>
@@ -2441,8 +2441,8 @@
   </sheetPr>
   <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B142" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Add Cisco Type 4
Added Cisco Type 4
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="749">
   <si>
     <t>Hash</t>
   </si>
@@ -201,6 +201,18 @@
   </si>
   <si>
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.bsdi_crypt.html</t>
+  </si>
+  <si>
+    <t>Cisco Type 4</t>
+  </si>
+  <si>
+    <t>^(\$cisco4\$)?[a-z0-9\/.]{43}$/i</t>
+  </si>
+  <si>
+    <t>jHSXiU.oQTuJ/lmrcyVL1on3EL4Jdd5J7S3y34QiQDQ </t>
+  </si>
+  <si>
+    <t>http://www.tobtu.com/cisco4tosha256.php</t>
   </si>
   <si>
     <t>Cisco Type 8</t>
@@ -2435,10 +2447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B190" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2734,17 +2746,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="9" t="n">
-        <v>9200</v>
-      </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -2759,29 +2768,30 @@
         <v>67</v>
       </c>
       <c r="C16" s="9" t="n">
-        <v>9300</v>
+        <v>9200</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>68</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="9" t="n">
+        <v>9300</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2791,143 +2801,143 @@
       <c r="B18" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="8" t="n">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="8" t="n">
         <v>2410</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="8" t="n">
+      <c r="E19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="8" t="n">
         <v>500</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="8" t="s">
+      <c r="D20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="8" t="n">
-        <v>5700</v>
-      </c>
-      <c r="D20" s="8"/>
       <c r="E20" s="8" t="s">
         <v>85</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C21" s="8" t="n">
-        <v>2400</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>88</v>
-      </c>
+        <v>5700</v>
+      </c>
+      <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>90</v>
+      <c r="G21" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="8" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="8" t="n">
-        <v>8100</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="8" t="n">
+        <v>8100</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
       <c r="E23" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="F23" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="2" t="s">
+    </row>
+    <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="14" t="n">
+      <c r="B24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="14" t="n">
         <v>10200</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="2" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2936,49 +2946,47 @@
         <v>107</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
-        <v>112</v>
+      <c r="A28" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C28" s="11"/>
-      <c r="D28" s="11" t="s">
-        <v>114</v>
-      </c>
+      <c r="D28" s="11"/>
       <c r="E28" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>106</v>
+      <c r="F28" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2986,64 +2994,66 @@
         <v>116</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="D29" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="E29" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F31" s="8"/>
-      <c r="G31" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F32" s="8" t="s">
         <v>127</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,60 +3085,61 @@
         <v>134</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" s="8" t="n">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="8" t="n">
         <v>3100</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C36" s="8" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>139</v>
-      </c>
+      <c r="D36" s="8"/>
       <c r="E36" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="8"/>
+      <c r="G36" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="C37" s="8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C37" s="3"/>
       <c r="E37" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="8" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3184,261 +3195,253 @@
       <c r="B41" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C41" s="3" t="n">
-        <v>10000</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C41" s="3"/>
+      <c r="E41" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E41" s="8" t="s">
+      <c r="F41" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="8" t="n">
-        <v>800</v>
-      </c>
-      <c r="D42" s="8"/>
       <c r="E42" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>167</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
+      <c r="C43" s="8" t="n">
+        <v>800</v>
+      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="4" t="s">
-        <v>82</v>
+      <c r="F43" s="8" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="C45" s="11" t="n">
-        <v>8300</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="F45" s="8" t="s">
         <v>176</v>
       </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C46" s="8" t="n">
-        <v>1100</v>
-      </c>
-      <c r="D46" s="8" t="s">
+      <c r="C46" s="11" t="n">
+        <v>8300</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="F46" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="C47" s="8" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C47" s="8" t="n">
+      <c r="E47" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48" s="8" t="n">
         <v>2100</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B48" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="C48" s="11" t="n">
-        <v>2600</v>
-      </c>
-      <c r="D48" s="11"/>
       <c r="E48" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>82</v>
+      <c r="F48" s="8" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C49" s="11" t="n">
-        <v>4500</v>
+        <v>2600</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10" t="s">
-        <v>193</v>
+      <c r="A50" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C50" s="8" t="n">
-        <v>7900</v>
-      </c>
-      <c r="D50" s="8" t="s">
         <v>195</v>
       </c>
+      <c r="C50" s="11" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D50" s="11"/>
       <c r="E50" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="G50" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="s">
+      <c r="B51" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="C51" s="8" t="n">
+        <v>7900</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11" t="s">
+      <c r="E51" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="F51" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
         <v>202</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>16</v>
+        <v>203</v>
       </c>
       <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="D52" s="11" t="s">
+        <v>204</v>
+      </c>
       <c r="E52" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="F52" s="8"/>
+      <c r="G52" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="53" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C53" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="54" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C54" s="8" t="n">
         <v>123</v>
       </c>
-      <c r="D53" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B54" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="8" t="n">
-        <v>141</v>
-      </c>
-      <c r="D54" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="F54" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,70 +3452,77 @@
         <v>215</v>
       </c>
       <c r="C55" s="8" t="n">
-        <v>1441</v>
-      </c>
-      <c r="D55" s="8"/>
+        <v>141</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>216</v>
+      </c>
       <c r="E55" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>217</v>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10" t="s">
+        <v>218</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
+        <v>219</v>
+      </c>
+      <c r="C56" s="8" t="n">
+        <v>1441</v>
+      </c>
+      <c r="D56" s="8"/>
       <c r="E56" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="F56" s="8" t="s">
         <v>220</v>
       </c>
+      <c r="F56" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="1" t="s">
         <v>221</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>104</v>
+        <v>222</v>
       </c>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>16</v>
@@ -3520,15 +3530,15 @@
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="F59" s="8" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>16</v>
@@ -3536,89 +3546,88 @@
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="F60" s="8"/>
-      <c r="G60" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>231</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C62" s="8" t="n">
-        <v>7000</v>
-      </c>
-      <c r="D62" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="F62" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="10" t="s">
         <v>238</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>79</v>
+        <v>239</v>
       </c>
       <c r="C63" s="8" t="n">
+        <v>7000</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="8" t="n">
         <v>500</v>
       </c>
-      <c r="D63" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
+      <c r="D64" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="E64" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="F64" s="8"/>
+        <v>85</v>
+      </c>
       <c r="G64" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>16</v>
@@ -3626,48 +3635,47 @@
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
       <c r="E65" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F65" s="8"/>
       <c r="G65" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="C66" s="8" t="n">
-        <v>6900</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>245</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
       <c r="E66" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="F66" s="8" t="s">
-        <v>247</v>
+      <c r="F66" s="8"/>
+      <c r="G66" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="C67" s="8" t="n">
+        <v>6900</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="C67" s="8" t="n">
-        <v>7200</v>
-      </c>
-      <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="F67" s="9" t="s">
+      <c r="F67" s="8" t="s">
         <v>251</v>
       </c>
     </row>
@@ -3676,46 +3684,46 @@
         <v>252</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>119</v>
+        <v>253</v>
       </c>
       <c r="C68" s="8" t="n">
-        <v>5100</v>
+        <v>7200</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
+        <v>123</v>
+      </c>
+      <c r="C69" s="8" t="n">
+        <v>5100</v>
+      </c>
+      <c r="D69" s="8"/>
       <c r="E69" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="F69" s="8" t="s">
         <v>257</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C70" s="11"/>
-      <c r="D70" s="11" t="s">
-        <v>259</v>
-      </c>
+      <c r="D70" s="11"/>
       <c r="E70" s="8" t="s">
         <v>260</v>
       </c>
@@ -3728,77 +3736,75 @@
         <v>262</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
+      <c r="D71" s="11" t="s">
+        <v>263</v>
+      </c>
       <c r="E71" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>265</v>
+        <v>195</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
       <c r="E73" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="C74" s="11"/>
-      <c r="D74" s="11" t="s">
-        <v>271</v>
-      </c>
+      <c r="D74" s="11"/>
       <c r="E74" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>273</v>
+      <c r="A75" s="10" t="s">
+        <v>274</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C75" s="11" t="n">
-        <v>1421</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="C75" s="11"/>
       <c r="D75" s="11" t="s">
         <v>275</v>
       </c>
@@ -3806,27 +3812,27 @@
         <v>276</v>
       </c>
       <c r="F75" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="76" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="12" t="s">
+      <c r="B76" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="C76" s="11" t="n">
+        <v>1421</v>
+      </c>
+      <c r="D76" s="11" t="s">
         <v>279</v>
-      </c>
-      <c r="C76" s="9" t="n">
-        <v>5300</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3837,105 +3843,107 @@
         <v>283</v>
       </c>
       <c r="C77" s="9" t="n">
-        <v>5400</v>
+        <v>5300</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>284</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="15" t="s">
+    <row r="78" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C78" s="9" t="n">
+        <v>5400</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C78" s="8" t="n">
+      <c r="G78" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C79" s="8" t="n">
         <v>2811</v>
       </c>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C79" s="11" t="n">
+      <c r="D79" s="8"/>
+      <c r="E79" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C80" s="11" t="n">
         <v>7300</v>
       </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C80" s="8" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>293</v>
-      </c>
+      <c r="D80" s="11"/>
       <c r="E80" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="F80" s="8" t="s">
-        <v>295</v>
+      <c r="G80" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="B81" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
+      <c r="C81" s="8" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>297</v>
+      </c>
       <c r="E81" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="F81" s="2" t="s">
         <v>298</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="C82" s="8" t="n">
-        <v>11</v>
-      </c>
-      <c r="D82" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
       <c r="E82" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="F82" s="2" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3946,76 +3954,76 @@
       <c r="B83" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="C83" s="8" t="s">
-        <v>305</v>
+      <c r="C83" s="8" t="n">
+        <v>11</v>
       </c>
       <c r="D83" s="8"/>
       <c r="E83" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="F83" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="C84" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="C84" s="8" t="n">
+      <c r="D84" s="8"/>
+      <c r="E84" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C85" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="D84" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="B85" s="8" t="s">
+      <c r="D85" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="C85" s="8" t="n">
+      <c r="E85" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C86" s="8" t="n">
         <v>7500</v>
       </c>
-      <c r="D85" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="B86" s="8" t="s">
+      <c r="D86" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="C86" s="8" t="n">
-        <v>6800</v>
-      </c>
-      <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="F86" s="8" t="s">
+      <c r="F86" s="9" t="s">
         <v>321</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4026,7 +4034,7 @@
         <v>323</v>
       </c>
       <c r="C87" s="8" t="n">
-        <v>1711</v>
+        <v>6800</v>
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="8" t="s">
@@ -4036,41 +4044,39 @@
         <v>325</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
         <v>326</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
+      <c r="C88" s="8" t="n">
+        <v>1711</v>
+      </c>
+      <c r="D88" s="8"/>
       <c r="E88" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="F88" s="8"/>
-      <c r="G88" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F88" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C89" s="8" t="n">
-        <v>190</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>330</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
       <c r="E89" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="F89" s="8" t="s">
         <v>332</v>
+      </c>
+      <c r="F89" s="8"/>
+      <c r="G89" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4078,10 +4084,10 @@
         <v>333</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C90" s="8" t="n">
-        <v>3000</v>
+        <v>190</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>334</v>
@@ -4093,85 +4099,89 @@
         <v>336</v>
       </c>
     </row>
-    <row r="91" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
         <v>337</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C91" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C91" s="8" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D91" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="D91" s="14" t="s">
+      <c r="E91" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="F91" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="G91" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="92" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
         <v>341</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C92" s="11" t="s">
         <v>342</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="D92" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="D92" s="11" t="s">
+      <c r="E92" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="G92" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G92" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
+      <c r="B93" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="C93" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="C93" s="9" t="n">
+      <c r="D93" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="C94" s="9" t="n">
         <v>9100</v>
       </c>
-      <c r="E93" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
       <c r="E94" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="F94" s="8" t="s">
         <v>352</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>354</v>
+        <v>195</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
@@ -4187,14 +4197,10 @@
         <v>357</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C96" s="8" t="n">
-        <v>900</v>
-      </c>
-      <c r="D96" s="8" t="s">
         <v>358</v>
       </c>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
       <c r="E96" s="8" t="s">
         <v>359</v>
       </c>
@@ -4207,170 +4213,170 @@
         <v>361</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C97" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C97" s="8" t="n">
+        <v>900</v>
+      </c>
+      <c r="D97" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="D97" s="8" t="s">
+      <c r="E97" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="F97" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="F97" s="8" t="s">
+    </row>
+    <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="10" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="98" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="10" t="s">
+      <c r="B98" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C98" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C98" s="8" t="n">
+      <c r="D98" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="E98" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="99" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C99" s="8" t="n">
         <v>500</v>
       </c>
-      <c r="D98" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="F98" s="8" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C99" s="8" t="n">
-        <v>1600</v>
-      </c>
-      <c r="D99" s="8"/>
+      <c r="D99" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="E99" s="8" t="s">
-        <v>46</v>
+        <v>371</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>47</v>
+        <v>372</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>292</v>
+        <v>45</v>
       </c>
       <c r="C100" s="8" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>293</v>
-      </c>
+        <v>1600</v>
+      </c>
+      <c r="D100" s="8"/>
       <c r="E100" s="8" t="s">
-        <v>294</v>
+        <v>46</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>295</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="C101" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="D101" s="11" t="s">
-        <v>374</v>
+        <v>296</v>
+      </c>
+      <c r="C101" s="8" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>297</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>375</v>
+        <v>298</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>376</v>
+        <v>299</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="C102" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="D102" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
       <c r="E102" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="F102" s="9" t="s">
+      <c r="F102" s="8" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="103" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="12" t="s">
+    <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="10" t="s">
         <v>381</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="C103" s="9" t="n">
-        <v>9700</v>
-      </c>
-      <c r="D103" s="3" t="s">
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="F103" s="9" t="s">
         <v>384</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="C104" s="9" t="n">
+        <v>9700</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C104" s="9" t="n">
+      <c r="E104" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="105" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="C105" s="9" t="n">
         <v>9800</v>
       </c>
-      <c r="E104" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="s">
+      <c r="E105" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="C105" s="9" t="n">
-        <v>9400</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4381,46 +4387,50 @@
         <v>394</v>
       </c>
       <c r="C106" s="9" t="n">
-        <v>9500</v>
-      </c>
-      <c r="E106" s="16" t="s">
+        <v>9400</v>
+      </c>
+      <c r="D106" s="3" t="s">
         <v>395</v>
       </c>
+      <c r="E106" s="8" t="s">
+        <v>396</v>
+      </c>
       <c r="F106" s="2" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C107" s="9" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E107" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C108" s="9" t="n">
         <v>9600</v>
       </c>
-      <c r="E107" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="F108" s="8" t="s">
+      <c r="E108" s="9" t="s">
         <v>402</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,73 +4456,69 @@
       <c r="B110" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="C110" s="8" t="n">
-        <v>131</v>
-      </c>
-      <c r="D110" s="8" t="s">
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="E110" s="8" t="s">
+      <c r="F110" s="8" t="s">
         <v>410</v>
-      </c>
-      <c r="F110" s="8" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="C111" s="8" t="n">
+        <v>131</v>
+      </c>
+      <c r="D111" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="C111" s="8" t="n">
-        <v>132</v>
-      </c>
-      <c r="D111" s="8" t="s">
+      <c r="E111" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="E111" s="8" t="s">
+      <c r="F111" s="8" t="s">
         <v>415</v>
-      </c>
-      <c r="F111" s="8" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="C112" s="11" t="n">
+      <c r="C112" s="8" t="n">
         <v>132</v>
       </c>
-      <c r="D112" s="11"/>
-      <c r="E112" s="8"/>
-      <c r="G112" s="4" t="s">
-        <v>82</v>
+      <c r="D112" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="C113" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>421</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="C113" s="11" t="n">
+        <v>132</v>
+      </c>
+      <c r="D113" s="11"/>
+      <c r="E113" s="8"/>
       <c r="G113" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4520,32 +4526,34 @@
         <v>422</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C114" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>423</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C115" s="8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D115" s="8"/>
+        <v>1731</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>424</v>
+      </c>
       <c r="E115" s="8" t="s">
         <v>427</v>
       </c>
@@ -4558,14 +4566,12 @@
         <v>429</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>119</v>
+        <v>430</v>
       </c>
       <c r="C116" s="8" t="n">
-        <v>200</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>430</v>
-      </c>
+        <v>2811</v>
+      </c>
+      <c r="D116" s="8"/>
       <c r="E116" s="8" t="s">
         <v>431</v>
       </c>
@@ -4574,85 +4580,85 @@
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="15" t="s">
+      <c r="A117" s="10" t="s">
         <v>433</v>
       </c>
       <c r="B117" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C117" s="8" t="n">
+        <v>200</v>
+      </c>
+      <c r="D117" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="C117" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="D117" s="8" t="s">
+      <c r="E117" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="E117" s="8" t="s">
+      <c r="F117" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="F117" s="8" t="s">
+    </row>
+    <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="15" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="10" t="s">
+      <c r="B118" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>434</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="E118" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="F118" s="8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C119" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D119" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="F118" s="8"/>
-      <c r="G118" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="C119" s="8" t="n">
+      <c r="E119" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="F119" s="8"/>
+      <c r="G119" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="C120" s="8" t="n">
         <v>5500</v>
       </c>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="G119" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="120" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="C120" s="8" t="n">
-        <v>5600</v>
-      </c>
-      <c r="D120" s="12" t="s">
-        <v>445</v>
-      </c>
+      <c r="D120" s="8"/>
       <c r="E120" s="8" t="s">
         <v>446</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="121" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
         <v>447</v>
       </c>
@@ -4660,16 +4666,16 @@
         <v>448</v>
       </c>
       <c r="C121" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D121" s="8" t="s">
+        <v>5600</v>
+      </c>
+      <c r="D121" s="12" t="s">
         <v>449</v>
       </c>
       <c r="E121" s="8" t="s">
         <v>450</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4680,7 +4686,7 @@
         <v>452</v>
       </c>
       <c r="C122" s="8" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>453</v>
@@ -4689,7 +4695,7 @@
         <v>454</v>
       </c>
       <c r="G122" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4699,13 +4705,17 @@
       <c r="B123" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
+      <c r="C123" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="E123" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="F123" s="8" t="s">
         <v>458</v>
+      </c>
+      <c r="G123" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4715,66 +4725,64 @@
       <c r="B124" s="8" t="s">
         <v>460</v>
       </c>
-      <c r="C124" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D124" s="8" t="s">
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
+      <c r="E124" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="E124" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="G124" s="4" t="s">
-        <v>82</v>
+      <c r="F124" s="8" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C125" s="8" t="n">
-        <v>112</v>
+        <v>1000</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="F125" s="8" t="s">
-        <v>466</v>
+        <v>363</v>
+      </c>
+      <c r="G125" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="B126" s="8" t="s">
-        <v>119</v>
-      </c>
       <c r="C126" s="8" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D126" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>468</v>
+      </c>
       <c r="E126" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F126" s="8" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>471</v>
+        <v>123</v>
       </c>
       <c r="C127" s="8" t="n">
-        <v>21</v>
+        <v>3100</v>
       </c>
       <c r="D127" s="8"/>
       <c r="E127" s="8" t="s">
@@ -4789,39 +4797,37 @@
         <v>474</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>265</v>
+        <v>475</v>
       </c>
       <c r="C128" s="8" t="n">
-        <v>122</v>
-      </c>
-      <c r="D128" s="8" t="s">
-        <v>475</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D128" s="8"/>
       <c r="E128" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="G128" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="129" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F128" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>478</v>
+        <v>269</v>
       </c>
       <c r="C129" s="8" t="n">
-        <v>1722</v>
-      </c>
-      <c r="D129" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D129" s="8" t="s">
         <v>479</v>
       </c>
       <c r="E129" s="8" t="s">
         <v>480</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4832,7 +4838,7 @@
         <v>482</v>
       </c>
       <c r="C130" s="8" t="n">
-        <v>7100</v>
+        <v>1722</v>
       </c>
       <c r="D130" s="12" t="s">
         <v>483</v>
@@ -4841,39 +4847,44 @@
         <v>484</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="131" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
         <v>485</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
+      <c r="C131" s="8" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D131" s="12" t="s">
+        <v>487</v>
+      </c>
       <c r="E131" s="8" t="s">
-        <v>487</v>
-      </c>
-      <c r="F131" s="8"/>
+        <v>488</v>
+      </c>
       <c r="G131" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="C132" s="3"/>
+        <v>490</v>
+      </c>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
       <c r="E132" s="8" t="s">
-        <v>490</v>
-      </c>
-      <c r="F132" s="9" t="s">
         <v>491</v>
+      </c>
+      <c r="F132" s="8"/>
+      <c r="G132" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4883,12 +4894,11 @@
       <c r="B133" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="C133" s="11"/>
-      <c r="D133" s="11"/>
+      <c r="C133" s="3"/>
       <c r="E133" s="8" t="s">
         <v>494</v>
       </c>
-      <c r="F133" s="8" t="s">
+      <c r="F133" s="9" t="s">
         <v>495</v>
       </c>
     </row>
@@ -4909,173 +4919,171 @@
       </c>
     </row>
     <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="s">
+      <c r="A135" s="10" t="s">
         <v>500</v>
       </c>
       <c r="B135" s="8" t="s">
         <v>501</v>
       </c>
       <c r="C135" s="11"/>
-      <c r="D135" s="11" t="s">
+      <c r="D135" s="11"/>
+      <c r="E135" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="E135" s="8" t="s">
+      <c r="F135" s="8" t="s">
         <v>503</v>
-      </c>
-      <c r="F135" s="8" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B136" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="B136" s="8" t="s">
+      <c r="C136" s="11"/>
+      <c r="D136" s="11" t="s">
         <v>506</v>
-      </c>
-      <c r="C136" s="9" t="n">
-        <v>133</v>
       </c>
       <c r="E136" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="F136" s="9" t="s">
+      <c r="F136" s="8" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="10" t="s">
+      <c r="A137" s="1" t="s">
         <v>509</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="C137" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D137" s="8" t="s">
         <v>510</v>
+      </c>
+      <c r="C137" s="9" t="n">
+        <v>133</v>
       </c>
       <c r="E137" s="8" t="s">
         <v>511</v>
       </c>
-      <c r="F137" s="8" t="s">
+      <c r="F137" s="9" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
+    <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="10" t="s">
         <v>513</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>514</v>
+        <v>308</v>
       </c>
       <c r="C138" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="E138" s="8" t="s">
         <v>515</v>
       </c>
-      <c r="F138" s="8"/>
-      <c r="G138" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F138" s="8" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>517</v>
-      </c>
-      <c r="C139" s="9" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D139" s="9" t="s">
         <v>518</v>
+      </c>
+      <c r="C139" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D139" s="8" t="s">
+        <v>514</v>
       </c>
       <c r="E139" s="8" t="s">
         <v>519</v>
       </c>
-      <c r="F139" s="8" t="s">
-        <v>520</v>
+      <c r="F139" s="8"/>
+      <c r="G139" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B140" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="B140" s="8" t="s">
+      <c r="C140" s="9" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D140" s="9" t="s">
         <v>522</v>
       </c>
-      <c r="C140" s="3"/>
       <c r="E140" s="8" t="s">
         <v>523</v>
       </c>
-      <c r="F140" s="9" t="s">
+      <c r="F140" s="8" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="10" t="s">
+      <c r="A141" s="1" t="s">
         <v>525</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="C141" s="8" t="s">
+      <c r="C141" s="3"/>
+      <c r="E141" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="D141" s="8" t="s">
+      <c r="F141" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="E141" s="8" t="s">
+    </row>
+    <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="F141" s="8" t="s">
+      <c r="B142" s="8" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="10" t="s">
+      <c r="C142" s="8" t="s">
         <v>531</v>
       </c>
-      <c r="B142" s="8" t="s">
+      <c r="D142" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="C142" s="11" t="s">
+      <c r="E142" s="8" t="s">
         <v>533</v>
       </c>
-      <c r="D142" s="11" t="s">
+      <c r="F142" s="8" t="s">
         <v>534</v>
       </c>
-      <c r="E142" s="8" t="s">
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="10" t="s">
+      <c r="B143" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="B143" s="8" t="s">
+      <c r="C143" s="11" t="s">
         <v>537</v>
       </c>
-      <c r="C143" s="8" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D143" s="8"/>
+      <c r="D143" s="11" t="s">
+        <v>538</v>
+      </c>
       <c r="E143" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="F143" s="8" t="s">
         <v>539</v>
+      </c>
+      <c r="F143" s="8"/>
+      <c r="G143" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5083,12 +5091,12 @@
         <v>540</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11" t="s">
         <v>541</v>
       </c>
+      <c r="C144" s="8" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D144" s="8"/>
       <c r="E144" s="8" t="s">
         <v>542</v>
       </c>
@@ -5101,12 +5109,10 @@
         <v>544</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C145" s="8" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D145" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C145" s="11"/>
+      <c r="D145" s="11" t="s">
         <v>545</v>
       </c>
       <c r="E145" s="8" t="s">
@@ -5121,47 +5127,51 @@
         <v>548</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="C146" s="11"/>
-      <c r="D146" s="11"/>
+        <v>195</v>
+      </c>
+      <c r="C146" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D146" s="8" t="s">
+        <v>549</v>
+      </c>
       <c r="E146" s="8" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F146" s="8" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>551</v>
+        <v>248</v>
       </c>
       <c r="C147" s="11"/>
       <c r="D147" s="11"/>
       <c r="E147" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C148" s="11"/>
       <c r="D148" s="11"/>
       <c r="E148" s="8" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5169,23 +5179,23 @@
         <v>557</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="C149" s="11"/>
       <c r="D149" s="11"/>
       <c r="E149" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C150" s="11"/>
       <c r="D150" s="11"/>
@@ -5203,110 +5213,106 @@
       <c r="B151" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="C151" s="8" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D151" s="8" t="s">
+      <c r="C151" s="11"/>
+      <c r="D151" s="11"/>
+      <c r="E151" s="8" t="s">
         <v>566</v>
       </c>
-      <c r="E151" s="8" t="s">
+      <c r="F151" s="8" t="s">
         <v>567</v>
-      </c>
-      <c r="F151" s="8" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
+        <v>568</v>
+      </c>
+      <c r="B152" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="B152" s="8" t="s">
+      <c r="C152" s="8" t="n">
+        <v>7700</v>
+      </c>
+      <c r="D152" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="C152" s="8" t="n">
+      <c r="E152" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="F152" s="8" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="C153" s="8" t="n">
         <v>7800</v>
       </c>
-      <c r="D152" s="8" t="s">
-        <v>571</v>
-      </c>
-      <c r="E152" s="8" t="s">
+      <c r="D153" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="E153" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="F153" s="8" t="s">
         <v>572</v>
       </c>
-      <c r="F152" s="8" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="153" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="s">
-        <v>573</v>
-      </c>
-      <c r="B153" s="17" t="s">
-        <v>574</v>
-      </c>
-      <c r="C153" s="14" t="n">
+    </row>
+    <row r="154" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="B154" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="C154" s="14" t="n">
         <v>10300</v>
       </c>
-      <c r="D153" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="F153" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="10" t="s">
-        <v>578</v>
-      </c>
-      <c r="B154" s="8" t="s">
+      <c r="D154" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="C154" s="11"/>
-      <c r="D154" s="11"/>
-      <c r="E154" s="8" t="s">
+      <c r="E154" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="F154" s="8" t="s">
+      <c r="F154" s="2" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="155" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="s">
+    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="10" t="s">
         <v>582</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="C155" s="9" t="n">
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
+      <c r="E155" s="8" t="s">
+        <v>584</v>
+      </c>
+      <c r="F155" s="8" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="156" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="C156" s="9" t="n">
         <v>8900</v>
       </c>
-      <c r="E155" s="12" t="s">
-        <v>584</v>
-      </c>
-      <c r="G155" s="4" t="s">
+      <c r="E156" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="G156" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="10" t="s">
-        <v>585</v>
-      </c>
-      <c r="B156" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C156" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="D156" s="11" t="s">
-        <v>586</v>
-      </c>
-      <c r="E156" s="8" t="s">
-        <v>587</v>
-      </c>
-      <c r="F156" s="8" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5314,72 +5320,74 @@
         <v>589</v>
       </c>
       <c r="B157" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C157" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D157" s="11" t="s">
         <v>590</v>
       </c>
-      <c r="C157" s="11"/>
-      <c r="D157" s="11" t="s">
+      <c r="E157" s="8" t="s">
         <v>591</v>
       </c>
-      <c r="E157" s="8" t="s">
+      <c r="F157" s="8" t="s">
         <v>592</v>
       </c>
-      <c r="F157" s="8" t="s">
+    </row>
+    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="10" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="158" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="10" t="s">
+      <c r="B158" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="B158" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="C158" s="8" t="n">
+      <c r="C158" s="11"/>
+      <c r="D158" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="E158" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="F158" s="8" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="159" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="10" t="s">
+        <v>598</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C159" s="8" t="n">
         <v>101</v>
       </c>
-      <c r="D158" s="12" t="s">
-        <v>449</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>450</v>
-      </c>
-      <c r="G158" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="B159" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="C159" s="11"/>
-      <c r="D159" s="11"/>
+      <c r="D159" s="12" t="s">
+        <v>453</v>
+      </c>
       <c r="E159" s="8" t="s">
-        <v>596</v>
-      </c>
-      <c r="F159" s="8"/>
+        <v>454</v>
+      </c>
       <c r="G159" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C160" s="11"/>
-      <c r="D160" s="11" t="s">
-        <v>598</v>
-      </c>
+      <c r="D160" s="11"/>
       <c r="E160" s="8" t="s">
-        <v>599</v>
-      </c>
-      <c r="F160" s="8" t="s">
         <v>600</v>
+      </c>
+      <c r="F160" s="8"/>
+      <c r="G160" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5387,30 +5395,28 @@
         <v>601</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="C161" s="8" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D161" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C161" s="11"/>
+      <c r="D161" s="11" t="s">
         <v>602</v>
       </c>
       <c r="E161" s="8" t="s">
         <v>603</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="s">
-        <v>604</v>
+      <c r="A162" s="10" t="s">
+        <v>605</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>605</v>
+        <v>248</v>
       </c>
       <c r="C162" s="8" t="n">
-        <v>7400</v>
+        <v>1400</v>
       </c>
       <c r="D162" s="8" t="s">
         <v>606</v>
@@ -5419,25 +5425,27 @@
         <v>607</v>
       </c>
       <c r="F162" s="8" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="10" t="s">
+      <c r="B163" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="C163" s="8" t="n">
+        <v>7400</v>
+      </c>
+      <c r="D163" s="8" t="s">
         <v>610</v>
       </c>
-      <c r="C163" s="11"/>
-      <c r="D163" s="11" t="s">
+      <c r="E163" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="E163" s="8" t="s">
+      <c r="F163" s="8" t="s">
         <v>612</v>
-      </c>
-      <c r="F163" s="8" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5445,30 +5453,28 @@
         <v>613</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="C164" s="8" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D164" s="8" t="s">
         <v>614</v>
       </c>
+      <c r="C164" s="11"/>
+      <c r="D164" s="11" t="s">
+        <v>615</v>
+      </c>
       <c r="E164" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>617</v>
+        <v>558</v>
       </c>
       <c r="C165" s="8" t="n">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="D165" s="8" t="s">
         <v>618</v>
@@ -5477,42 +5483,42 @@
         <v>619</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>620</v>
+        <v>604</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
+        <v>620</v>
+      </c>
+      <c r="B166" s="8" t="s">
         <v>621</v>
       </c>
-      <c r="B166" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="C166" s="3"/>
+      <c r="C166" s="8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D166" s="8" t="s">
+        <v>622</v>
+      </c>
       <c r="E166" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="C167" s="11" t="s">
-        <v>625</v>
-      </c>
-      <c r="D167" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C167" s="3"/>
+      <c r="E167" s="8" t="s">
         <v>626</v>
       </c>
-      <c r="E167" s="8" t="s">
+      <c r="F167" s="8" t="s">
         <v>627</v>
-      </c>
-      <c r="F167" s="8" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5520,66 +5526,70 @@
         <v>628</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>610</v>
-      </c>
-      <c r="C168" s="11"/>
-      <c r="D168" s="11"/>
+        <v>248</v>
+      </c>
+      <c r="C168" s="11" t="s">
+        <v>629</v>
+      </c>
+      <c r="D168" s="11" t="s">
+        <v>630</v>
+      </c>
       <c r="E168" s="8" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="C169" s="11"/>
-      <c r="D169" s="11" t="s">
-        <v>631</v>
-      </c>
+      <c r="D169" s="11"/>
       <c r="E169" s="8" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="170" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="B170" s="2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="10" t="s">
         <v>634</v>
       </c>
-      <c r="C170" s="14" t="n">
+      <c r="B170" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="C170" s="11"/>
+      <c r="D170" s="11" t="s">
+        <v>635</v>
+      </c>
+      <c r="E170" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="F170" s="8" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="171" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="C171" s="14" t="n">
         <v>10100</v>
       </c>
-      <c r="E170" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="G170" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="B171" s="8" t="s">
-        <v>637</v>
-      </c>
-      <c r="C171" s="11"/>
-      <c r="D171" s="11"/>
-      <c r="E171" s="8" t="s">
-        <v>638</v>
-      </c>
-      <c r="F171" s="8" t="s">
+      <c r="E171" s="2" t="s">
         <v>639</v>
+      </c>
+      <c r="G171" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5587,248 +5597,246 @@
         <v>640</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>610</v>
+        <v>641</v>
       </c>
       <c r="C172" s="11"/>
       <c r="D172" s="11"/>
       <c r="E172" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>554</v>
+        <v>614</v>
       </c>
       <c r="C173" s="11"/>
       <c r="D173" s="11"/>
       <c r="E173" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="F173" s="8" t="s">
         <v>643</v>
-      </c>
-      <c r="F173" s="8" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>244</v>
+        <v>558</v>
       </c>
       <c r="C174" s="11"/>
-      <c r="D174" s="11" t="s">
-        <v>645</v>
-      </c>
+      <c r="D174" s="11"/>
       <c r="E174" s="8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>188</v>
+        <v>248</v>
       </c>
       <c r="C175" s="11"/>
-      <c r="D175" s="11"/>
+      <c r="D175" s="11" t="s">
+        <v>649</v>
+      </c>
       <c r="E175" s="8" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C176" s="11"/>
       <c r="D176" s="11"/>
       <c r="E176" s="8" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>268</v>
+        <v>195</v>
       </c>
       <c r="C177" s="11"/>
       <c r="D177" s="11"/>
       <c r="E177" s="8" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>554</v>
+        <v>272</v>
       </c>
       <c r="C178" s="11"/>
-      <c r="D178" s="11" t="s">
-        <v>654</v>
-      </c>
+      <c r="D178" s="11"/>
       <c r="E178" s="8" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>188</v>
+        <v>558</v>
       </c>
       <c r="C179" s="11"/>
-      <c r="D179" s="11"/>
+      <c r="D179" s="11" t="s">
+        <v>658</v>
+      </c>
       <c r="E179" s="8" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>268</v>
+        <v>195</v>
       </c>
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="C182" s="11"/>
       <c r="D182" s="11"/>
       <c r="E182" s="8" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>610</v>
+        <v>248</v>
       </c>
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="s">
-        <v>666</v>
+      <c r="A184" s="10" t="s">
+        <v>668</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="C184" s="9" t="n">
-        <v>23</v>
-      </c>
+        <v>614</v>
+      </c>
+      <c r="C184" s="11"/>
+      <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>668</v>
-      </c>
-      <c r="F184" s="9" t="s">
         <v>669</v>
       </c>
+      <c r="F184" s="8" t="s">
+        <v>643</v>
+      </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="10" t="s">
+      <c r="A185" s="1" t="s">
         <v>670</v>
       </c>
       <c r="B185" s="8" t="s">
         <v>671</v>
       </c>
-      <c r="C185" s="8" t="n">
-        <v>121</v>
-      </c>
-      <c r="D185" s="8"/>
+      <c r="C185" s="9" t="n">
+        <v>23</v>
+      </c>
       <c r="E185" s="8" t="s">
         <v>672</v>
       </c>
-      <c r="G185" s="4" t="s">
-        <v>82</v>
+      <c r="F185" s="9" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C186" s="11"/>
-      <c r="D186" s="11" t="s">
-        <v>674</v>
-      </c>
+        <v>675</v>
+      </c>
+      <c r="C186" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="D186" s="8"/>
       <c r="E186" s="8" t="s">
-        <v>675</v>
-      </c>
-      <c r="F186" s="8" t="s">
         <v>676</v>
+      </c>
+      <c r="G186" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,17 +5844,17 @@
         <v>677</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>678</v>
+        <v>192</v>
       </c>
       <c r="C187" s="11"/>
       <c r="D187" s="11" t="s">
+        <v>678</v>
+      </c>
+      <c r="E187" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="E187" s="8" t="s">
+      <c r="F187" s="8" t="s">
         <v>680</v>
-      </c>
-      <c r="F187" s="8" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5856,229 +5864,229 @@
       <c r="B188" s="8" t="s">
         <v>682</v>
       </c>
-      <c r="C188" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D188" s="8"/>
+      <c r="C188" s="11"/>
+      <c r="D188" s="11" t="s">
+        <v>683</v>
+      </c>
       <c r="E188" s="8" t="s">
-        <v>454</v>
-      </c>
-      <c r="G188" s="4" t="s">
-        <v>82</v>
+        <v>684</v>
+      </c>
+      <c r="F188" s="8" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>323</v>
+        <v>686</v>
       </c>
       <c r="C189" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D189" s="8"/>
+      <c r="E189" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="G189" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C190" s="8" t="n">
         <v>1711</v>
       </c>
-      <c r="D189" s="8" t="s">
-        <v>684</v>
-      </c>
-      <c r="E189" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="F189" s="8" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="B190" s="8" t="s">
-        <v>686</v>
-      </c>
-      <c r="C190" s="8" t="n">
+      <c r="D190" s="8" t="s">
+        <v>688</v>
+      </c>
+      <c r="E190" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="F190" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="C191" s="8" t="n">
         <v>3300</v>
       </c>
-      <c r="D190" s="8" t="s">
-        <v>687</v>
-      </c>
-      <c r="E190" s="8" t="s">
-        <v>688</v>
-      </c>
-      <c r="F190" s="8" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="10" t="s">
-        <v>690</v>
-      </c>
-      <c r="B191" s="8" t="s">
+      <c r="D191" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="C191" s="8" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D191" s="8" t="s">
+      <c r="E191" s="8" t="s">
         <v>692</v>
       </c>
-      <c r="E191" s="8" t="s">
+      <c r="F191" s="8" t="s">
         <v>693</v>
-      </c>
-      <c r="F191" s="8" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
+        <v>694</v>
+      </c>
+      <c r="B192" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B192" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C192" s="11"/>
-      <c r="D192" s="11"/>
+      <c r="C192" s="8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D192" s="8" t="s">
+        <v>696</v>
+      </c>
       <c r="E192" s="8" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C193" s="11"/>
       <c r="D193" s="11"/>
       <c r="E193" s="8" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>265</v>
+        <v>195</v>
       </c>
       <c r="C194" s="11"/>
-      <c r="D194" s="11" t="s">
+      <c r="D194" s="11"/>
+      <c r="E194" s="8" t="s">
+        <v>703</v>
+      </c>
+      <c r="F194" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="E194" s="8" t="s">
-        <v>702</v>
-      </c>
-      <c r="F194" s="8" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="195" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C195" s="8" t="n">
+        <v>269</v>
+      </c>
+      <c r="C195" s="11"/>
+      <c r="D195" s="11" t="s">
+        <v>705</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="F195" s="8" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="196" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C196" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="D195" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E195" s="8" t="s">
-        <v>704</v>
-      </c>
-      <c r="F195" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="10" t="s">
-        <v>705</v>
-      </c>
-      <c r="B196" s="8" t="s">
-        <v>706</v>
-      </c>
-      <c r="C196" s="8" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D196" s="8"/>
+      <c r="D196" s="12" t="s">
+        <v>143</v>
+      </c>
       <c r="E196" s="8" t="s">
-        <v>707</v>
-      </c>
-      <c r="G196" s="4" t="s">
-        <v>82</v>
+        <v>708</v>
+      </c>
+      <c r="F196" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C197" s="8" t="n">
-        <v>2711</v>
+        <v>2611</v>
       </c>
       <c r="D197" s="8"/>
       <c r="E197" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="G197" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="C198" s="11"/>
-      <c r="D198" s="11"/>
+        <v>713</v>
+      </c>
+      <c r="C198" s="8" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D198" s="8"/>
       <c r="E198" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="F198" s="8"/>
+        <v>714</v>
+      </c>
       <c r="G198" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>714</v>
+        <v>248</v>
       </c>
       <c r="C199" s="11"/>
-      <c r="D199" s="11" t="s">
-        <v>715</v>
-      </c>
+      <c r="D199" s="11"/>
       <c r="E199" s="8" t="s">
         <v>716</v>
       </c>
-      <c r="F199" s="8" t="s">
-        <v>717</v>
+      <c r="F199" s="8"/>
+      <c r="G199" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
+        <v>717</v>
+      </c>
+      <c r="B200" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="B200" s="8" t="s">
+      <c r="C200" s="11"/>
+      <c r="D200" s="11" t="s">
         <v>719</v>
       </c>
-      <c r="C200" s="8" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D200" s="8"/>
       <c r="E200" s="8" t="s">
         <v>720</v>
       </c>
@@ -6091,14 +6099,12 @@
         <v>722</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>554</v>
+        <v>723</v>
       </c>
       <c r="C201" s="8" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D201" s="8" t="s">
-        <v>723</v>
-      </c>
+        <v>3721</v>
+      </c>
+      <c r="D201" s="8"/>
       <c r="E201" s="8" t="s">
         <v>724</v>
       </c>
@@ -6111,121 +6117,141 @@
         <v>726</v>
       </c>
       <c r="B202" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="C202" s="8" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D202" s="8" t="s">
         <v>727</v>
       </c>
-      <c r="C202" s="11" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D202" s="11" t="s">
+      <c r="E202" s="8" t="s">
         <v>728</v>
       </c>
-      <c r="E202" s="8" t="s">
+      <c r="F202" s="8" t="s">
         <v>729</v>
-      </c>
-      <c r="F202" s="8" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="B203" s="8" t="s">
         <v>731</v>
       </c>
-      <c r="B203" s="8" t="s">
+      <c r="C203" s="11" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D203" s="11" t="s">
+        <v>732</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="F203" s="8" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="B204" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C203" s="3"/>
-      <c r="E203" s="8" t="s">
-        <v>732</v>
-      </c>
-      <c r="F203" s="8" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B204" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="C204" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D204" s="8"/>
+      <c r="C204" s="3"/>
       <c r="E204" s="8" t="s">
-        <v>735</v>
-      </c>
-      <c r="F204" s="8"/>
-      <c r="G204" s="4" t="s">
-        <v>82</v>
+        <v>736</v>
+      </c>
+      <c r="F204" s="8" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>514</v>
+        <v>308</v>
       </c>
       <c r="C205" s="8" t="n">
         <v>400</v>
       </c>
-      <c r="D205" s="8" t="s">
-        <v>510</v>
-      </c>
+      <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="F205" s="8"/>
       <c r="G205" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="10" t="s">
-        <v>738</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
+        <v>740</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C206" s="11"/>
-      <c r="D206" s="11"/>
+        <v>518</v>
+      </c>
+      <c r="C206" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D206" s="8" t="s">
+        <v>514</v>
+      </c>
       <c r="E206" s="8" t="s">
-        <v>739</v>
-      </c>
-      <c r="F206" s="8" t="s">
-        <v>740</v>
+        <v>741</v>
+      </c>
+      <c r="F206" s="8"/>
+      <c r="G206" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="C207" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="C207" s="11"/>
+      <c r="D207" s="11"/>
+      <c r="E207" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="F207" s="8" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="C208" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="D207" s="8"/>
-      <c r="E207" s="8" t="s">
-        <v>742</v>
-      </c>
-      <c r="G207" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="B208" s="8" t="s">
-        <v>188</v>
-      </c>
+      <c r="D208" s="8"/>
       <c r="E208" s="8" t="s">
-        <v>744</v>
-      </c>
-      <c r="F208" s="8"/>
+        <v>746</v>
+      </c>
+      <c r="G208" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E209" s="8" t="s">
+        <v>748</v>
+      </c>
+      <c r="F209" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed EPiServer 6.x < v4 and EPiServer 6.x ≥ v4
Fixed EPiServer 6.x < v4 and EPiServer 6.x ≥ v4 regular expression
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="749">
   <si>
     <t>Hash</t>
   </si>
@@ -209,7 +209,7 @@
     <t>^(\$cisco4\$)?[a-z0-9\/.]{43}$/i</t>
   </si>
   <si>
-    <t>jHSXiU.oQTuJ/lmrcyVL1on3EL4Jdd5J7S3y34QiQDQ </t>
+    <t>jHSXiU.oQTuJ/lmrcyVL1on3EL4Jdd5J7S3y34QiQDQ</t>
   </si>
   <si>
     <t>http://www.tobtu.com/cisco4tosha256.php</t>
@@ -662,7 +662,7 @@
     <t>EPiServer 6.x &lt; v4</t>
   </si>
   <si>
-    <t>^\$episerver\$\*0\*[a-z0-9*\/=+]{52,53}$/i</t>
+    <t>^\$episerver\$\*0\*[a-z0-9\/=+]+\*[a-z0-9\/=+]{27,28}$/i</t>
   </si>
   <si>
     <t>episerver</t>
@@ -674,7 +674,7 @@
     <t>EPiServer 6.x ≥ v4</t>
   </si>
   <si>
-    <t>^\$episerver\$\*1\*[a-z0-9=*+]{68}$/i</t>
+    <t>^\$episerver\$\*1\*[a-z0-9\/=+]+\*[a-z0-9\/=+]{42,43}$/i</t>
   </si>
   <si>
     <t>$episerver$*1*MDEyMzQ1Njc4OWFiY2RlZg==*lRjiU46qHA7S6ZE7RfKUcYhB85ofArj1j7TrCtu3u6Y</t>
@@ -2449,8 +2449,8 @@
   </sheetPr>
   <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2746,7 +2746,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
@@ -3463,9 +3463,6 @@
       <c r="F55" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G55" s="4" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
@@ -3483,9 +3480,6 @@
       </c>
       <c r="F56" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fixed GRUB 2 regex
Fixed GRUB 2 regular expression
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -776,7 +776,7 @@
     <t>GRUB 2</t>
   </si>
   <si>
-    <t>^grub\.pbkdf2\.sha512\.[0-9]+\.[a-f0-9]{128,2048}\.[a-f0-9]{128}$/i</t>
+    <t>^grub\.pbkdf2\.sha512\.[0-9]+\.([a-f0-9]{128,2048}|[0-9]+)?\.[a-f0-9]{128}$/i</t>
   </si>
   <si>
     <t>grub.pbkdf2.sha512.10000.7d391ef48645f626b427b1fae06a7219b5b54f4f02b2621f86b5e36e83ae492bd1db60871e45bc07925cecb46ff8ba3db31c723c0c6acbd4f06f60c5b246ecbf.26d59c52b50df90d043f070bd9cbcd92a74424da42b3666fdeb08f1a54b8f1d2f4f56cf436f9382419c26798dc2c209a86003982b1e5a9fcef905f4dfaa4c524</t>
@@ -2449,8 +2449,8 @@
   </sheetPr>
   <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3444,7 +3444,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
         <v>214</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
         <v>218</v>
       </c>

</xml_diff>

<commit_message>
Add JtR format mssql05
Forgot to add JtR format to MSSQL(2008)
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="750">
   <si>
     <t>Hash</t>
   </si>
@@ -776,7 +776,7 @@
     <t>GRUB 2</t>
   </si>
   <si>
-    <t>^grub\.pbkdf2\.sha512\.[0-9]+\.([a-f0-9]{128,2048}|[0-9]+)?\.[a-f0-9]{128}$/i</t>
+    <t>^grub\.pbkdf2\.sha512\.[0-9]+\.([a-f0-9]{128,2048}\.|[0-9]+\.)?[a-f0-9]{128}$/i</t>
   </si>
   <si>
     <t>grub.pbkdf2.sha512.10000.7d391ef48645f626b427b1fae06a7219b5b54f4f02b2621f86b5e36e83ae492bd1db60871e45bc07925cecb46ff8ba3db31c723c0c6acbd4f06f60c5b246ecbf.26d59c52b50df90d043f070bd9cbcd92a74424da42b3666fdeb08f1a54b8f1d2f4f56cf436f9382419c26798dc2c209a86003982b1e5a9fcef905f4dfaa4c524</t>
@@ -1281,6 +1281,9 @@
   </si>
   <si>
     <t>MSSQL(2008)</t>
+  </si>
+  <si>
+    <t>mssql05 </t>
   </si>
   <si>
     <t>MSSQL(2012)</t>
@@ -2449,8 +2452,8 @@
   </sheetPr>
   <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A113" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4499,7 +4502,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
         <v>421</v>
       </c>
@@ -4509,7 +4512,9 @@
       <c r="C113" s="11" t="n">
         <v>132</v>
       </c>
-      <c r="D113" s="11"/>
+      <c r="D113" s="12" t="s">
+        <v>422</v>
+      </c>
       <c r="E113" s="8"/>
       <c r="G113" s="4" t="s">
         <v>86</v>
@@ -4517,19 +4522,19 @@
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C114" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="G114" s="4" t="s">
         <v>86</v>
@@ -4537,45 +4542,45 @@
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C115" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C116" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D116" s="8"/>
       <c r="E116" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>123</v>
@@ -4584,50 +4589,50 @@
         <v>200</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="15" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C119" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F119" s="8"/>
       <c r="G119" s="4" t="s">
@@ -4636,17 +4641,17 @@
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C120" s="8" t="n">
         <v>5500</v>
       </c>
       <c r="D120" s="8"/>
       <c r="E120" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>86</v>
@@ -4654,19 +4659,19 @@
     </row>
     <row r="121" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>86</v>
@@ -4674,19 +4679,19 @@
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C122" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>86</v>
@@ -4694,19 +4699,19 @@
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C123" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>86</v>
@@ -4714,32 +4719,32 @@
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C124" s="11"/>
       <c r="D124" s="11"/>
       <c r="E124" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C125" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E125" s="8" t="s">
         <v>363</v>
@@ -4750,27 +4755,27 @@
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C126" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F126" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B127" s="8" t="s">
         <v>123</v>
@@ -4780,33 +4785,33 @@
       </c>
       <c r="D127" s="8"/>
       <c r="E127" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>269</v>
@@ -4815,10 +4820,10 @@
         <v>122</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G129" s="4" t="s">
         <v>86</v>
@@ -4826,19 +4831,19 @@
     </row>
     <row r="130" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C130" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="G130" s="4" t="s">
         <v>86</v>
@@ -4846,19 +4851,19 @@
     </row>
     <row r="131" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C131" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="G131" s="4" t="s">
         <v>86</v>
@@ -4866,15 +4871,15 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C132" s="11"/>
       <c r="D132" s="11"/>
       <c r="E132" s="8" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F132" s="8"/>
       <c r="G132" s="4" t="s">
@@ -4883,89 +4888,89 @@
     </row>
     <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C133" s="3"/>
       <c r="E133" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C134" s="11"/>
       <c r="D134" s="11"/>
       <c r="E134" s="8" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F134" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="8" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C136" s="11"/>
       <c r="D136" s="11" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C137" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E137" s="8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>308</v>
@@ -4974,30 +4979,30 @@
         <v>400</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C139" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E139" s="8" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F139" s="8"/>
       <c r="G139" s="4" t="s">
@@ -5006,74 +5011,74 @@
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C140" s="9" t="n">
         <v>2612</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E140" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C141" s="3"/>
       <c r="E141" s="8" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="10" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="F142" s="8" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F143" s="8"/>
       <c r="G143" s="4" t="s">
@@ -5082,43 +5087,43 @@
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="10" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C144" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D144" s="8"/>
       <c r="E144" s="8" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F144" s="8" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>192</v>
       </c>
       <c r="C145" s="11"/>
       <c r="D145" s="11" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="10" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B146" s="8" t="s">
         <v>195</v>
@@ -5127,18 +5132,18 @@
         <v>6000</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F146" s="8" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>248</v>
@@ -5146,164 +5151,164 @@
       <c r="C147" s="11"/>
       <c r="D147" s="11"/>
       <c r="E147" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C148" s="11"/>
       <c r="D148" s="11"/>
       <c r="E148" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C149" s="11"/>
       <c r="D149" s="11"/>
       <c r="E149" s="8" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C150" s="11"/>
       <c r="D150" s="11"/>
       <c r="E150" s="8" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C151" s="11"/>
       <c r="D151" s="11"/>
       <c r="E151" s="8" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C152" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E152" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C153" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D153" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E153" s="8" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B154" s="17" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C154" s="14" t="n">
         <v>10300</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C156" s="9" t="n">
         <v>8900</v>
       </c>
       <c r="E156" s="12" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="G156" s="4" t="s">
         <v>11</v>
@@ -5311,7 +5316,7 @@
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B157" s="8" t="s">
         <v>195</v>
@@ -5320,48 +5325,48 @@
         <v>100</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E157" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C158" s="11"/>
       <c r="D158" s="11" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C159" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D159" s="12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G159" s="4" t="s">
         <v>86</v>
@@ -5369,7 +5374,7 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>269</v>
@@ -5377,7 +5382,7 @@
       <c r="C160" s="11"/>
       <c r="D160" s="11"/>
       <c r="E160" s="8" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F160" s="8"/>
       <c r="G160" s="4" t="s">
@@ -5386,25 +5391,25 @@
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B161" s="8" t="s">
         <v>272</v>
       </c>
       <c r="C161" s="11"/>
       <c r="D161" s="11" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="E161" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="10" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>248</v>
@@ -5413,174 +5418,174 @@
         <v>1400</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C163" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C164" s="11"/>
       <c r="D164" s="11" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="E164" s="8" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C165" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="E165" s="8" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C166" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E166" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>272</v>
       </c>
       <c r="C167" s="3"/>
       <c r="E167" s="8" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="10" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>248</v>
       </c>
       <c r="C168" s="11" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D168" s="11" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C169" s="11"/>
       <c r="D169" s="11"/>
       <c r="E169" s="8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C170" s="11"/>
       <c r="D170" s="11" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C171" s="14" t="n">
         <v>10100</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="G171" s="4" t="s">
         <v>86</v>
@@ -5588,73 +5593,73 @@
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C172" s="11"/>
       <c r="D172" s="11"/>
       <c r="E172" s="8" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C173" s="11"/>
       <c r="D173" s="11"/>
       <c r="E173" s="8" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C174" s="11"/>
       <c r="D174" s="11"/>
       <c r="E174" s="8" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B175" s="8" t="s">
         <v>248</v>
       </c>
       <c r="C175" s="11"/>
       <c r="D175" s="11" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E175" s="8" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B176" s="8" t="s">
         <v>192</v>
@@ -5662,15 +5667,15 @@
       <c r="C176" s="11"/>
       <c r="D176" s="11"/>
       <c r="E176" s="8" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B177" s="8" t="s">
         <v>195</v>
@@ -5678,15 +5683,15 @@
       <c r="C177" s="11"/>
       <c r="D177" s="11"/>
       <c r="E177" s="8" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B178" s="8" t="s">
         <v>272</v>
@@ -5694,33 +5699,33 @@
       <c r="C178" s="11"/>
       <c r="D178" s="11"/>
       <c r="E178" s="8" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E179" s="8" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B180" s="8" t="s">
         <v>192</v>
@@ -5728,15 +5733,15 @@
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>195</v>
@@ -5744,15 +5749,15 @@
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>272</v>
@@ -5760,15 +5765,15 @@
       <c r="C182" s="11"/>
       <c r="D182" s="11"/>
       <c r="E182" s="8" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>248</v>
@@ -5776,58 +5781,58 @@
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C185" s="9" t="n">
         <v>23</v>
       </c>
       <c r="E185" s="8" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="F185" s="9" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C186" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D186" s="8"/>
       <c r="E186" s="8" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="G186" s="4" t="s">
         <v>86</v>
@@ -5835,53 +5840,53 @@
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B187" s="8" t="s">
         <v>192</v>
       </c>
       <c r="C187" s="11"/>
       <c r="D187" s="11" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E187" s="8" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C188" s="11"/>
       <c r="D188" s="11" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E188" s="8" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C189" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D189" s="8"/>
       <c r="E189" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G189" s="4" t="s">
         <v>86</v>
@@ -5889,7 +5894,7 @@
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B190" s="8" t="s">
         <v>327</v>
@@ -5898,7 +5903,7 @@
         <v>1711</v>
       </c>
       <c r="D190" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="E190" s="8" t="s">
         <v>328</v>
@@ -5909,47 +5914,47 @@
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C191" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D191" s="8" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="E191" s="8" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C192" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B193" s="8" t="s">
         <v>192</v>
@@ -5957,15 +5962,15 @@
       <c r="C193" s="11"/>
       <c r="D193" s="11"/>
       <c r="E193" s="8" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B194" s="8" t="s">
         <v>195</v>
@@ -5973,33 +5978,33 @@
       <c r="C194" s="11"/>
       <c r="D194" s="11"/>
       <c r="E194" s="8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B195" s="8" t="s">
         <v>269</v>
       </c>
       <c r="C195" s="11"/>
       <c r="D195" s="11" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="E195" s="8" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B196" s="8" t="s">
         <v>142</v>
@@ -6011,7 +6016,7 @@
         <v>143</v>
       </c>
       <c r="E196" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="F196" s="8" t="s">
         <v>145</v>
@@ -6019,17 +6024,17 @@
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C197" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D197" s="8"/>
       <c r="E197" s="8" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="G197" s="4" t="s">
         <v>86</v>
@@ -6037,17 +6042,17 @@
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C198" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D198" s="8"/>
       <c r="E198" s="8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G198" s="4" t="s">
         <v>86</v>
@@ -6055,7 +6060,7 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B199" s="8" t="s">
         <v>248</v>
@@ -6063,7 +6068,7 @@
       <c r="C199" s="11"/>
       <c r="D199" s="11"/>
       <c r="E199" s="8" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F199" s="8"/>
       <c r="G199" s="4" t="s">
@@ -6072,98 +6077,98 @@
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C200" s="11"/>
       <c r="D200" s="11" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="E200" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C201" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D201" s="8"/>
       <c r="E201" s="8" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C202" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E202" s="8" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C203" s="11" t="n">
         <v>8400</v>
       </c>
       <c r="D203" s="11" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="E203" s="8" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="F203" s="8" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B204" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C204" s="3"/>
       <c r="E204" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B205" s="8" t="s">
         <v>308</v>
@@ -6173,7 +6178,7 @@
       </c>
       <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="F205" s="8"/>
       <c r="G205" s="4" t="s">
@@ -6182,19 +6187,19 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C206" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E206" s="8" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="F206" s="8"/>
       <c r="G206" s="4" t="s">
@@ -6203,7 +6208,7 @@
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B207" s="8" t="s">
         <v>16</v>
@@ -6211,25 +6216,25 @@
       <c r="C207" s="11"/>
       <c r="D207" s="11"/>
       <c r="E207" s="8" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C208" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="8" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="G208" s="4" t="s">
         <v>86</v>
@@ -6237,13 +6242,13 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B209" s="8" t="s">
         <v>192</v>
       </c>
       <c r="E209" s="8" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="F209" s="8"/>
     </row>

</xml_diff>

<commit_message>
Add JtR format for Cisco Type 4,8 & 9
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="765">
   <si>
     <t>Hash</t>
   </si>
@@ -209,7 +209,10 @@
     <t>^(\$cisco4\$)?[a-z0-9\/.]{43}$/i</t>
   </si>
   <si>
-    <t>jHSXiU.oQTuJ/lmrcyVL1on3EL4Jdd5J7S3y34QiQDQ</t>
+    <t>cisco4</t>
+  </si>
+  <si>
+    <t>$cisco4$jHSXiU.oQTuJ/lmrcyVL1on3EL4Jdd5J7S3y34QiQDQ</t>
   </si>
   <si>
     <t>http://www.tobtu.com/cisco4tosha256.php</t>
@@ -221,7 +224,10 @@
     <t>^\$8\$[a-z0-9\/.]{14}\$[a-z0-9\/.]{43}$/i</t>
   </si>
   <si>
-    <t>$8$TnGX/fE4KGHOVU$pEhnEvxrvaynpi8j4f.EMHr6M.FzU8xnZnBr/tJdFWk</t>
+    <t>cisco8</t>
+  </si>
+  <si>
+    <t>$8$BlV23O2yWA.Qrb$wGsPC6b6KxfjBHdq3RHQCEGrx27.cucxi9cmtyRKczQ</t>
   </si>
   <si>
     <t>http://hashcat.net/forum/thread-3803.html</t>
@@ -231,6 +237,9 @@
   </si>
   <si>
     <t>^\$9\$[a-z0-9\/.]{14}\$[a-z0-9\/.]{43}$/i</t>
+  </si>
+  <si>
+    <t>cisco9</t>
   </si>
   <si>
     <t>$9$2MJBozw/9R3UsU$2lFhcKvpghcyw8deP25GOfyZaagyUOGBymkryvOdfo6</t>
@@ -2488,8 +2497,8 @@
   </sheetPr>
   <dimension ref="A1:G212"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2792,263 +2801,272 @@
       <c r="B15" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="E15" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="9" t="n">
         <v>9200</v>
       </c>
+      <c r="D16" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="E16" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C17" s="9" t="n">
         <v>9300</v>
       </c>
+      <c r="D17" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="E17" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C19" s="8" t="n">
         <v>2410</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C20" s="8" t="n">
         <v>500</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C21" s="8" t="n">
         <v>5700</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C22" s="8" t="n">
         <v>2400</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C23" s="8" t="n">
         <v>8100</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C25" s="14" t="n">
         <v>10200</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>16</v>
@@ -3056,410 +3074,410 @@
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="8" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C36" s="8" t="n">
         <v>3100</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F36" s="8"/>
       <c r="G36" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C37" s="8" t="n">
         <v>1500</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>10000</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="8" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
       <c r="E46" s="8" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C47" s="11" t="n">
         <v>8300</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="8" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C48" s="8" t="n">
         <v>1100</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C49" s="8" t="n">
         <v>2100</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C50" s="11" t="n">
         <v>2600</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="8" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C51" s="11" t="n">
         <v>4500</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="8" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C52" s="8" t="n">
         <v>7900</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="11" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>16</v>
@@ -3467,105 +3485,105 @@
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" s="8" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C55" s="8" t="n">
         <v>123</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C56" s="8" t="n">
         <v>141</v>
       </c>
       <c r="D56" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C57" s="8" t="n">
         <v>1441</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="8" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="8" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="8" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>16</v>
@@ -3573,15 +3591,15 @@
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="8" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>16</v>
@@ -3589,15 +3607,15 @@
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="8" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>16</v>
@@ -3605,72 +3623,72 @@
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="8" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="10" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="8" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C64" s="8" t="n">
         <v>7000</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C65" s="8" t="n">
         <v>500</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>16</v>
@@ -3678,16 +3696,16 @@
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
       <c r="E66" s="8" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="F66" s="8"/>
       <c r="G66" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>16</v>
@@ -3695,204 +3713,204 @@
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="8" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C68" s="8" t="n">
         <v>6900</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C69" s="8" t="n">
         <v>7200</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="8" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C70" s="8" t="n">
         <v>5100</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="8" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="8" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
       <c r="E73" s="8" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
       <c r="E74" s="8" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
       <c r="E75" s="8" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C77" s="11" t="n">
         <v>1421</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="12" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C78" s="9" t="n">
         <v>5300</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>11</v>
@@ -3900,19 +3918,19 @@
     </row>
     <row r="79" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C79" s="9" t="n">
         <v>5400</v>
       </c>
       <c r="E79" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="F79" s="9" t="s">
         <v>293</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>290</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>11</v>
@@ -3920,63 +3938,63 @@
     </row>
     <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="15" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C80" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D80" s="8"/>
       <c r="E80" s="8" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C81" s="11" t="n">
         <v>7300</v>
       </c>
       <c r="D81" s="11"/>
       <c r="E81" s="8" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C82" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>16</v>
@@ -3984,86 +4002,86 @@
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
       <c r="E83" s="8" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C84" s="8" t="n">
         <v>11</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="8" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C86" s="8" t="n">
         <v>22</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="C87" s="8" t="n">
         <v>7500</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>11</v>
@@ -4071,249 +4089,249 @@
     </row>
     <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C88" s="8" t="n">
         <v>6800</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="8" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C89" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="8" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
       <c r="E90" s="8" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F90" s="8"/>
       <c r="G90" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C91" s="8" t="n">
         <v>190</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C92" s="8" t="n">
         <v>3000</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C95" s="9" t="n">
         <v>9100</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="8" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="8" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C98" s="8" t="n">
         <v>900</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C100" s="8" t="n">
         <v>500</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>45</v>
@@ -4331,1056 +4349,1056 @@
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C102" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E102" s="8" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
       <c r="E104" s="8" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="12" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C105" s="9" t="n">
         <v>9700</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="12" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C106" s="9" t="n">
         <v>9800</v>
       </c>
       <c r="E106" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="F106" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C107" s="9" t="n">
         <v>9400</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C108" s="9" t="n">
         <v>9500</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C109" s="9" t="n">
         <v>9600</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
       <c r="E110" s="8" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="8" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C112" s="8" t="n">
         <v>131</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C113" s="8" t="n">
         <v>132</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C114" s="11" t="n">
         <v>132</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E114" s="8"/>
       <c r="G114" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C115" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>431</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>428</v>
       </c>
       <c r="C116" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C117" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="8" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>200</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="15" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C119" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C120" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F120" s="8"/>
       <c r="G120" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>5500</v>
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="8" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="C122" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="G122" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="C123" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="C125" s="11"/>
       <c r="D125" s="11"/>
       <c r="E125" s="8" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="C126" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C127" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>3100</v>
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="8" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C129" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="8" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C130" s="8" t="n">
         <v>122</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C131" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="G131" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="C132" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="C133" s="11"/>
       <c r="D133" s="11"/>
       <c r="E133" s="8" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="F133" s="8"/>
       <c r="G133" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="F134" s="8" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="E135" s="12" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="C137" s="3"/>
       <c r="E137" s="8" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="8" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="8" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="C140" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E140" s="8" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C141" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C142" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="F142" s="8"/>
       <c r="G142" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C143" s="9" t="n">
         <v>2612</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="F143" s="8" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="F144" s="9" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="10" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="D146" s="11" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="F146" s="8"/>
       <c r="G146" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C147" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D147" s="8"/>
       <c r="E147" s="8" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C148" s="11"/>
       <c r="D148" s="11" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C149" s="8" t="n">
         <v>6000</v>
       </c>
       <c r="D149" s="8" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="E149" s="8" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C150" s="11"/>
       <c r="D150" s="11"/>
       <c r="E150" s="8" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="C151" s="11"/>
       <c r="D151" s="11"/>
       <c r="E151" s="8" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
       <c r="E152" s="8" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
+        <v>577</v>
+      </c>
+      <c r="B153" s="8" t="s">
         <v>574</v>
-      </c>
-      <c r="B153" s="8" t="s">
-        <v>571</v>
       </c>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="8" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="C155" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D155" s="8" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="E155" s="8" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="C156" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D156" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="E156" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="F156" s="8" t="s">
         <v>588</v>
-      </c>
-      <c r="E156" s="8" t="s">
-        <v>589</v>
-      </c>
-      <c r="F156" s="8" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="B157" s="17" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="C157" s="14" t="n">
         <v>10300</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
       <c r="E158" s="8" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C159" s="9" t="n">
         <v>8900</v>
       </c>
       <c r="E159" s="12" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="G159" s="4" t="s">
         <v>11</v>
@@ -5388,897 +5406,897 @@
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C160" s="11" t="n">
         <v>100</v>
       </c>
       <c r="D160" s="11" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="E160" s="8" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="C161" s="11"/>
       <c r="D161" s="11" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="E161" s="8" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="10" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C162" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="G162" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C163" s="11"/>
       <c r="D163" s="11"/>
       <c r="E163" s="8" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="F163" s="8"/>
       <c r="G163" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C164" s="11"/>
       <c r="D164" s="11" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="E164" s="8" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C165" s="8" t="n">
         <v>1400</v>
       </c>
       <c r="D165" s="8" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="E165" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="F165" s="8" t="s">
         <v>621</v>
-      </c>
-      <c r="F165" s="8" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="C166" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="E166" s="8" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C167" s="11"/>
       <c r="D167" s="11" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="E167" s="8" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="10" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C168" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="C169" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C171" s="11" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="D171" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="E171" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="F171" s="8" t="s">
         <v>644</v>
-      </c>
-      <c r="E171" s="8" t="s">
-        <v>645</v>
-      </c>
-      <c r="F171" s="8" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C172" s="11"/>
       <c r="D172" s="11"/>
       <c r="E172" s="8" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C173" s="11"/>
       <c r="D173" s="11" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="E173" s="8" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="C174" s="14" t="n">
         <v>10100</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="G174" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="C175" s="11"/>
       <c r="D175" s="11"/>
       <c r="E175" s="8" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C176" s="11"/>
       <c r="D176" s="11"/>
       <c r="E176" s="8" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C177" s="11"/>
       <c r="D177" s="11"/>
       <c r="E177" s="8" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C178" s="11"/>
       <c r="D178" s="11" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="E178" s="8" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11"/>
       <c r="E179" s="8" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C182" s="11"/>
       <c r="D182" s="11" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="E182" s="8" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C186" s="11"/>
       <c r="D186" s="11"/>
       <c r="E186" s="8" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="C188" s="9" t="n">
         <v>23</v>
       </c>
       <c r="E188" s="8" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="F188" s="9" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="C189" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D189" s="8"/>
       <c r="E189" s="8" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="G189" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C190" s="11"/>
       <c r="D190" s="11" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="E190" s="8" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="C191" s="11"/>
       <c r="D191" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="F191" s="8" t="s">
         <v>697</v>
-      </c>
-      <c r="E191" s="8" t="s">
-        <v>698</v>
-      </c>
-      <c r="F191" s="8" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C192" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D192" s="8"/>
       <c r="E192" s="8" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="G192" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C193" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D193" s="8" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="E193" s="8" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="C194" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="E194" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="C195" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="E195" s="8" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C196" s="11"/>
       <c r="D196" s="11"/>
       <c r="E196" s="8" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C197" s="11"/>
       <c r="D197" s="11"/>
       <c r="E197" s="8" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C198" s="11"/>
       <c r="D198" s="11" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="E198" s="8" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C199" s="8" t="n">
         <v>1500</v>
       </c>
       <c r="D199" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E199" s="8" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="C200" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D200" s="8"/>
       <c r="E200" s="8" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="G200" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="C201" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D201" s="8"/>
       <c r="E201" s="8" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="G201" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C202" s="11"/>
       <c r="D202" s="11"/>
       <c r="E202" s="8" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="F202" s="8"/>
       <c r="G202" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="C203" s="11"/>
       <c r="D203" s="11" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="E203" s="8" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="F203" s="8" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="C204" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D204" s="8"/>
       <c r="E204" s="8" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C205" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="E205" s="8" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
     </row>
     <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="C206" s="11" t="n">
         <v>8400</v>
       </c>
       <c r="D206" s="11" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="E206" s="8" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="F206" s="8" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B207" s="8" t="s">
         <v>53</v>
       </c>
       <c r="E207" s="8" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C208" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="8" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="F208" s="8"/>
       <c r="G208" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C209" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E209" s="8" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="F209" s="8"/>
       <c r="G209" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="10" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="B210" s="8" t="s">
         <v>16</v>
@@ -6286,39 +6304,39 @@
       <c r="C210" s="11"/>
       <c r="D210" s="11"/>
       <c r="E210" s="8" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="F210" s="8" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
     </row>
     <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="10" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C211" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D211" s="8"/>
       <c r="E211" s="8" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="G211" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E212" s="8" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="F212" s="8"/>
     </row>

</xml_diff>

<commit_message>
Add JtR format for MD2
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="770">
   <si>
     <t>Hash</t>
   </si>
@@ -1118,7 +1118,10 @@
     <t>^(\$md2\$)?[a-f0-9]{32}$/i</t>
   </si>
   <si>
-    <t>8350e5a3e24c153df2275c9f80692773</t>
+    <t>rawmd2</t>
+  </si>
+  <si>
+    <t>fcdcaaa9794d753db7da35230ef5dd7a</t>
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/MD2_%28cryptography%29</t>
@@ -2509,8 +2512,8 @@
   </sheetPr>
   <dimension ref="A1:G213"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A143" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4273,17 +4276,19 @@
         <v>366</v>
       </c>
       <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
+      <c r="D97" s="11" t="s">
+        <v>367</v>
+      </c>
       <c r="E97" s="8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>200</v>
@@ -4292,38 +4297,38 @@
         <v>900</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>200</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>86</v>
@@ -4335,15 +4340,15 @@
         <v>87</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>45</v>
@@ -4361,7 +4366,7 @@
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>304</v>
@@ -4381,215 +4386,215 @@
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C104" s="11"/>
       <c r="D104" s="11"/>
       <c r="E104" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="12" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C105" s="9" t="n">
         <v>9700</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="12" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C106" s="9" t="n">
         <v>9800</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C107" s="9" t="n">
         <v>9400</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C108" s="9" t="n">
         <v>9500</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C109" s="9" t="n">
         <v>9600</v>
       </c>
       <c r="E109" s="9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
       <c r="E110" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C112" s="8" t="n">
         <v>131</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C113" s="8" t="n">
         <v>132</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C114" s="11" t="n">
         <v>132</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E114" s="8"/>
       <c r="G114" s="4" t="s">
@@ -4598,19 +4603,19 @@
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C115" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>89</v>
@@ -4618,45 +4623,45 @@
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C116" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C117" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>126</v>
@@ -4665,50 +4670,50 @@
         <v>200</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="15" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C119" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C120" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F120" s="8"/>
       <c r="G120" s="4" t="s">
@@ -4717,17 +4722,17 @@
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>5500</v>
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>89</v>
@@ -4735,19 +4740,19 @@
     </row>
     <row r="122" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C122" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>89</v>
@@ -4755,19 +4760,19 @@
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C123" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>89</v>
@@ -4775,19 +4780,19 @@
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>89</v>
@@ -4795,35 +4800,35 @@
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C125" s="11"/>
       <c r="D125" s="11"/>
       <c r="E125" s="8" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C126" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>89</v>
@@ -4831,27 +4836,27 @@
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C127" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>126</v>
@@ -4861,33 +4866,33 @@
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C129" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>277</v>
@@ -4896,10 +4901,10 @@
         <v>122</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="G130" s="4" t="s">
         <v>89</v>
@@ -4907,19 +4912,19 @@
     </row>
     <row r="131" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C131" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G131" s="4" t="s">
         <v>89</v>
@@ -4927,19 +4932,19 @@
     </row>
     <row r="132" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C132" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="G132" s="4" t="s">
         <v>89</v>
@@ -4947,15 +4952,15 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C133" s="11"/>
       <c r="D133" s="11"/>
       <c r="E133" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F133" s="8"/>
       <c r="G133" s="4" t="s">
@@ -4964,116 +4969,116 @@
     </row>
     <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F134" s="8" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E135" s="12" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C137" s="3"/>
       <c r="E137" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="8" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C140" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E140" s="8" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>316</v>
@@ -5082,30 +5087,30 @@
         <v>400</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C142" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F142" s="8"/>
       <c r="G142" s="4" t="s">
@@ -5114,39 +5119,39 @@
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C143" s="9" t="n">
         <v>2612</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F143" s="8" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C144" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G144" s="4" t="s">
         <v>89</v>
@@ -5154,53 +5159,53 @@
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F145" s="9" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="10" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F146" s="8" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D147" s="11" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F147" s="8"/>
       <c r="G147" s="4" t="s">
@@ -5209,43 +5214,43 @@
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C148" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D148" s="8"/>
       <c r="E148" s="8" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B149" s="8" t="s">
         <v>200</v>
       </c>
       <c r="C149" s="11"/>
       <c r="D149" s="11" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E149" s="8" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>203</v>
@@ -5254,18 +5259,18 @@
         <v>6000</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E150" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>256</v>
@@ -5273,164 +5278,164 @@
       <c r="C151" s="11"/>
       <c r="D151" s="11"/>
       <c r="E151" s="8" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
       <c r="E152" s="8" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="8" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C156" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E156" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C157" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E157" s="8" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B158" s="17" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C158" s="14" t="n">
         <v>10300</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C159" s="11"/>
       <c r="D159" s="11"/>
       <c r="E159" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C160" s="9" t="n">
         <v>8900</v>
       </c>
       <c r="E160" s="12" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G160" s="4" t="s">
         <v>11</v>
@@ -5438,7 +5443,7 @@
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B161" s="8" t="s">
         <v>203</v>
@@ -5447,48 +5452,48 @@
         <v>100</v>
       </c>
       <c r="D161" s="11" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E161" s="8" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="10" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C162" s="11"/>
       <c r="D162" s="11" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C163" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D163" s="12" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="G163" s="4" t="s">
         <v>89</v>
@@ -5496,7 +5501,7 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B164" s="8" t="s">
         <v>277</v>
@@ -5504,7 +5509,7 @@
       <c r="C164" s="11"/>
       <c r="D164" s="11"/>
       <c r="E164" s="8" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="F164" s="8"/>
       <c r="G164" s="4" t="s">
@@ -5513,25 +5518,25 @@
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>280</v>
       </c>
       <c r="C165" s="11"/>
       <c r="D165" s="11" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="E165" s="8" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>256</v>
@@ -5540,173 +5545,173 @@
         <v>1400</v>
       </c>
       <c r="D166" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E166" s="8" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C167" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E167" s="8" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="10" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C168" s="11"/>
       <c r="D168" s="11" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C169" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C170" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B171" s="8" t="s">
         <v>280</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B172" s="8" t="s">
         <v>256</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D172" s="11" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C173" s="11"/>
       <c r="D173" s="11"/>
       <c r="E173" s="8" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C174" s="11"/>
       <c r="D174" s="11" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E174" s="8" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C175" s="14" t="n">
         <v>10100</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="G175" s="4" t="s">
         <v>89</v>
@@ -5714,73 +5719,73 @@
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C176" s="11"/>
       <c r="D176" s="11"/>
       <c r="E176" s="8" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C177" s="11"/>
       <c r="D177" s="11"/>
       <c r="E177" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C178" s="11"/>
       <c r="D178" s="11"/>
       <c r="E178" s="8" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B179" s="8" t="s">
         <v>256</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="E179" s="8" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B180" s="8" t="s">
         <v>200</v>
@@ -5788,15 +5793,15 @@
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>203</v>
@@ -5804,15 +5809,15 @@
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>280</v>
@@ -5820,33 +5825,33 @@
       <c r="C182" s="11"/>
       <c r="D182" s="11"/>
       <c r="E182" s="8" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C183" s="11"/>
       <c r="D183" s="11" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="E183" s="8" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B184" s="8" t="s">
         <v>200</v>
@@ -5854,15 +5859,15 @@
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B185" s="8" t="s">
         <v>203</v>
@@ -5870,15 +5875,15 @@
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B186" s="8" t="s">
         <v>280</v>
@@ -5886,15 +5891,15 @@
       <c r="C186" s="11"/>
       <c r="D186" s="11"/>
       <c r="E186" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B187" s="8" t="s">
         <v>256</v>
@@ -5902,58 +5907,58 @@
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C189" s="9" t="n">
         <v>23</v>
       </c>
       <c r="E189" s="8" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="F189" s="9" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C190" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D190" s="8"/>
       <c r="E190" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="G190" s="4" t="s">
         <v>89</v>
@@ -5961,53 +5966,53 @@
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B191" s="8" t="s">
         <v>200</v>
       </c>
       <c r="C191" s="11"/>
       <c r="D191" s="11" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="E191" s="8" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C192" s="11"/>
       <c r="D192" s="11" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C193" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G193" s="4" t="s">
         <v>89</v>
@@ -6015,7 +6020,7 @@
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B194" s="8" t="s">
         <v>335</v>
@@ -6024,7 +6029,7 @@
         <v>1711</v>
       </c>
       <c r="D194" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>336</v>
@@ -6035,47 +6040,47 @@
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C195" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="E195" s="8" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C196" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="E196" s="8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B197" s="8" t="s">
         <v>200</v>
@@ -6083,15 +6088,15 @@
       <c r="C197" s="11"/>
       <c r="D197" s="11"/>
       <c r="E197" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>203</v>
@@ -6099,33 +6104,33 @@
       <c r="C198" s="11"/>
       <c r="D198" s="11"/>
       <c r="E198" s="8" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B199" s="8" t="s">
         <v>277</v>
       </c>
       <c r="C199" s="11"/>
       <c r="D199" s="11" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E199" s="8" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>145</v>
@@ -6137,7 +6142,7 @@
         <v>146</v>
       </c>
       <c r="E200" s="8" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="F200" s="8" t="s">
         <v>148</v>
@@ -6145,17 +6150,17 @@
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C201" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D201" s="8"/>
       <c r="E201" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G201" s="4" t="s">
         <v>89</v>
@@ -6163,17 +6168,17 @@
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C202" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D202" s="8"/>
       <c r="E202" s="8" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="G202" s="4" t="s">
         <v>89</v>
@@ -6181,7 +6186,7 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B203" s="8" t="s">
         <v>256</v>
@@ -6189,7 +6194,7 @@
       <c r="C203" s="11"/>
       <c r="D203" s="11"/>
       <c r="E203" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="F203" s="8"/>
       <c r="G203" s="4" t="s">
@@ -6198,97 +6203,97 @@
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C204" s="11"/>
       <c r="D204" s="11" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="E204" s="8" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C205" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C206" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="E206" s="8" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="F206" s="8" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C207" s="11" t="n">
         <v>8400</v>
       </c>
       <c r="D207" s="11" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="E207" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B208" s="8" t="s">
         <v>53</v>
       </c>
       <c r="E208" s="8" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B209" s="8" t="s">
         <v>316</v>
@@ -6298,7 +6303,7 @@
       </c>
       <c r="D209" s="8"/>
       <c r="E209" s="8" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="F209" s="8"/>
       <c r="G209" s="4" t="s">
@@ -6307,19 +6312,19 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C210" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D210" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E210" s="8" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="F210" s="8"/>
       <c r="G210" s="4" t="s">
@@ -6328,7 +6333,7 @@
     </row>
     <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B211" s="8" t="s">
         <v>16</v>
@@ -6336,25 +6341,25 @@
       <c r="C211" s="11"/>
       <c r="D211" s="11"/>
       <c r="E211" s="8" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="10" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C212" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D212" s="8"/>
       <c r="E212" s="8" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="G212" s="4" t="s">
         <v>89</v>
@@ -6362,13 +6367,13 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B213" s="8" t="s">
         <v>200</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="F213" s="8"/>
     </row>

</xml_diff>

<commit_message>
Changed example hashes of AIX formats
AIX(ssha1), AIX(ssha256) & AIX(ssha512) example hash is now plaintext
"hashid" (generated using pass_gen.pl from JtR)
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -98,7 +98,7 @@
     <t>aix-ssha1</t>
   </si>
   <si>
-    <t>{ssha1}06$0123456789abcdef$pPDynUWwKgFKx8N5CP.d8D5C.wZ</t>
+    <t>{ssha1}06$0XBHm9SZpIYoMh4O$mYuhpJ405Vx4az8zelu4AaCZ.Ew</t>
   </si>
   <si>
     <t>AIX(ssha256)</t>
@@ -110,7 +110,7 @@
     <t>aix-ssha256</t>
   </si>
   <si>
-    <t>{ssha256}06$0123456789abcdef$9zHeDVOh2swHIvL1O9LPvTDeWwv0zbsB5n531R3J.UP</t>
+    <t>{ssha256}06$Rtyh5TThkOJILkUU$s.CmqkoEIasFVCrEQ2zqs5Xj3EbE4IniMaq52CK5.cs</t>
   </si>
   <si>
     <t>AIX(ssha512)</t>
@@ -122,7 +122,7 @@
     <t>aix-ssha512</t>
   </si>
   <si>
-    <t>{ssha512}06$otYx2eSXx.OkEY4F$71vDkRp8S0GNO96tgcvKDz7y8YYEenW8/mltpQsHuiueaHxSEMl1LMzQZTGQt7w.NLWoyb0WKZZfLuVtFIK...</t>
+    <t>{ssha512}06$BNlRyJFIRwc5fbdl$nHi24Li3fLfxEnEf2lnh9uJbsxM9iAPSIZDOr7fqBcQmK7yswabvzWbnmJ8lFfNMfWeB/GIZUcU1yHMIfDIQ..</t>
   </si>
   <si>
     <t>Android FDE ≤ 4.3</t>
@@ -2528,7 +2528,7 @@
   <dimension ref="A1:G214"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Fixed round size of AIX(ssha1) & AIX(ssha256)
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -92,7 +92,7 @@
     <t>AIX(ssha1)</t>
   </si>
   <si>
-    <t>^{ssha1}[a-z0-9$\/.]{47}$/i</t>
+    <t>^{ssha1}[0-9]{2}\$[a-z0-9$\/.]{44}$/i</t>
   </si>
   <si>
     <t>aix-ssha1</t>
@@ -104,7 +104,7 @@
     <t>AIX(ssha256)</t>
   </si>
   <si>
-    <t>^{ssha256}[a-z0-9$\/.]{63}$/i</t>
+    <t>^{ssha256}[0-9]{2}\$[a-z0-9$\/.]{60}$/i</t>
   </si>
   <si>
     <t>aix-ssha256</t>
@@ -2528,7 +2528,7 @@
   <dimension ref="A1:G214"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Updated and added more Resource links
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="782">
   <si>
     <t>Hash</t>
   </si>
@@ -674,6 +674,9 @@
     <t>+3nynz1ThEqm.</t>
   </si>
   <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/BFEgg_fmt_plug.c</t>
+  </si>
+  <si>
     <t>ELF-32</t>
   </si>
   <si>
@@ -782,6 +785,9 @@
     <t>AK1AAECAwQFBgcICRARNGqgeC3is8gv2xWWRony9NJnDgEA</t>
   </si>
   <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/FGT_fmt_plug.c</t>
+  </si>
+  <si>
     <t>FreeBSD MD5</t>
   </si>
   <si>
@@ -1337,6 +1343,9 @@
     <t>0x02000102030434ea1b17802fd95ea6316bd61d2c94622ca3812793e8fb1672487b5c904a45a31b2ab4a78890d563d2fcf5663e46fe797d71550494be50cf4915d3f4d55ec375</t>
   </si>
   <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/mssql12_fmt_plug.c</t>
+  </si>
+  <si>
     <t>MSSQL(2014)</t>
   </si>
   <si>
@@ -1499,7 +1508,10 @@
     <t>xsha</t>
   </si>
   <si>
-    <t>1430823483d07626ef8be3fda2ff056d0dfd818dbfe47683</t>
+    <t>31474835450D8103E7AEB9E7DFAC5C8CFE4A9F9F900F151D</t>
+  </si>
+  <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/XSHA_fmt_plug.c</t>
   </si>
   <si>
     <t>OSX v10.7</t>
@@ -1511,7 +1523,10 @@
     <t>xsha512</t>
   </si>
   <si>
-    <t>648742485c9b0acd786a233b2330197223118111b481abfa0ab8b3e8ede5f014fc7c523991c007db6882680b09962d16fd9c45568260531bdb34804a5e31c22b4cfeb32d</t>
+    <t>4c665543c5a19b495a987e95c014cfd5158af9042df969a6c43e7d8b00d641436ac6136eb4b8d9166772dd1422104448521246ecb3881b416639e5e70c84d27f3413e311</t>
+  </si>
+  <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/XSHA512_fmt_plug.c</t>
   </si>
   <si>
     <t>OSX v10.8-10.9</t>
@@ -1520,9 +1535,6 @@
     <t>^\$ml\$[0-9]+\$[a-f0-9]{64}\$[a-f0-9]{128}$/i</t>
   </si>
   <si>
-    <t>pbkdf2-hmac-sha512</t>
-  </si>
-  <si>
     <t>$ml$35460$93a94bd24b5de64d79a5e49fa372827e739f4d7b6975c752c9a0ff1e5cf72e05$752351df64dd2ce9dc9c64a72ad91de6581a15c19176266b44d98919dfa81f0f96cbcb20a1ffb400718c20382030f637892f776627d34e021bad4f81b7de8222</t>
   </si>
   <si>
@@ -1670,6 +1682,9 @@
     <t>$postgres$postgres*3677456e*00280f7a10b1c1f09c2053c9f0f5c0ea</t>
   </si>
   <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/postgres_fmt_plug.c</t>
+  </si>
+  <si>
     <t>PostgreSQL MD5</t>
   </si>
   <si>
@@ -1715,6 +1730,9 @@
     <t>6d0bb00954ceb7fbee436bb55a8397a9</t>
   </si>
   <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/radmin_fmt_plug.c</t>
+  </si>
+  <si>
     <t>Redmine Project Management Web App</t>
   </si>
   <si>
@@ -2016,6 +2034,9 @@
   </si>
   <si>
     <t>ad61d78c06037cd9:2:4:81533218127174468417660201434054</t>
+  </si>
+  <si>
+    <t>https://131002.net/siphash/</t>
   </si>
   <si>
     <t>Skein-1024</t>
@@ -2527,8 +2548,8 @@
   </sheetPr>
   <dimension ref="A1:G214"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2934,7 +2955,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
         <v>90</v>
       </c>
@@ -2954,7 +2975,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
         <v>95</v>
       </c>
@@ -3012,7 +3033,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>108</v>
       </c>
@@ -3447,7 +3468,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>204</v>
       </c>
@@ -3465,7 +3486,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>207</v>
       </c>
@@ -3517,14 +3538,13 @@
       <c r="E54" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="4" t="s">
-        <v>94</v>
+      <c r="F54" s="8" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>16</v>
@@ -3532,89 +3552,89 @@
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C56" s="8" t="n">
         <v>123</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C57" s="8" t="n">
         <v>141</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C58" s="8" t="n">
         <v>1441</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>116</v>
@@ -3622,15 +3642,15 @@
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>16</v>
@@ -3638,15 +3658,15 @@
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>16</v>
@@ -3654,15 +3674,15 @@
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>16</v>
@@ -3670,7 +3690,7 @@
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="4" t="s">
@@ -3679,7 +3699,7 @@
     </row>
     <row r="64" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>131</v>
@@ -3687,35 +3707,35 @@
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="65" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C65" s="8" t="n">
         <v>7000</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>255</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>91</v>
@@ -3735,7 +3755,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>16</v>
@@ -3743,7 +3763,7 @@
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="8" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F67" s="8"/>
       <c r="G67" s="4" t="s">
@@ -3752,7 +3772,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>16</v>
@@ -3760,7 +3780,7 @@
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="8" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="4" t="s">
@@ -3769,45 +3789,45 @@
     </row>
     <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C69" s="8" t="n">
         <v>6900</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C70" s="8" t="n">
         <v>7200</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="8" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>131</v>
@@ -3817,15 +3837,15 @@
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="8" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>208</v>
@@ -3833,33 +3853,33 @@
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="8" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>208</v>
@@ -3867,97 +3887,97 @@
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
       <c r="E74" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="F74" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="F74" s="8" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
       <c r="E75" s="8" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
       <c r="E76" s="8" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="10" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="11" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C78" s="11" t="n">
         <v>1421</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="79" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C79" s="9" t="n">
         <v>5300</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>11</v>
@@ -3965,55 +3985,55 @@
     </row>
     <row r="80" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="12" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C80" s="9" t="n">
         <v>5400</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="15" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C81" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="8" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C82" s="11" t="n">
         <v>7300</v>
       </c>
       <c r="D82" s="11"/>
       <c r="E82" s="8" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>94</v>
@@ -4021,27 +4041,27 @@
     </row>
     <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C83" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>16</v>
@@ -4049,86 +4069,86 @@
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="8" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C85" s="8" t="n">
         <v>11</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C87" s="8" t="n">
         <v>22</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C88" s="8" t="n">
         <v>7500</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>11</v>
@@ -4136,51 +4156,51 @@
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C89" s="8" t="n">
         <v>6800</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="8" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C90" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="8" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="8" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F91" s="8"/>
       <c r="G91" s="4" t="s">
@@ -4189,7 +4209,7 @@
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>208</v>
@@ -4198,18 +4218,18 @@
         <v>190</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>205</v>
@@ -4218,50 +4238,50 @@
         <v>3000</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="94" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>94</v>
@@ -4269,24 +4289,24 @@
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C96" s="9" t="n">
         <v>9100</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>208</v>
@@ -4294,33 +4314,33 @@
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="8" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="11" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>205</v>
@@ -4329,38 +4349,38 @@
         <v>900</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>91</v>
@@ -4372,15 +4392,15 @@
         <v>92</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>45</v>
@@ -4398,302 +4418,302 @@
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C103" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="10" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="8" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="12" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C106" s="9" t="n">
         <v>9700</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="12" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C107" s="9" t="n">
         <v>9800</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C108" s="9" t="n">
         <v>9400</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C109" s="9" t="n">
         <v>9500</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C110" s="9" t="n">
         <v>9600</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="8" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="8" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C113" s="8" t="n">
         <v>131</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C114" s="8" t="n">
         <v>132</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E114" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="F114" s="8" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="B115" s="8" t="s">
         <v>433</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="115" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>431</v>
       </c>
       <c r="C115" s="11" t="n">
         <v>132</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E115" s="8"/>
       <c r="G115" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C116" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="G116" s="4" t="s">
-        <v>94</v>
+        <v>441</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C117" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D118" s="8"/>
       <c r="E118" s="8" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B119" s="8" t="s">
         <v>131</v>
@@ -4702,129 +4722,128 @@
         <v>200</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="15" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C120" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="F121" s="8"/>
-      <c r="G121" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>460</v>
+      </c>
+      <c r="F121" s="8" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C122" s="8" t="n">
         <v>5500</v>
       </c>
       <c r="D122" s="8"/>
       <c r="E122" s="8" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="123" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C123" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C125" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="G125" s="4" t="s">
         <v>94</v>
@@ -4832,35 +4851,35 @@
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C126" s="11"/>
       <c r="D126" s="11"/>
       <c r="E126" s="8" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="F126" s="8" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C127" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G127" s="4" t="s">
         <v>94</v>
@@ -4868,27 +4887,27 @@
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>131</v>
@@ -4898,85 +4917,83 @@
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="8" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="C130" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C131" s="8" t="n">
         <v>122</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>494</v>
-      </c>
-      <c r="G131" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="132" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>497</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="C132" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="G132" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="133" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>502</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="C133" s="8" t="n">
         <v>7100</v>
       </c>
-      <c r="D133" s="12" t="s">
-        <v>501</v>
-      </c>
+      <c r="D133" s="12"/>
       <c r="E133" s="8" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="G133" s="4" t="s">
         <v>94</v>
@@ -4984,15 +5001,15 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="C134" s="11"/>
       <c r="D134" s="11"/>
       <c r="E134" s="8" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="F134" s="8"/>
       <c r="G134" s="4" t="s">
@@ -5001,148 +5018,148 @@
     </row>
     <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="E136" s="12" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="C138" s="3"/>
       <c r="E138" s="8" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="8" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="8" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="C141" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="10" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C142" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="F142" s="8" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C143" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="F143" s="8"/>
       <c r="G143" s="4" t="s">
@@ -5151,138 +5168,137 @@
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="C144" s="9" t="n">
         <v>2612</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="F144" s="8" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="C145" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="G145" s="4" t="s">
-        <v>94</v>
+        <v>554</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>565</v>
-      </c>
-      <c r="F148" s="8"/>
-      <c r="G148" s="4" t="s">
-        <v>94</v>
+        <v>570</v>
+      </c>
+      <c r="F148" s="8" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="C149" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D149" s="8"/>
       <c r="E149" s="8" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C150" s="11"/>
       <c r="D150" s="11" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="E150" s="8" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>208</v>
@@ -5291,183 +5307,184 @@
         <v>6000</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
       <c r="E152" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="F152" s="8" t="s">
         <v>579</v>
-      </c>
-      <c r="F152" s="8" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>580</v>
+        <v>586</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>581</v>
+        <v>587</v>
       </c>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="8" t="s">
-        <v>582</v>
+        <v>588</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>587</v>
+        <v>593</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>589</v>
+        <v>595</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>590</v>
+        <v>596</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>591</v>
+        <v>597</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
       <c r="E156" s="8" t="s">
-        <v>592</v>
+        <v>598</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>594</v>
+        <v>600</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="C157" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="E157" s="8" t="s">
-        <v>597</v>
+        <v>603</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>598</v>
+        <v>604</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>599</v>
+        <v>605</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>600</v>
+        <v>606</v>
       </c>
       <c r="C158" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>601</v>
+        <v>607</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>598</v>
+        <v>604</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="B159" s="17" t="s">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="C159" s="14" t="n">
         <v>10300</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>607</v>
+        <v>613</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
-        <v>608</v>
+        <v>614</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="C160" s="11"/>
       <c r="D160" s="11"/>
       <c r="E160" s="8" t="s">
-        <v>610</v>
+        <v>616</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="161" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>612</v>
+        <v>618</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>613</v>
+        <v>619</v>
       </c>
       <c r="C161" s="9" t="n">
         <v>8900</v>
       </c>
+      <c r="D161" s="1"/>
       <c r="E161" s="12" t="s">
-        <v>614</v>
+        <v>620</v>
       </c>
       <c r="G161" s="4" t="s">
         <v>11</v>
@@ -5475,7 +5492,7 @@
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="10" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>208</v>
@@ -5484,48 +5501,48 @@
         <v>100</v>
       </c>
       <c r="D162" s="11" t="s">
-        <v>616</v>
+        <v>622</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>617</v>
+        <v>623</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>618</v>
+        <v>624</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>619</v>
+        <v>625</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>620</v>
+        <v>626</v>
       </c>
       <c r="C163" s="11"/>
       <c r="D163" s="11" t="s">
-        <v>621</v>
+        <v>627</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>622</v>
+        <v>628</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="164" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>624</v>
+        <v>630</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="C164" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D164" s="12" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="E164" s="8" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G164" s="4" t="s">
         <v>94</v>
@@ -5533,15 +5550,15 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C165" s="11"/>
       <c r="D165" s="11"/>
       <c r="E165" s="8" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="F165" s="8"/>
       <c r="G165" s="4" t="s">
@@ -5550,274 +5567,275 @@
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
-        <v>628</v>
+        <v>634</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C166" s="11"/>
       <c r="D166" s="11" t="s">
-        <v>629</v>
+        <v>635</v>
       </c>
       <c r="E166" s="8" t="s">
-        <v>630</v>
+        <v>636</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C167" s="8" t="n">
         <v>1400</v>
       </c>
       <c r="D167" s="8" t="s">
-        <v>633</v>
+        <v>639</v>
       </c>
       <c r="E167" s="8" t="s">
-        <v>634</v>
+        <v>640</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="C168" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>638</v>
+        <v>644</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>639</v>
+        <v>645</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="C169" s="11"/>
       <c r="D169" s="11" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="C170" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>646</v>
+        <v>652</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>647</v>
+        <v>653</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="C171" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>649</v>
+        <v>655</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>650</v>
+        <v>656</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>653</v>
+        <v>659</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>655</v>
+        <v>661</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="D173" s="11" t="s">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="E173" s="8" t="s">
-        <v>658</v>
+        <v>664</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>659</v>
+        <v>665</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="C174" s="11"/>
       <c r="D174" s="11"/>
       <c r="E174" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="F174" s="8" t="s">
         <v>660</v>
-      </c>
-      <c r="F174" s="8" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="C175" s="11"/>
       <c r="D175" s="11" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="E175" s="8" t="s">
-        <v>663</v>
+        <v>669</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="176" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>665</v>
+        <v>671</v>
       </c>
       <c r="C176" s="14" t="n">
         <v>10100</v>
       </c>
+      <c r="D176" s="1"/>
       <c r="E176" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="G176" s="4" t="s">
-        <v>94</v>
+        <v>672</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>668</v>
+        <v>675</v>
       </c>
       <c r="C177" s="11"/>
       <c r="D177" s="11"/>
       <c r="E177" s="8" t="s">
-        <v>669</v>
+        <v>676</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>671</v>
+        <v>678</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="C178" s="11"/>
       <c r="D178" s="11"/>
       <c r="E178" s="8" t="s">
-        <v>672</v>
+        <v>679</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>673</v>
+        <v>680</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11"/>
       <c r="E179" s="8" t="s">
-        <v>674</v>
+        <v>681</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>675</v>
+        <v>682</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11" t="s">
-        <v>676</v>
+        <v>683</v>
       </c>
       <c r="E180" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="F180" s="8" t="s">
         <v>677</v>
-      </c>
-      <c r="F180" s="8" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>678</v>
+        <v>685</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>205</v>
@@ -5825,15 +5843,15 @@
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>679</v>
+        <v>686</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>680</v>
+        <v>687</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>208</v>
@@ -5841,49 +5859,49 @@
       <c r="C182" s="11"/>
       <c r="D182" s="11"/>
       <c r="E182" s="8" t="s">
-        <v>681</v>
+        <v>688</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>682</v>
+        <v>689</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>683</v>
+        <v>690</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>684</v>
+        <v>691</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="C184" s="11"/>
       <c r="D184" s="11" t="s">
-        <v>685</v>
+        <v>692</v>
       </c>
       <c r="E184" s="8" t="s">
-        <v>686</v>
+        <v>693</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>687</v>
+        <v>694</v>
       </c>
       <c r="B185" s="8" t="s">
         <v>205</v>
@@ -5891,15 +5909,15 @@
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>688</v>
+        <v>695</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>689</v>
+        <v>696</v>
       </c>
       <c r="B186" s="8" t="s">
         <v>208</v>
@@ -5907,90 +5925,90 @@
       <c r="C186" s="11"/>
       <c r="D186" s="11"/>
       <c r="E186" s="8" t="s">
-        <v>690</v>
+        <v>697</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>691</v>
+        <v>698</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>692</v>
+        <v>699</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>693</v>
+        <v>700</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>694</v>
+        <v>701</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>695</v>
+        <v>702</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="8" t="s">
-        <v>696</v>
+        <v>703</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="C190" s="9" t="n">
         <v>23</v>
       </c>
       <c r="E190" s="8" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
       <c r="F190" s="9" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>701</v>
+        <v>708</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>702</v>
+        <v>709</v>
       </c>
       <c r="C191" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D191" s="8"/>
       <c r="E191" s="8" t="s">
-        <v>703</v>
+        <v>710</v>
       </c>
       <c r="G191" s="4" t="s">
         <v>94</v>
@@ -5998,53 +6016,53 @@
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>704</v>
+        <v>711</v>
       </c>
       <c r="B192" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C192" s="11"/>
       <c r="D192" s="11" t="s">
-        <v>705</v>
+        <v>712</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>708</v>
+        <v>715</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>709</v>
+        <v>716</v>
       </c>
       <c r="C193" s="11"/>
       <c r="D193" s="11" t="s">
-        <v>710</v>
+        <v>717</v>
       </c>
       <c r="E193" s="8" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C194" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D194" s="8"/>
       <c r="E194" s="8" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="G194" s="4" t="s">
         <v>94</v>
@@ -6052,67 +6070,67 @@
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>713</v>
+        <v>720</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C195" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>714</v>
+        <v>721</v>
       </c>
       <c r="E195" s="8" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>715</v>
+        <v>722</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>716</v>
+        <v>723</v>
       </c>
       <c r="C196" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
       <c r="E196" s="8" t="s">
-        <v>718</v>
+        <v>725</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>719</v>
+        <v>726</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>721</v>
+        <v>728</v>
       </c>
       <c r="C197" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>722</v>
+        <v>729</v>
       </c>
       <c r="E197" s="8" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>724</v>
+        <v>731</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>205</v>
@@ -6120,15 +6138,15 @@
       <c r="C198" s="11"/>
       <c r="D198" s="11"/>
       <c r="E198" s="8" t="s">
-        <v>726</v>
+        <v>733</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>727</v>
+        <v>734</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>728</v>
+        <v>735</v>
       </c>
       <c r="B199" s="8" t="s">
         <v>208</v>
@@ -6136,33 +6154,33 @@
       <c r="C199" s="11"/>
       <c r="D199" s="11"/>
       <c r="E199" s="8" t="s">
-        <v>729</v>
+        <v>736</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>727</v>
+        <v>734</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C200" s="11"/>
       <c r="D200" s="11" t="s">
-        <v>731</v>
+        <v>738</v>
       </c>
       <c r="E200" s="8" t="s">
-        <v>732</v>
+        <v>739</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>727</v>
+        <v>734</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>733</v>
+        <v>740</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>150</v>
@@ -6174,43 +6192,43 @@
         <v>151</v>
       </c>
       <c r="E201" s="8" t="s">
-        <v>734</v>
+        <v>741</v>
       </c>
       <c r="F201" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>735</v>
+        <v>742</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>736</v>
+        <v>743</v>
       </c>
       <c r="C202" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D202" s="8"/>
       <c r="E202" s="8" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="G202" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>738</v>
+        <v>745</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>739</v>
+        <v>746</v>
       </c>
       <c r="C203" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D203" s="8"/>
       <c r="E203" s="8" t="s">
-        <v>740</v>
+        <v>747</v>
       </c>
       <c r="G203" s="4" t="s">
         <v>94</v>
@@ -6218,15 +6236,15 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>741</v>
+        <v>748</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C204" s="11"/>
       <c r="D204" s="11"/>
       <c r="E204" s="8" t="s">
-        <v>742</v>
+        <v>749</v>
       </c>
       <c r="F204" s="8"/>
       <c r="G204" s="4" t="s">
@@ -6235,107 +6253,107 @@
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>743</v>
+        <v>750</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>744</v>
+        <v>751</v>
       </c>
       <c r="C205" s="11"/>
       <c r="D205" s="11" t="s">
-        <v>745</v>
+        <v>752</v>
       </c>
       <c r="E205" s="8" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>747</v>
+        <v>754</v>
       </c>
     </row>
     <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>748</v>
+        <v>755</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>749</v>
+        <v>756</v>
       </c>
       <c r="C206" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D206" s="8"/>
       <c r="E206" s="8" t="s">
-        <v>750</v>
+        <v>757</v>
       </c>
       <c r="F206" s="8" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>752</v>
+        <v>759</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
       <c r="C207" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>753</v>
+        <v>760</v>
       </c>
       <c r="E207" s="8" t="s">
-        <v>754</v>
+        <v>761</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>755</v>
+        <v>762</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>756</v>
+        <v>763</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="C208" s="11" t="n">
         <v>8400</v>
       </c>
       <c r="D208" s="11" t="s">
-        <v>758</v>
+        <v>765</v>
       </c>
       <c r="E208" s="8" t="s">
-        <v>759</v>
+        <v>766</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>760</v>
+        <v>767</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>761</v>
+        <v>768</v>
       </c>
       <c r="B209" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E209" s="8" t="s">
-        <v>762</v>
+        <v>769</v>
       </c>
       <c r="F209" s="8" t="s">
-        <v>763</v>
+        <v>770</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>764</v>
+        <v>771</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C210" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D210" s="8"/>
       <c r="E210" s="8" t="s">
-        <v>765</v>
+        <v>772</v>
       </c>
       <c r="F210" s="8"/>
       <c r="G210" s="4" t="s">
@@ -6344,19 +6362,19 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C211" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="E211" s="8" t="s">
-        <v>767</v>
+        <v>774</v>
       </c>
       <c r="F211" s="8"/>
       <c r="G211" s="4" t="s">
@@ -6365,7 +6383,7 @@
     </row>
     <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="10" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
       <c r="B212" s="8" t="s">
         <v>16</v>
@@ -6373,25 +6391,25 @@
       <c r="C212" s="11"/>
       <c r="D212" s="11"/>
       <c r="E212" s="8" t="s">
-        <v>769</v>
+        <v>776</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="10" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="C213" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="8" t="s">
-        <v>772</v>
+        <v>779</v>
       </c>
       <c r="G213" s="4" t="s">
         <v>94</v>
@@ -6399,13 +6417,13 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
       <c r="B214" s="8" t="s">
         <v>205</v>
       </c>
       <c r="E214" s="8" t="s">
-        <v>774</v>
+        <v>781</v>
       </c>
       <c r="F214" s="8"/>
     </row>

</xml_diff>

<commit_message>
Add JtR format for nsldaps
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="784">
   <si>
     <t>Hash</t>
   </si>
@@ -1430,7 +1430,10 @@
     <t>nsldap</t>
   </si>
   <si>
-    <t>{SHA}uJ6qx+YUFzQbcQtyd2gpTQ5qJ3s=</t>
+    <t>{SHA}zTsOichpYtEkA2Gj50dM0twCn4c=</t>
+  </si>
+  <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/nsldap_fmt_plug.c</t>
   </si>
   <si>
     <t>Netscape LDAP SSHA</t>
@@ -1439,10 +1442,13 @@
     <t>^{SSHA}[a-z0-9\/+]{38}==$/i</t>
   </si>
   <si>
-    <t>ssha</t>
-  </si>
-  <si>
-    <t>{SSHA}LTVdoLa0oBVS6cFo++7TQ0165sDWsurD5h+KoQ==</t>
+    <t>nsldaps</t>
+  </si>
+  <si>
+    <t>{SSHA}hSuTO5/BAElWjcrs1rM82DKSuNk4djZMbHNJZg==</t>
+  </si>
+  <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/opencl_nsldaps_fmt_plug.c</t>
   </si>
   <si>
     <t>NTHash(FreeBSD Variant)</t>
@@ -2548,8 +2554,8 @@
   </sheetPr>
   <dimension ref="A1:G214"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A138" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F165" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4825,58 +4831,58 @@
       <c r="E124" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="G124" s="4" t="s">
-        <v>94</v>
+      <c r="F124" s="2" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C125" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="G125" s="4" t="s">
-        <v>94</v>
+        <v>476</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C126" s="11"/>
       <c r="D126" s="11"/>
       <c r="E126" s="8" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="F126" s="8" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C127" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E127" s="8" t="s">
         <v>379</v>
@@ -4887,27 +4893,27 @@
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B129" s="8" t="s">
         <v>131</v>
@@ -4917,33 +4923,33 @@
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="8" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C130" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>284</v>
@@ -4952,48 +4958,48 @@
         <v>122</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C132" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C133" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D133" s="12"/>
       <c r="E133" s="8" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="G133" s="4" t="s">
         <v>94</v>
@@ -5001,15 +5007,15 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C134" s="11"/>
       <c r="D134" s="11"/>
       <c r="E134" s="8" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="F134" s="8"/>
       <c r="G134" s="4" t="s">
@@ -5018,116 +5024,116 @@
     </row>
     <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E136" s="12" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="10" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C138" s="3"/>
       <c r="E138" s="8" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="8" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="8" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C141" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="10" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>323</v>
@@ -5136,30 +5142,30 @@
         <v>400</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="F142" s="8" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C143" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="F143" s="8"/>
       <c r="G143" s="4" t="s">
@@ -5168,137 +5174,137 @@
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C144" s="9" t="n">
         <v>2612</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="F144" s="8" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C145" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C149" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D149" s="8"/>
       <c r="E149" s="8" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C150" s="11"/>
       <c r="D150" s="11" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="E150" s="8" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>208</v>
@@ -5307,18 +5313,18 @@
         <v>6000</v>
       </c>
       <c r="D151" s="8" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>263</v>
@@ -5326,165 +5332,165 @@
       <c r="C152" s="11"/>
       <c r="D152" s="11"/>
       <c r="E152" s="8" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="8" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
       <c r="E156" s="8" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C157" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D157" s="8" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="E157" s="8" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C158" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B159" s="17" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C159" s="14" t="n">
         <v>10300</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C160" s="11"/>
       <c r="D160" s="11"/>
       <c r="E160" s="8" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C161" s="9" t="n">
         <v>8900</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="12" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="G161" s="4" t="s">
         <v>11</v>
@@ -5492,7 +5498,7 @@
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="10" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>208</v>
@@ -5501,39 +5507,39 @@
         <v>100</v>
       </c>
       <c r="D162" s="11" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="C163" s="11"/>
       <c r="D163" s="11" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="C164" s="8" t="n">
         <v>101</v>
@@ -5544,13 +5550,13 @@
       <c r="E164" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="G164" s="4" t="s">
-        <v>94</v>
+      <c r="F164" s="2" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B165" s="8" t="s">
         <v>284</v>
@@ -5558,7 +5564,7 @@
       <c r="C165" s="11"/>
       <c r="D165" s="11"/>
       <c r="E165" s="8" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="F165" s="8"/>
       <c r="G165" s="4" t="s">
@@ -5567,25 +5573,25 @@
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>287</v>
       </c>
       <c r="C166" s="11"/>
       <c r="D166" s="11" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="E166" s="8" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>263</v>
@@ -5594,248 +5600,248 @@
         <v>1400</v>
       </c>
       <c r="D167" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="F167" s="8" t="s">
         <v>639</v>
-      </c>
-      <c r="E167" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="F167" s="8" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C168" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C169" s="11"/>
       <c r="D169" s="11" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C170" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D170" s="8" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="C171" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B172" s="8" t="s">
         <v>287</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>263</v>
       </c>
       <c r="C173" s="11" t="s">
+        <v>664</v>
+      </c>
+      <c r="D173" s="11" t="s">
+        <v>665</v>
+      </c>
+      <c r="E173" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="F173" s="8" t="s">
         <v>662</v>
-      </c>
-      <c r="D173" s="11" t="s">
-        <v>663</v>
-      </c>
-      <c r="E173" s="8" t="s">
-        <v>664</v>
-      </c>
-      <c r="F173" s="8" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C174" s="11"/>
       <c r="D174" s="11"/>
       <c r="E174" s="8" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C175" s="11"/>
       <c r="D175" s="11" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="E175" s="8" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="C176" s="14" t="n">
         <v>10100</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="2" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="C177" s="11"/>
       <c r="D177" s="11"/>
       <c r="E177" s="8" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C178" s="11"/>
       <c r="D178" s="11"/>
       <c r="E178" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="F178" s="8" t="s">
         <v>679</v>
-      </c>
-      <c r="F178" s="8" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11"/>
       <c r="E179" s="8" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B180" s="8" t="s">
         <v>263</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="E180" s="8" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>205</v>
@@ -5843,15 +5849,15 @@
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>208</v>
@@ -5859,15 +5865,15 @@
       <c r="C182" s="11"/>
       <c r="D182" s="11"/>
       <c r="E182" s="8" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>287</v>
@@ -5875,33 +5881,33 @@
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C184" s="11"/>
       <c r="D184" s="11" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="E184" s="8" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B185" s="8" t="s">
         <v>205</v>
@@ -5909,15 +5915,15 @@
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B186" s="8" t="s">
         <v>208</v>
@@ -5925,15 +5931,15 @@
       <c r="C186" s="11"/>
       <c r="D186" s="11"/>
       <c r="E186" s="8" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B187" s="8" t="s">
         <v>287</v>
@@ -5941,15 +5947,15 @@
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B188" s="8" t="s">
         <v>263</v>
@@ -5957,58 +5963,58 @@
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="8" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C190" s="9" t="n">
         <v>23</v>
       </c>
       <c r="E190" s="8" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="F190" s="9" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="C191" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D191" s="8"/>
       <c r="E191" s="8" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="G191" s="4" t="s">
         <v>94</v>
@@ -6016,61 +6022,63 @@
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B192" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C192" s="11"/>
       <c r="D192" s="11" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C193" s="11"/>
       <c r="D193" s="11" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="E193" s="8" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C194" s="8" t="n">
         <v>111</v>
       </c>
-      <c r="D194" s="8"/>
+      <c r="D194" s="8" t="s">
+        <v>475</v>
+      </c>
       <c r="E194" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="G194" s="4" t="s">
-        <v>94</v>
+        <v>476</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="B195" s="8" t="s">
         <v>342</v>
@@ -6079,7 +6087,7 @@
         <v>1711</v>
       </c>
       <c r="D195" s="8" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>343</v>
@@ -6090,47 +6098,47 @@
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C196" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="E196" s="8" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C197" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="E197" s="8" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>205</v>
@@ -6138,15 +6146,15 @@
       <c r="C198" s="11"/>
       <c r="D198" s="11"/>
       <c r="E198" s="8" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B199" s="8" t="s">
         <v>208</v>
@@ -6154,33 +6162,33 @@
       <c r="C199" s="11"/>
       <c r="D199" s="11"/>
       <c r="E199" s="8" t="s">
+        <v>738</v>
+      </c>
+      <c r="F199" s="8" t="s">
         <v>736</v>
-      </c>
-      <c r="F199" s="8" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>284</v>
       </c>
       <c r="C200" s="11"/>
       <c r="D200" s="11" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="E200" s="8" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>150</v>
@@ -6192,7 +6200,7 @@
         <v>151</v>
       </c>
       <c r="E201" s="8" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="F201" s="8" t="s">
         <v>153</v>
@@ -6200,17 +6208,17 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="C202" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D202" s="8"/>
       <c r="E202" s="8" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="G202" s="4" t="s">
         <v>94</v>
@@ -6218,17 +6226,17 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="C203" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D203" s="8"/>
       <c r="E203" s="8" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="G203" s="4" t="s">
         <v>94</v>
@@ -6236,7 +6244,7 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B204" s="8" t="s">
         <v>263</v>
@@ -6244,7 +6252,7 @@
       <c r="C204" s="11"/>
       <c r="D204" s="11"/>
       <c r="E204" s="8" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="F204" s="8"/>
       <c r="G204" s="4" t="s">
@@ -6253,97 +6261,97 @@
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C205" s="11"/>
       <c r="D205" s="11" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="E205" s="8" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
     </row>
     <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C206" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D206" s="8"/>
       <c r="E206" s="8" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="F206" s="8" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C207" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="E207" s="8" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C208" s="11" t="n">
         <v>8400</v>
       </c>
       <c r="D208" s="11" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="E208" s="8" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="B209" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E209" s="8" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="F209" s="8" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="B210" s="8" t="s">
         <v>323</v>
@@ -6353,7 +6361,7 @@
       </c>
       <c r="D210" s="8"/>
       <c r="E210" s="8" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="F210" s="8"/>
       <c r="G210" s="4" t="s">
@@ -6362,19 +6370,19 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C211" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E211" s="8" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F211" s="8"/>
       <c r="G211" s="4" t="s">
@@ -6383,7 +6391,7 @@
     </row>
     <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="10" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B212" s="8" t="s">
         <v>16</v>
@@ -6391,25 +6399,25 @@
       <c r="C212" s="11"/>
       <c r="D212" s="11"/>
       <c r="E212" s="8" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="10" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C213" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="8" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="G213" s="4" t="s">
         <v>94</v>
@@ -6417,13 +6425,13 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B214" s="8" t="s">
         <v>205</v>
       </c>
       <c r="E214" s="8" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="F214" s="8"/>
     </row>

</xml_diff>

<commit_message>
Add Microsoft Outlook PST
Implemented using pass_gen.pl
(https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/run/pass_gen.pl)
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="793">
   <si>
     <t>Hash</t>
   </si>
@@ -1274,6 +1274,21 @@
     <t>$office$*2013*100000*256*16*7dd611d7eb4c899f74816d1dec817b3b*948dc0b2c2c6c32f14b5995a543ad037*0b7ee0e48e935f937192a59de48a7d561ef2691d5c8a3ba87ec2d04402a94895</t>
   </si>
   <si>
+    <t>Microsoft Outlook PST</t>
+  </si>
+  <si>
+    <t>^(\$pst\$)?[a-f0-9]{8}$/i</t>
+  </si>
+  <si>
+    <t>pst</t>
+  </si>
+  <si>
+    <t>$pst$815b338f</t>
+  </si>
+  <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/pst_fmt_plug.c</t>
+  </si>
+  <si>
     <t>Minecraft(AuthMe Reloaded)</t>
   </si>
   <si>
@@ -1859,7 +1874,7 @@
     <t>saph</t>
   </si>
   <si>
-    <t>{x-issha, 1024}C0624EvGSdAMCtuWnBBYBGA0chvqAflKY74oEpw/rpY=</t>
+    <t>{x-issha, 1024}4efI42lF15lGXwJkxNL94fndDzVnR1RRWjFOcXdZWk8=</t>
   </si>
   <si>
     <t>http://hashcat.net/forum/thread-3804.html</t>
@@ -2225,7 +2240,7 @@
     <t>sybasease</t>
   </si>
   <si>
-    <t>0xc00778168388631428230545ed2c976790af96768afa0806fe6c0da3b28f3e132137eac56f9bad027ea2</t>
+    <t>0xc0074f31384f5a464c760f312ec641098c248fdf57b8d3843be451e38ce37351c69edb25cdae6aab7da3</t>
   </si>
   <si>
     <t>http://marcellmajor.com/sybase_sha256.html</t>
@@ -2564,10 +2579,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G215"/>
+  <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B177" activeCellId="0" sqref="B177"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A178" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A190" activeCellId="0" sqref="A1:G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4581,51 +4596,48 @@
         <v>405</v>
       </c>
     </row>
-    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="10" t="s">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="8" t="s">
+      <c r="D111" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="F111" s="8" t="s">
+      <c r="E111" s="2" t="s">
         <v>422</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="C113" s="8" t="n">
-        <v>131</v>
-      </c>
-      <c r="D113" s="8" t="s">
         <v>429</v>
       </c>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
       <c r="E113" s="8" t="s">
         <v>430</v>
       </c>
@@ -4641,7 +4653,7 @@
         <v>433</v>
       </c>
       <c r="C114" s="8" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>434</v>
@@ -4653,42 +4665,42 @@
         <v>436</v>
       </c>
     </row>
-    <row r="115" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
         <v>437</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="C115" s="11" t="n">
+        <v>438</v>
+      </c>
+      <c r="C115" s="8" t="n">
         <v>132</v>
       </c>
-      <c r="D115" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="E115" s="8"/>
-      <c r="G115" s="4" t="s">
+      <c r="D115" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="116" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C116" s="11" t="n">
+        <v>132</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="E116" s="8"/>
+      <c r="G116" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="B116" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="C116" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E116" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4696,68 +4708,68 @@
         <v>443</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="C117" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C118" s="8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D118" s="8"/>
+        <v>1731</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>445</v>
+      </c>
       <c r="E118" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B119" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C119" s="8" t="n">
+        <v>2811</v>
+      </c>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="F119" s="8" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C119" s="8" t="n">
+      <c r="C120" s="8" t="n">
         <v>200</v>
-      </c>
-      <c r="D119" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="C120" s="8" t="n">
-        <v>300</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>456</v>
@@ -4770,81 +4782,81 @@
       </c>
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="10" t="s">
+      <c r="A121" s="15" t="s">
         <v>459</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="F121" s="8" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C122" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D122" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="B122" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="C122" s="8" t="n">
+      <c r="E122" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="F122" s="8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="C123" s="8" t="n">
         <v>5500</v>
       </c>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="G122" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="123" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="10" t="s">
-        <v>464</v>
-      </c>
-      <c r="B123" s="8" t="s">
-        <v>465</v>
-      </c>
-      <c r="C123" s="8" t="n">
-        <v>5600</v>
-      </c>
-      <c r="D123" s="12" t="s">
-        <v>466</v>
-      </c>
+      <c r="D123" s="8"/>
       <c r="E123" s="8" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C124" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D124" s="8" t="s">
-        <v>470</v>
+        <v>5600</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>471</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="F124" s="2" t="s">
         <v>472</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4855,7 +4867,7 @@
         <v>474</v>
       </c>
       <c r="C125" s="8" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>475</v>
@@ -4874,53 +4886,53 @@
       <c r="B126" s="8" t="s">
         <v>479</v>
       </c>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
+      <c r="C126" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>480</v>
+      </c>
       <c r="E126" s="8" t="s">
-        <v>480</v>
-      </c>
-      <c r="F126" s="8" t="s">
         <v>481</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>483</v>
-      </c>
-      <c r="C127" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D127" s="8" t="s">
         <v>484</v>
       </c>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
       <c r="E127" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="G127" s="4" t="s">
-        <v>94</v>
+        <v>485</v>
+      </c>
+      <c r="F127" s="8" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C128" s="8" t="n">
-        <v>112</v>
+        <v>1000</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="F128" s="8" t="s">
-        <v>489</v>
+        <v>379</v>
+      </c>
+      <c r="G128" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4928,68 +4940,68 @@
         <v>490</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>131</v>
+        <v>491</v>
       </c>
       <c r="C129" s="8" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D129" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>492</v>
+      </c>
       <c r="E129" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>494</v>
+        <v>131</v>
       </c>
       <c r="C130" s="8" t="n">
-        <v>21</v>
+        <v>3100</v>
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B131" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="C131" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="D131" s="8"/>
+      <c r="E131" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="F131" s="8" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="B132" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C131" s="8" t="n">
+      <c r="C132" s="8" t="n">
         <v>122</v>
       </c>
-      <c r="D131" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="E131" s="8" t="s">
-        <v>499</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="132" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="C132" s="8" t="n">
-        <v>1722</v>
-      </c>
-      <c r="D132" s="12" t="s">
+      <c r="D132" s="8" t="s">
         <v>503</v>
       </c>
       <c r="E132" s="8" t="s">
@@ -4999,7 +5011,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
         <v>506</v>
       </c>
@@ -5007,55 +5019,58 @@
         <v>507</v>
       </c>
       <c r="C133" s="8" t="n">
+        <v>1722</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="C134" s="8" t="n">
         <v>7100</v>
       </c>
-      <c r="D133" s="12"/>
-      <c r="E133" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="G133" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="10" t="s">
-        <v>509</v>
-      </c>
-      <c r="B134" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="C134" s="11"/>
-      <c r="D134" s="11"/>
+      <c r="D134" s="12"/>
       <c r="E134" s="8" t="s">
-        <v>511</v>
-      </c>
-      <c r="F134" s="8"/>
+        <v>513</v>
+      </c>
       <c r="G134" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="E135" s="2" t="s">
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="F135" s="8" t="s">
+      <c r="B135" s="8" t="s">
         <v>515</v>
+      </c>
+      <c r="C135" s="11"/>
+      <c r="D135" s="11"/>
+      <c r="E135" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="F135" s="8"/>
+      <c r="G135" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="D136" s="3" t="s">
         <v>518</v>
       </c>
       <c r="E136" s="2" t="s">
@@ -5072,155 +5087,152 @@
       <c r="B137" s="2" t="s">
         <v>522</v>
       </c>
+      <c r="D137" s="3" t="s">
+        <v>523</v>
+      </c>
       <c r="E137" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="B138" s="8" t="s">
+      <c r="A138" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="C138" s="3"/>
-      <c r="E138" s="8" t="s">
+      <c r="B138" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="F138" s="9" t="s">
+      <c r="E138" s="2" t="s">
         <v>528</v>
+      </c>
+      <c r="F138" s="8" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="C139" s="11"/>
-      <c r="D139" s="11"/>
+        <v>531</v>
+      </c>
+      <c r="C139" s="3"/>
       <c r="E139" s="8" t="s">
-        <v>531</v>
-      </c>
-      <c r="F139" s="8" t="s">
         <v>532</v>
+      </c>
+      <c r="F139" s="9" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="8" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
-        <v>537</v>
+      <c r="A141" s="10" t="s">
+        <v>538</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="C141" s="9" t="n">
+        <v>539</v>
+      </c>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
+      <c r="E141" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="F141" s="8" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="C142" s="9" t="n">
         <v>133</v>
       </c>
-      <c r="E141" s="8" t="s">
-        <v>539</v>
-      </c>
-      <c r="F141" s="9" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="10" t="s">
-        <v>541</v>
-      </c>
-      <c r="B142" s="8" t="s">
+      <c r="E142" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="F142" s="9" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="B143" s="8" t="s">
         <v>323</v>
-      </c>
-      <c r="C142" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D142" s="8" t="s">
-        <v>542</v>
-      </c>
-      <c r="E142" s="8" t="s">
-        <v>543</v>
-      </c>
-      <c r="F142" s="8" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="B143" s="8" t="s">
-        <v>546</v>
       </c>
       <c r="C143" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="E143" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="F143" s="8" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="C144" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D144" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="F143" s="8"/>
-      <c r="G143" s="4" t="s">
+      <c r="E144" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="F144" s="8"/>
+      <c r="G144" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="B144" s="8" t="s">
-        <v>549</v>
-      </c>
-      <c r="C144" s="9" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D144" s="9" t="s">
-        <v>550</v>
-      </c>
-      <c r="E144" s="8" t="s">
-        <v>551</v>
-      </c>
-      <c r="F144" s="8" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="C145" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D145" s="3" t="s">
+      <c r="C145" s="9" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D145" s="9" t="s">
         <v>555</v>
       </c>
-      <c r="E145" s="2" t="s">
+      <c r="E145" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="F145" s="2" t="s">
+      <c r="F145" s="8" t="s">
         <v>557</v>
       </c>
     </row>
@@ -5228,205 +5240,205 @@
       <c r="A146" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="B146" s="8" t="s">
+      <c r="B146" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="E146" s="8" t="s">
+      <c r="C146" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D146" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="F146" s="9" t="s">
+      <c r="E146" s="2" t="s">
         <v>561</v>
       </c>
+      <c r="F146" s="2" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="10" t="s">
-        <v>562</v>
+      <c r="A147" s="1" t="s">
+        <v>563</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>563</v>
-      </c>
-      <c r="C147" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="D147" s="8" t="s">
+      <c r="E147" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="E147" s="8" t="s">
+      <c r="F147" s="9" t="s">
         <v>566</v>
-      </c>
-      <c r="F147" s="8" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="B148" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="B148" s="8" t="s">
+      <c r="C148" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="C148" s="11" t="s">
+      <c r="D148" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="D148" s="11" t="s">
+      <c r="E148" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="E148" s="8" t="s">
+      <c r="F148" s="8" t="s">
         <v>572</v>
-      </c>
-      <c r="F148" s="8" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="B149" s="8" t="s">
         <v>574</v>
       </c>
-      <c r="B149" s="8" t="s">
+      <c r="C149" s="11" t="s">
         <v>575</v>
       </c>
-      <c r="C149" s="8" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D149" s="8"/>
+      <c r="D149" s="11" t="s">
+        <v>576</v>
+      </c>
       <c r="E149" s="8" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C150" s="11"/>
-      <c r="D150" s="11" t="s">
-        <v>579</v>
-      </c>
+        <v>580</v>
+      </c>
+      <c r="C150" s="8" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D150" s="8"/>
       <c r="E150" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C151" s="8" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D151" s="8" t="s">
-        <v>583</v>
+        <v>205</v>
+      </c>
+      <c r="C151" s="11"/>
+      <c r="D151" s="11" t="s">
+        <v>584</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="C152" s="11"/>
-      <c r="D152" s="11"/>
+        <v>208</v>
+      </c>
+      <c r="C152" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>588</v>
+      </c>
       <c r="E152" s="8" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>581</v>
+        <v>590</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>589</v>
+        <v>263</v>
       </c>
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="8" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
       <c r="E156" s="8" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>603</v>
-      </c>
-      <c r="C157" s="8" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D157" s="8" t="s">
         <v>604</v>
       </c>
+      <c r="C157" s="11"/>
+      <c r="D157" s="11"/>
       <c r="E157" s="8" t="s">
         <v>605</v>
       </c>
@@ -5442,7 +5454,7 @@
         <v>608</v>
       </c>
       <c r="C158" s="8" t="n">
-        <v>7800</v>
+        <v>7700</v>
       </c>
       <c r="D158" s="8" t="s">
         <v>609</v>
@@ -5451,90 +5463,92 @@
         <v>610</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="159" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="B159" s="17" t="s">
+    </row>
+    <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="10" t="s">
         <v>612</v>
       </c>
-      <c r="C159" s="14" t="n">
+      <c r="B159" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="C159" s="8" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="F159" s="8" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="160" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B160" s="17" t="s">
+        <v>617</v>
+      </c>
+      <c r="C160" s="14" t="n">
         <v>10300</v>
       </c>
-      <c r="D159" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="B160" s="8" t="s">
-        <v>617</v>
-      </c>
-      <c r="C160" s="11"/>
-      <c r="D160" s="11"/>
-      <c r="E160" s="8" t="s">
+      <c r="D160" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="F160" s="8" t="s">
+      <c r="E160" s="2" t="s">
         <v>619</v>
       </c>
+      <c r="F160" s="2" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="s">
-        <v>620</v>
+      <c r="A161" s="10" t="s">
+        <v>621</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>621</v>
-      </c>
-      <c r="C161" s="9" t="n">
+        <v>622</v>
+      </c>
+      <c r="C161" s="11"/>
+      <c r="D161" s="11"/>
+      <c r="E161" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="F161" s="8" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="C162" s="9" t="n">
         <v>8900</v>
       </c>
-      <c r="E161" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="G161" s="4" t="s">
+      <c r="E162" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="G162" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="10" t="s">
-        <v>623</v>
-      </c>
-      <c r="B162" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C162" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="D162" s="11" t="s">
-        <v>624</v>
-      </c>
-      <c r="E162" s="8" t="s">
-        <v>625</v>
-      </c>
-      <c r="F162" s="8" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>628</v>
-      </c>
-      <c r="C163" s="11"/>
+        <v>208</v>
+      </c>
+      <c r="C163" s="11" t="n">
+        <v>100</v>
+      </c>
       <c r="D163" s="11" t="s">
         <v>629</v>
       </c>
@@ -5545,157 +5559,155 @@
         <v>631</v>
       </c>
     </row>
-    <row r="164" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
         <v>632</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="C164" s="8" t="n">
+        <v>633</v>
+      </c>
+      <c r="C164" s="11"/>
+      <c r="D164" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="E164" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="F164" s="8" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="165" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="C165" s="8" t="n">
         <v>101</v>
       </c>
-      <c r="D164" s="12" t="s">
-        <v>470</v>
-      </c>
-      <c r="E164" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="F164" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="10" t="s">
-        <v>633</v>
-      </c>
-      <c r="B165" s="8" t="s">
+      <c r="D165" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="E165" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="10" t="s">
+        <v>638</v>
+      </c>
+      <c r="B166" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C165" s="11"/>
-      <c r="D165" s="11"/>
-      <c r="E165" s="8" t="s">
-        <v>634</v>
-      </c>
-      <c r="F165" s="8"/>
-      <c r="G165" s="4" t="s">
+      <c r="C166" s="11"/>
+      <c r="D166" s="11"/>
+      <c r="E166" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="F166" s="8"/>
+      <c r="G166" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="10" t="s">
-        <v>635</v>
-      </c>
-      <c r="B166" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="C166" s="11"/>
-      <c r="D166" s="11" t="s">
-        <v>636</v>
-      </c>
-      <c r="E166" s="8" t="s">
-        <v>637</v>
-      </c>
-      <c r="F166" s="8" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B167" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C167" s="11"/>
+      <c r="D167" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="F167" s="8" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="10" t="s">
+        <v>644</v>
+      </c>
+      <c r="B168" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="C167" s="8" t="n">
+      <c r="C168" s="8" t="n">
         <v>1400</v>
       </c>
-      <c r="D167" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="E167" s="8" t="s">
-        <v>641</v>
-      </c>
-      <c r="F167" s="8" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="B168" s="8" t="s">
+      <c r="D168" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="E168" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="F168" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="C168" s="8" t="n">
-        <v>7400</v>
-      </c>
-      <c r="D168" s="8" t="s">
-        <v>644</v>
-      </c>
-      <c r="E168" s="8" t="s">
-        <v>645</v>
-      </c>
-      <c r="F168" s="8" t="s">
-        <v>646</v>
-      </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="10" t="s">
+      <c r="A169" s="1" t="s">
         <v>647</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="C169" s="11"/>
-      <c r="D169" s="11" t="s">
+      <c r="C169" s="8" t="n">
+        <v>7400</v>
+      </c>
+      <c r="D169" s="8" t="s">
         <v>649</v>
       </c>
       <c r="E169" s="8" t="s">
         <v>650</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>638</v>
+        <v>651</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>592</v>
-      </c>
-      <c r="C170" s="8" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D170" s="8" t="s">
-        <v>652</v>
+        <v>653</v>
+      </c>
+      <c r="C170" s="11"/>
+      <c r="D170" s="11" t="s">
+        <v>654</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>655</v>
+        <v>597</v>
       </c>
       <c r="C171" s="8" t="n">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5703,374 +5715,376 @@
         <v>659</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>287</v>
+        <v>660</v>
+      </c>
+      <c r="C172" s="8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D172" s="8" t="s">
+        <v>661</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="C173" s="11" t="s">
-        <v>663</v>
-      </c>
-      <c r="D173" s="11" t="s">
-        <v>664</v>
+        <v>287</v>
       </c>
       <c r="E173" s="8" t="s">
         <v>665</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C174" s="11" t="s">
+        <v>668</v>
+      </c>
+      <c r="D174" s="11" t="s">
+        <v>669</v>
+      </c>
+      <c r="E174" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="F174" s="8" t="s">
         <v>666</v>
-      </c>
-      <c r="B174" s="8" t="s">
-        <v>648</v>
-      </c>
-      <c r="C174" s="11"/>
-      <c r="D174" s="11"/>
-      <c r="E174" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="F174" s="8" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>592</v>
+        <v>653</v>
       </c>
       <c r="C175" s="11"/>
-      <c r="D175" s="11" t="s">
-        <v>669</v>
-      </c>
+      <c r="D175" s="11"/>
       <c r="E175" s="8" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="D176" s="3" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="10" t="s">
         <v>673</v>
       </c>
-      <c r="E176" s="2" t="s">
+      <c r="B176" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="C176" s="11"/>
+      <c r="D176" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="F176" s="2" t="s">
+      <c r="E176" s="8" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="177" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F176" s="8" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
         <v>676</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="C177" s="14" t="n">
+      <c r="D177" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="178" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C178" s="14" t="n">
         <v>10100</v>
       </c>
-      <c r="E177" s="2" t="s">
-        <v>678</v>
-      </c>
-      <c r="F177" s="2" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="10" t="s">
-        <v>680</v>
-      </c>
-      <c r="B178" s="8" t="s">
-        <v>681</v>
-      </c>
-      <c r="C178" s="11"/>
-      <c r="D178" s="11"/>
-      <c r="E178" s="8" t="s">
-        <v>682</v>
-      </c>
-      <c r="F178" s="8" t="s">
+      <c r="E178" s="2" t="s">
         <v>683</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>648</v>
+        <v>686</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11"/>
       <c r="E179" s="8" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>592</v>
+        <v>653</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="C181" s="11"/>
+      <c r="D181" s="11"/>
+      <c r="E181" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="F181" s="8" t="s">
         <v>688</v>
-      </c>
-      <c r="B181" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="C181" s="11"/>
-      <c r="D181" s="11" t="s">
-        <v>689</v>
-      </c>
-      <c r="E181" s="8" t="s">
-        <v>690</v>
-      </c>
-      <c r="F181" s="8" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>205</v>
+        <v>263</v>
       </c>
       <c r="C182" s="11"/>
-      <c r="D182" s="11"/>
+      <c r="D182" s="11" t="s">
+        <v>694</v>
+      </c>
       <c r="E182" s="8" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>287</v>
+        <v>208</v>
       </c>
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>592</v>
+        <v>287</v>
       </c>
       <c r="C185" s="11"/>
-      <c r="D185" s="11" t="s">
-        <v>698</v>
-      </c>
+      <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>205</v>
+        <v>597</v>
       </c>
       <c r="C186" s="11"/>
-      <c r="D186" s="11"/>
+      <c r="D186" s="11" t="s">
+        <v>703</v>
+      </c>
       <c r="E186" s="8" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>287</v>
+        <v>208</v>
       </c>
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="8" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>648</v>
+        <v>263</v>
       </c>
       <c r="C190" s="11"/>
       <c r="D190" s="11"/>
       <c r="E190" s="8" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="1" t="s">
-        <v>710</v>
+      <c r="A191" s="10" t="s">
+        <v>713</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>711</v>
-      </c>
-      <c r="C191" s="9" t="n">
+        <v>653</v>
+      </c>
+      <c r="C191" s="11"/>
+      <c r="D191" s="11"/>
+      <c r="E191" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="F191" s="8" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="C192" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="E191" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="F191" s="9" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="10" t="s">
-        <v>714</v>
-      </c>
-      <c r="B192" s="8" t="s">
-        <v>715</v>
-      </c>
-      <c r="C192" s="8" t="n">
-        <v>121</v>
-      </c>
-      <c r="D192" s="8"/>
       <c r="E192" s="8" t="s">
-        <v>716</v>
-      </c>
-      <c r="G192" s="4" t="s">
-        <v>94</v>
+        <v>717</v>
+      </c>
+      <c r="F192" s="9" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C193" s="11"/>
-      <c r="D193" s="11" t="s">
-        <v>718</v>
-      </c>
+        <v>720</v>
+      </c>
+      <c r="C193" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>719</v>
-      </c>
-      <c r="F193" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
+      </c>
+      <c r="G193" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>722</v>
+        <v>205</v>
       </c>
       <c r="C194" s="11"/>
       <c r="D194" s="11" t="s">
@@ -6080,78 +6094,76 @@
         <v>724</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
+        <v>726</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="C195" s="11"/>
+      <c r="D195" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>729</v>
+      </c>
+      <c r="F195" s="8" t="s">
         <v>725</v>
-      </c>
-      <c r="B195" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="C195" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D195" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="E195" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="F195" s="2" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
-        <v>726</v>
+        <v>730</v>
       </c>
       <c r="B196" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="C196" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D196" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="E196" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="B197" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="C196" s="8" t="n">
+      <c r="C197" s="8" t="n">
         <v>1711</v>
       </c>
-      <c r="D196" s="8" t="s">
-        <v>727</v>
-      </c>
-      <c r="E196" s="8" t="s">
+      <c r="D197" s="8" t="s">
+        <v>732</v>
+      </c>
+      <c r="E197" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="F196" s="8" t="s">
+      <c r="F197" s="8" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="B197" s="8" t="s">
-        <v>729</v>
-      </c>
-      <c r="C197" s="8" t="n">
-        <v>3300</v>
-      </c>
-      <c r="D197" s="8" t="s">
-        <v>730</v>
-      </c>
-      <c r="E197" s="8" t="s">
-        <v>731</v>
-      </c>
-      <c r="F197" s="8" t="s">
-        <v>732</v>
-      </c>
-    </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="10" t="s">
+      <c r="A198" s="1" t="s">
         <v>733</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>734</v>
       </c>
       <c r="C198" s="8" t="n">
-        <v>8000</v>
+        <v>3300</v>
       </c>
       <c r="D198" s="8" t="s">
         <v>735</v>
@@ -6168,140 +6180,142 @@
         <v>738</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C199" s="11"/>
-      <c r="D199" s="11"/>
+        <v>739</v>
+      </c>
+      <c r="C199" s="8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D199" s="8" t="s">
+        <v>740</v>
+      </c>
       <c r="E199" s="8" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C200" s="11"/>
       <c r="D200" s="11"/>
       <c r="E200" s="8" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="B201" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C201" s="11"/>
+      <c r="D201" s="11"/>
+      <c r="E201" s="8" t="s">
+        <v>747</v>
+      </c>
+      <c r="F201" s="8" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="10" t="s">
+        <v>748</v>
+      </c>
+      <c r="B202" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="C201" s="11"/>
-      <c r="D201" s="11" t="s">
-        <v>744</v>
-      </c>
-      <c r="E201" s="8" t="s">
+      <c r="C202" s="11"/>
+      <c r="D202" s="11" t="s">
+        <v>749</v>
+      </c>
+      <c r="E202" s="8" t="s">
+        <v>750</v>
+      </c>
+      <c r="F202" s="8" t="s">
         <v>745</v>
       </c>
-      <c r="F201" s="8" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="202" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="10" t="s">
-        <v>746</v>
-      </c>
-      <c r="B202" s="8" t="s">
+    </row>
+    <row r="203" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="10" t="s">
+        <v>751</v>
+      </c>
+      <c r="B203" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C202" s="8" t="n">
+      <c r="C203" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="D202" s="12" t="s">
+      <c r="D203" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="E202" s="8" t="s">
-        <v>747</v>
-      </c>
-      <c r="F202" s="8" t="s">
+      <c r="E203" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="F203" s="8" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="10" t="s">
-        <v>748</v>
-      </c>
-      <c r="B203" s="8" t="s">
-        <v>749</v>
-      </c>
-      <c r="C203" s="8" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D203" s="8"/>
-      <c r="E203" s="8" t="s">
-        <v>750</v>
-      </c>
-      <c r="G203" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="C204" s="8" t="n">
-        <v>2711</v>
+        <v>2611</v>
       </c>
       <c r="D204" s="8"/>
       <c r="E204" s="8" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="G204" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="C205" s="11"/>
-      <c r="D205" s="11"/>
+        <v>757</v>
+      </c>
+      <c r="C205" s="8" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
-        <v>755</v>
-      </c>
-      <c r="F205" s="8"/>
+        <v>758</v>
+      </c>
       <c r="G205" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>757</v>
+        <v>263</v>
       </c>
       <c r="C206" s="11"/>
-      <c r="D206" s="11" t="s">
-        <v>758</v>
-      </c>
+      <c r="D206" s="11"/>
       <c r="E206" s="8" t="s">
-        <v>759</v>
-      </c>
-      <c r="F206" s="8" t="s">
         <v>760</v>
+      </c>
+      <c r="F206" s="8"/>
+      <c r="G206" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6311,48 +6325,46 @@
       <c r="B207" s="8" t="s">
         <v>762</v>
       </c>
-      <c r="C207" s="8" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D207" s="8"/>
+      <c r="C207" s="11"/>
+      <c r="D207" s="11" t="s">
+        <v>763</v>
+      </c>
       <c r="E207" s="8" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>592</v>
+        <v>767</v>
       </c>
       <c r="C208" s="8" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D208" s="8" t="s">
-        <v>766</v>
-      </c>
+        <v>3721</v>
+      </c>
+      <c r="D208" s="8"/>
       <c r="E208" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>770</v>
-      </c>
-      <c r="C209" s="11" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D209" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="C209" s="8" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D209" s="8" t="s">
         <v>771</v>
       </c>
       <c r="E209" s="8" t="s">
@@ -6367,100 +6379,120 @@
         <v>774</v>
       </c>
       <c r="B210" s="8" t="s">
+        <v>775</v>
+      </c>
+      <c r="C210" s="11" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D210" s="11" t="s">
+        <v>776</v>
+      </c>
+      <c r="E210" s="8" t="s">
+        <v>777</v>
+      </c>
+      <c r="F210" s="8" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="B211" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E210" s="8" t="s">
-        <v>775</v>
-      </c>
-      <c r="F210" s="8" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="B211" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C211" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D211" s="8"/>
       <c r="E211" s="8" t="s">
-        <v>778</v>
-      </c>
-      <c r="F211" s="8"/>
-      <c r="G211" s="4" t="s">
-        <v>94</v>
+        <v>780</v>
+      </c>
+      <c r="F211" s="8" t="s">
+        <v>781</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>546</v>
+        <v>323</v>
       </c>
       <c r="C212" s="8" t="n">
         <v>400</v>
       </c>
-      <c r="D212" s="8" t="s">
-        <v>542</v>
-      </c>
+      <c r="D212" s="8"/>
       <c r="E212" s="8" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="F212" s="8"/>
       <c r="G212" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="10" t="s">
-        <v>781</v>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>784</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C213" s="11"/>
-      <c r="D213" s="11"/>
+        <v>551</v>
+      </c>
+      <c r="C213" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D213" s="8" t="s">
+        <v>547</v>
+      </c>
       <c r="E213" s="8" t="s">
-        <v>782</v>
-      </c>
-      <c r="F213" s="8" t="s">
-        <v>783</v>
+        <v>785</v>
+      </c>
+      <c r="F213" s="8"/>
+      <c r="G213" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="10" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>494</v>
-      </c>
-      <c r="C214" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="C214" s="11"/>
+      <c r="D214" s="11"/>
+      <c r="E214" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="F214" s="8" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="10" t="s">
+        <v>789</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="C215" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="D214" s="8"/>
-      <c r="E214" s="8" t="s">
-        <v>785</v>
-      </c>
-      <c r="G214" s="4" t="s">
+      <c r="D215" s="8"/>
+      <c r="E215" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="G215" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="1" t="s">
-        <v>786</v>
-      </c>
-      <c r="B215" s="8" t="s">
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="B216" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E215" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="F215" s="8"/>
+      <c r="E216" s="8" t="s">
+        <v>792</v>
+      </c>
+      <c r="F216" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fix JtR format for MD2
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -1139,7 +1139,7 @@
     <t>^(\$md2\$)?[a-f0-9]{32}$/i</t>
   </si>
   <si>
-    <t>rawmd2</t>
+    <t>md2</t>
   </si>
   <si>
     <t>fcdcaaa9794d753db7da35230ef5dd7a</t>
@@ -2581,8 +2581,8 @@
   </sheetPr>
   <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E87" activeCellId="0" sqref="E87"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B98" activeCellId="0" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Fixed DCC & DCC 2 regex
Fixed Domain Cached Credentials & Domain Cached Credentials 2
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -602,7 +602,7 @@
     <t>Domain Cached Credentials</t>
   </si>
   <si>
-    <t>^[a-f0-9]{32}(:[^\\\/:*?"&lt;&gt;|]{1,20})?$/i</t>
+    <t>^([^\\\/:*?"&lt;&gt;|]{1,20}:)?[a-f0-9]{32}(:[^\\\/:*?"&lt;&gt;|]{1,20})?$/i</t>
   </si>
   <si>
     <t>mscach</t>
@@ -617,7 +617,7 @@
     <t>Domain Cached Credentials v2</t>
   </si>
   <si>
-    <t>^(\$DCC2\$10240#[^\\\/:*?"&lt;&gt;|]{1,20}#)?[a-f0-9]{32}$/i</t>
+    <t>^([^\\\/:*?"&lt;&gt;|]{1,20}:)?(\$DCC2\$10240#[^\\\/:*?"&lt;&gt;|]{1,20}#)?[a-f0-9]{32}$/i</t>
   </si>
   <si>
     <t>mscach2</t>
@@ -2584,8 +2584,8 @@
   </sheetPr>
   <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A177" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B194" activeCellId="0" sqref="B194"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Fixed NetNTLMv1-VANILLA / NetNTLMv1+ESS regex
..and added JtR format
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="795">
   <si>
     <t>Hash</t>
   </si>
@@ -1418,7 +1418,10 @@
     <t>NetNTLMv1-VANILLA / NetNTLMv1+ESS</t>
   </si>
   <si>
-    <t>^[^\\\/:*?"&lt;&gt;|]{1,20}::[^\\\/:*?"&lt;&gt;|]{1,20}:[a-f0-9]{48}:[a-f0-9]{48}:[a-f0-9]{16}$/i</t>
+    <t>^[^\\\/:*?"&lt;&gt;|]{1,20}[:]{2,3}([^\\\/:*?"&lt;&gt;|]{1,20})?:[a-f0-9]{48}:[a-f0-9]{48}:[a-f0-9]{16}$/i</t>
+  </si>
+  <si>
+    <t>netntlm</t>
   </si>
   <si>
     <t>u4-netntlm::kNS:338d08f8e26de93300000000000000000000000000000000:9526fb8c23a90751cdd619b6cea564742e1e4bf33006ba41:cb8086049ec4736c</t>
@@ -2584,8 +2587,8 @@
   </sheetPr>
   <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C123" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4834,29 +4837,31 @@
       <c r="C123" s="8" t="n">
         <v>5500</v>
       </c>
-      <c r="D123" s="8"/>
+      <c r="D123" s="8" t="s">
+        <v>468</v>
+      </c>
       <c r="E123" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>11</v>
@@ -4864,72 +4869,72 @@
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C125" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C126" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C127" s="11"/>
       <c r="D127" s="11"/>
       <c r="E127" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E128" s="8" t="s">
         <v>379</v>
@@ -4940,27 +4945,27 @@
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C129" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>131</v>
@@ -4970,33 +4975,33 @@
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C131" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D131" s="8"/>
       <c r="E131" s="8" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F131" s="8" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>284</v>
@@ -5005,48 +5010,48 @@
         <v>122</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C133" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C134" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D134" s="12"/>
       <c r="E134" s="8" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G134" s="4" t="s">
         <v>94</v>
@@ -5054,15 +5059,15 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="8" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="F135" s="8"/>
       <c r="G135" s="4" t="s">
@@ -5071,116 +5076,116 @@
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C139" s="3"/>
       <c r="E139" s="8" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="8" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C141" s="11"/>
       <c r="D141" s="11"/>
       <c r="E141" s="8" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C142" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>323</v>
@@ -5189,30 +5194,30 @@
         <v>400</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F143" s="8" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C144" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F144" s="8"/>
       <c r="G144" s="4" t="s">
@@ -5221,137 +5226,137 @@
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C145" s="9" t="n">
         <v>2612</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C146" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D149" s="11" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E149" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C150" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D150" s="8"/>
       <c r="E150" s="8" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C151" s="11"/>
       <c r="D151" s="11" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>208</v>
@@ -5360,18 +5365,18 @@
         <v>6000</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E152" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>263</v>
@@ -5379,164 +5384,164 @@
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
       <c r="E156" s="8" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C157" s="11"/>
       <c r="D157" s="11"/>
       <c r="E157" s="8" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C158" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C159" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B160" s="17" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C160" s="14" t="n">
         <v>10300</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C161" s="11"/>
       <c r="D161" s="11"/>
       <c r="E161" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C162" s="9" t="n">
         <v>8900</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="G162" s="4" t="s">
         <v>11</v>
@@ -5544,7 +5549,7 @@
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B163" s="8" t="s">
         <v>208</v>
@@ -5553,56 +5558,56 @@
         <v>100</v>
       </c>
       <c r="D163" s="11" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C164" s="11"/>
       <c r="D164" s="11" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E164" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C165" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E165" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>284</v>
@@ -5610,7 +5615,7 @@
       <c r="C166" s="11"/>
       <c r="D166" s="11"/>
       <c r="E166" s="8" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F166" s="8"/>
       <c r="G166" s="4" t="s">
@@ -5619,25 +5624,25 @@
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>287</v>
       </c>
       <c r="C167" s="11"/>
       <c r="D167" s="11" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E167" s="8" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="10" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>263</v>
@@ -5646,264 +5651,264 @@
         <v>1400</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E168" s="8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C169" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C170" s="11"/>
       <c r="D170" s="11" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C171" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C172" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>287</v>
       </c>
       <c r="E173" s="8" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B174" s="8" t="s">
         <v>263</v>
       </c>
       <c r="C174" s="11" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D174" s="11" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E174" s="8" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C175" s="11"/>
       <c r="D175" s="11"/>
       <c r="E175" s="8" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C176" s="11"/>
       <c r="D176" s="11" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E176" s="8" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C178" s="14" t="n">
         <v>10100</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11"/>
       <c r="E179" s="8" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>263</v>
       </c>
       <c r="C182" s="11"/>
       <c r="D182" s="11" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E182" s="8" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>205</v>
@@ -5911,15 +5916,15 @@
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B184" s="8" t="s">
         <v>208</v>
@@ -5927,15 +5932,15 @@
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B185" s="8" t="s">
         <v>287</v>
@@ -5943,33 +5948,33 @@
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C186" s="11"/>
       <c r="D186" s="11" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="E186" s="8" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B187" s="8" t="s">
         <v>205</v>
@@ -5977,15 +5982,15 @@
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B188" s="8" t="s">
         <v>208</v>
@@ -5993,15 +5998,15 @@
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B189" s="8" t="s">
         <v>287</v>
@@ -6009,15 +6014,15 @@
       <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B190" s="8" t="s">
         <v>263</v>
@@ -6025,58 +6030,58 @@
       <c r="C190" s="11"/>
       <c r="D190" s="11"/>
       <c r="E190" s="8" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C191" s="11"/>
       <c r="D191" s="11"/>
       <c r="E191" s="8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C192" s="9" t="n">
         <v>23</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="F192" s="9" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C193" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="G193" s="4" t="s">
         <v>94</v>
@@ -6084,63 +6089,63 @@
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C194" s="11"/>
       <c r="D194" s="11" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="E194" s="8" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C195" s="11"/>
       <c r="D195" s="11" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="E195" s="8" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C196" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E196" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B197" s="8" t="s">
         <v>342</v>
@@ -6149,7 +6154,7 @@
         <v>1711</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>343</v>
@@ -6160,47 +6165,47 @@
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C198" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="E198" s="8" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C199" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="E199" s="8" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>205</v>
@@ -6208,15 +6213,15 @@
       <c r="C200" s="11"/>
       <c r="D200" s="11"/>
       <c r="E200" s="8" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>208</v>
@@ -6224,33 +6229,33 @@
       <c r="C201" s="11"/>
       <c r="D201" s="11"/>
       <c r="E201" s="8" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B202" s="8" t="s">
         <v>284</v>
       </c>
       <c r="C202" s="11"/>
       <c r="D202" s="11" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="E202" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B203" s="8" t="s">
         <v>150</v>
@@ -6262,7 +6267,7 @@
         <v>151</v>
       </c>
       <c r="E203" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="F203" s="8" t="s">
         <v>153</v>
@@ -6270,17 +6275,17 @@
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C204" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D204" s="8"/>
       <c r="E204" s="8" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="G204" s="4" t="s">
         <v>94</v>
@@ -6288,17 +6293,17 @@
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C205" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="G205" s="4" t="s">
         <v>94</v>
@@ -6306,7 +6311,7 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B206" s="8" t="s">
         <v>263</v>
@@ -6314,7 +6319,7 @@
       <c r="C206" s="11"/>
       <c r="D206" s="11"/>
       <c r="E206" s="8" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="F206" s="8"/>
       <c r="G206" s="4" t="s">
@@ -6323,97 +6328,97 @@
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C207" s="11"/>
       <c r="D207" s="11" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="E207" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C208" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C209" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="E209" s="8" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="F209" s="8" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="10" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C210" s="11" t="n">
         <v>8400</v>
       </c>
       <c r="D210" s="11" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="E210" s="8" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="F210" s="8" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="10" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B211" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E211" s="8" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B212" s="8" t="s">
         <v>323</v>
@@ -6423,7 +6428,7 @@
       </c>
       <c r="D212" s="8"/>
       <c r="E212" s="8" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="F212" s="8"/>
       <c r="G212" s="4" t="s">
@@ -6432,19 +6437,19 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C213" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="F213" s="8"/>
       <c r="G213" s="4" t="s">
@@ -6453,7 +6458,7 @@
     </row>
     <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="10" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B214" s="8" t="s">
         <v>16</v>
@@ -6461,25 +6466,25 @@
       <c r="C214" s="11"/>
       <c r="D214" s="11"/>
       <c r="E214" s="8" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F214" s="8" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="10" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C215" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D215" s="8"/>
       <c r="E215" s="8" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="G215" s="4" t="s">
         <v>94</v>
@@ -6487,13 +6492,13 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B216" s="8" t="s">
         <v>205</v>
       </c>
       <c r="E216" s="8" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F216" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added more Resource links
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="800">
   <si>
     <t>Hash</t>
   </si>
@@ -947,6 +947,9 @@
     <t>b7c2d6f13a43dce2e44ad120a9cd8a13d0ca23f0414275c0bbe1070d2d1299b1c04da0f1a0f1e4e2537300263a2200000000000000000000140768617368636174:472bdabe2d5d4bffd6add7b3ba79a291d104a9ef</t>
   </si>
   <si>
+    <t>https://community.rapid7.com/community/metasploit/blog/2013/07/02/a-penetration-testers-guide-to-ipmi</t>
+  </si>
+  <si>
     <t>iSCSI CHAP Authentication</t>
   </si>
   <si>
@@ -1097,6 +1100,9 @@
     <t>3dd2e1e5ac03e230243d58b8c5ada076</t>
   </si>
   <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/lotus5_fmt_plug.c</t>
+  </si>
+  <si>
     <t>Lotus Notes/Domino 6</t>
   </si>
   <si>
@@ -1110,6 +1116,9 @@
   </si>
   <si>
     <t>(Gv0GtxzT8DYnLKAKDNsB)</t>
+  </si>
+  <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/DOMINOSEC_fmt_plug.c</t>
   </si>
   <si>
     <t>Lotus Notes/Domino 8</t>
@@ -2593,8 +2602,8 @@
   </sheetPr>
   <dimension ref="A1:G216"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4080,33 +4089,33 @@
       <c r="E82" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="G82" s="4" t="s">
-        <v>94</v>
+      <c r="F82" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C83" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>16</v>
@@ -4114,86 +4123,86 @@
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C85" s="8" t="n">
         <v>11</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C87" s="8" t="n">
         <v>22</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C88" s="8" t="n">
         <v>7500</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>11</v>
@@ -4201,51 +4210,51 @@
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C89" s="8" t="n">
         <v>6800</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C90" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F91" s="8"/>
       <c r="G91" s="4" t="s">
@@ -4254,7 +4263,7 @@
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>208</v>
@@ -4263,18 +4272,18 @@
         <v>190</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>205</v>
@@ -4283,75 +4292,75 @@
         <v>3000</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>94</v>
+        <v>360</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>94</v>
+        <v>366</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="C96" s="9" t="n">
         <v>9100</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>208</v>
@@ -4359,33 +4368,33 @@
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="8" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="11" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>205</v>
@@ -4394,38 +4403,38 @@
         <v>900</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>91</v>
@@ -4437,15 +4446,15 @@
         <v>92</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>45</v>
@@ -4463,252 +4472,252 @@
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C103" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="10" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="8" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="12" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C106" s="9" t="n">
         <v>9700</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="12" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C107" s="9" t="n">
         <v>9800</v>
       </c>
       <c r="E107" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="F107" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C108" s="9" t="n">
         <v>9400</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C109" s="9" t="n">
         <v>9500</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C110" s="9" t="n">
         <v>9600</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="8" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
       <c r="E113" s="8" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C114" s="8" t="n">
         <v>131</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="C115" s="8" t="n">
         <v>132</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="C116" s="11" t="n">
         <v>132</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E116" s="8"/>
       <c r="G116" s="4" t="s">
@@ -4717,65 +4726,65 @@
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C117" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="C119" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="8" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>131</v>
@@ -4784,166 +4793,166 @@
         <v>200</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="15" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="F121" s="8" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C122" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C123" s="8" t="n">
         <v>5500</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="124" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C125" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C126" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C127" s="11"/>
       <c r="D127" s="11"/>
       <c r="E127" s="8" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>94</v>
@@ -4951,27 +4960,27 @@
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C129" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>131</v>
@@ -4981,33 +4990,33 @@
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="C131" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D131" s="8"/>
       <c r="E131" s="8" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="F131" s="8" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>284</v>
@@ -5016,48 +5025,48 @@
         <v>122</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="C133" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C134" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D134" s="12"/>
       <c r="E134" s="8" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="G134" s="4" t="s">
         <v>94</v>
@@ -5065,15 +5074,15 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="8" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="F135" s="8"/>
       <c r="G135" s="4" t="s">
@@ -5082,148 +5091,148 @@
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="10" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C139" s="3"/>
       <c r="E139" s="8" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="8" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C141" s="11"/>
       <c r="D141" s="11"/>
       <c r="E141" s="8" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C142" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C143" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="F143" s="8" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C144" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="F144" s="8"/>
       <c r="G144" s="4" t="s">
@@ -5232,137 +5241,137 @@
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="C145" s="9" t="n">
         <v>2612</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="C146" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="D149" s="11" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="E149" s="8" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="C150" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D150" s="8"/>
       <c r="E150" s="8" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>205</v>
       </c>
       <c r="C151" s="11"/>
       <c r="D151" s="11" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>208</v>
@@ -5371,18 +5380,18 @@
         <v>6000</v>
       </c>
       <c r="D152" s="8" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="E152" s="8" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>263</v>
@@ -5390,165 +5399,165 @@
       <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="8" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
+        <v>606</v>
+      </c>
+      <c r="B156" s="8" t="s">
         <v>603</v>
-      </c>
-      <c r="B156" s="8" t="s">
-        <v>600</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
       <c r="E156" s="8" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="C157" s="11"/>
       <c r="D157" s="11"/>
       <c r="E157" s="8" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="C158" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D158" s="8" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="C159" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D159" s="8" t="s">
+        <v>620</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="F159" s="8" t="s">
         <v>617</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>618</v>
-      </c>
-      <c r="F159" s="8" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="B160" s="17" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="C160" s="14" t="n">
         <v>10300</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="C161" s="11"/>
       <c r="D161" s="11"/>
       <c r="E161" s="8" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="C162" s="9" t="n">
         <v>8900</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="2" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="G162" s="4" t="s">
         <v>11</v>
@@ -5556,7 +5565,7 @@
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="B163" s="8" t="s">
         <v>208</v>
@@ -5565,56 +5574,56 @@
         <v>100</v>
       </c>
       <c r="D163" s="11" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="C164" s="11"/>
       <c r="D164" s="11" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="E164" s="8" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C165" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="E165" s="8" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>284</v>
@@ -5622,7 +5631,7 @@
       <c r="C166" s="11"/>
       <c r="D166" s="11"/>
       <c r="E166" s="8" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="F166" s="8"/>
       <c r="G166" s="4" t="s">
@@ -5631,25 +5640,25 @@
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="B167" s="8" t="s">
         <v>287</v>
       </c>
       <c r="C167" s="11"/>
       <c r="D167" s="11" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="E167" s="8" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="10" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>263</v>
@@ -5658,264 +5667,264 @@
         <v>1400</v>
       </c>
       <c r="D168" s="8" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="E168" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F168" s="8" t="s">
         <v>649</v>
-      </c>
-      <c r="F168" s="8" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C169" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D169" s="8" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C170" s="11"/>
       <c r="D170" s="11" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C171" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D171" s="8" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="C172" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>287</v>
       </c>
       <c r="E173" s="8" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="B174" s="8" t="s">
         <v>263</v>
       </c>
       <c r="C174" s="11" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="D174" s="11" t="s">
+        <v>675</v>
+      </c>
+      <c r="E174" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="F174" s="8" t="s">
         <v>672</v>
-      </c>
-      <c r="E174" s="8" t="s">
-        <v>673</v>
-      </c>
-      <c r="F174" s="8" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C175" s="11"/>
       <c r="D175" s="11"/>
       <c r="E175" s="8" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C176" s="11"/>
       <c r="D176" s="11" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="E176" s="8" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="C178" s="14" t="n">
         <v>10100</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="C179" s="11"/>
       <c r="D179" s="11"/>
       <c r="E179" s="8" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>263</v>
       </c>
       <c r="C182" s="11"/>
       <c r="D182" s="11" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="E182" s="8" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>205</v>
@@ -5923,15 +5932,15 @@
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="B184" s="8" t="s">
         <v>208</v>
@@ -5939,15 +5948,15 @@
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="B185" s="8" t="s">
         <v>287</v>
@@ -5955,33 +5964,33 @@
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C186" s="11"/>
       <c r="D186" s="11" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="E186" s="8" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B187" s="8" t="s">
         <v>205</v>
@@ -5989,15 +5998,15 @@
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="B188" s="8" t="s">
         <v>208</v>
@@ -6005,15 +6014,15 @@
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="B189" s="8" t="s">
         <v>287</v>
@@ -6021,15 +6030,15 @@
       <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="8" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="B190" s="8" t="s">
         <v>263</v>
@@ -6037,58 +6046,58 @@
       <c r="C190" s="11"/>
       <c r="D190" s="11"/>
       <c r="E190" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C191" s="11"/>
       <c r="D191" s="11"/>
       <c r="E191" s="8" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="C192" s="9" t="n">
         <v>23</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="F192" s="9" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="C193" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="G193" s="4" t="s">
         <v>94</v>
@@ -6096,123 +6105,123 @@
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="C194" s="11"/>
       <c r="D194" s="11" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="E194" s="8" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="C195" s="11"/>
       <c r="D195" s="11" t="s">
+        <v>735</v>
+      </c>
+      <c r="E195" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="F195" s="8" t="s">
         <v>732</v>
-      </c>
-      <c r="E195" s="8" t="s">
-        <v>733</v>
-      </c>
-      <c r="F195" s="8" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C196" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="E196" s="8" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C197" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="E197" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="C198" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
       <c r="E198" s="8" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="C199" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="E199" s="8" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>205</v>
@@ -6220,15 +6229,15 @@
       <c r="C200" s="11"/>
       <c r="D200" s="11"/>
       <c r="E200" s="8" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>208</v>
@@ -6236,33 +6245,33 @@
       <c r="C201" s="11"/>
       <c r="D201" s="11"/>
       <c r="E201" s="8" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="B202" s="8" t="s">
         <v>284</v>
       </c>
       <c r="C202" s="11"/>
       <c r="D202" s="11" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="E202" s="8" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
       <c r="B203" s="8" t="s">
         <v>150</v>
@@ -6274,7 +6283,7 @@
         <v>151</v>
       </c>
       <c r="E203" s="8" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="F203" s="8" t="s">
         <v>153</v>
@@ -6282,17 +6291,17 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="C204" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D204" s="8"/>
       <c r="E204" s="8" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="G204" s="4" t="s">
         <v>94</v>
@@ -6300,17 +6309,17 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C205" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="G205" s="4" t="s">
         <v>94</v>
@@ -6318,7 +6327,7 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="B206" s="8" t="s">
         <v>263</v>
@@ -6326,7 +6335,7 @@
       <c r="C206" s="11"/>
       <c r="D206" s="11"/>
       <c r="E206" s="8" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="F206" s="8"/>
       <c r="G206" s="4" t="s">
@@ -6335,107 +6344,107 @@
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="C207" s="11"/>
       <c r="D207" s="11" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="E207" s="8" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="C208" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="8" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C209" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="E209" s="8" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="F209" s="8" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="10" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="C210" s="11" t="n">
         <v>8400</v>
       </c>
       <c r="D210" s="11" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="E210" s="8" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="F210" s="8" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
     </row>
     <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="10" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
       <c r="B211" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E211" s="8" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C212" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D212" s="8"/>
       <c r="E212" s="8" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="F212" s="8"/>
       <c r="G212" s="4" t="s">
@@ -6444,19 +6453,19 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C213" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="F213" s="8"/>
       <c r="G213" s="4" t="s">
@@ -6465,7 +6474,7 @@
     </row>
     <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="10" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="B214" s="8" t="s">
         <v>16</v>
@@ -6473,25 +6482,25 @@
       <c r="C214" s="11"/>
       <c r="D214" s="11"/>
       <c r="E214" s="8" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="F214" s="8" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="10" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="C215" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D215" s="8"/>
       <c r="E215" s="8" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="G215" s="4" t="s">
         <v>94</v>
@@ -6499,13 +6508,13 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="B216" s="8" t="s">
         <v>205</v>
       </c>
       <c r="E216" s="8" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="F216" s="8"/>
     </row>

</xml_diff>

<commit_message>
Add PDF 1.4 - 1.6 (Acrobat 5 - 8). #25
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="806">
   <si>
     <t>Hash</t>
   </si>
@@ -1665,6 +1665,21 @@
   </si>
   <si>
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.dlitz_pbkdf2_sha1.html</t>
+  </si>
+  <si>
+    <t>PDF 1.4 - 1.6 (Acrobat 5 - 8)</t>
+  </si>
+  <si>
+    <t>^\$pdf\$2\*3\*128\*[0-9-]{1,5}\*1\*16\*[a-f0-9]{32}\*32\*[a-f0-9]{64}\*(8|16|32)\*[a-f0-9]{16,64}$/i</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>$pdf$2*3*128*-1028*1*16*da42ee15d4b3e08fe5b9ecea0e02ad0f*32*c9b59d72c7c670c42eeb4fca1d2ca15000000000000000000000000000000000*32*c4ff3e868dc87604626c2b8c259297a14d58c6309c70b00afdfb1fbba10ee571 </t>
+  </si>
+  <si>
+    <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/run/pdf2john.py</t>
   </si>
   <si>
     <t>PeopleSoft</t>
@@ -2603,10 +2618,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G216"/>
+  <dimension ref="A1:G217"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A142" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5191,101 +5206,101 @@
         <v>549</v>
       </c>
     </row>
-    <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="s">
+    <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="B142" s="8" t="s">
+      <c r="B142" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C142" s="9" t="n">
+      <c r="C142" s="3" t="n">
+        <v>10500</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="C143" s="9" t="n">
         <v>133</v>
       </c>
-      <c r="E142" s="8" t="s">
-        <v>552</v>
-      </c>
-      <c r="F142" s="9" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="B143" s="8" t="s">
+      <c r="E143" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="F143" s="9" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="B144" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="C143" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D143" s="8" t="s">
-        <v>555</v>
-      </c>
-      <c r="E143" s="8" t="s">
-        <v>556</v>
-      </c>
-      <c r="F143" s="8" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="B144" s="8" t="s">
-        <v>559</v>
       </c>
       <c r="C144" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="E144" s="8" t="s">
+        <v>561</v>
+      </c>
+      <c r="F144" s="8" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="C145" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D145" s="8" t="s">
         <v>560</v>
       </c>
-      <c r="F144" s="8"/>
-      <c r="G144" s="4" t="s">
+      <c r="E145" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="F145" s="8"/>
+      <c r="G145" s="4" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="C145" s="9" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D145" s="9" t="s">
-        <v>563</v>
-      </c>
-      <c r="E145" s="8" t="s">
-        <v>564</v>
-      </c>
-      <c r="F145" s="8" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="C146" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D146" s="3" t="s">
+      <c r="C146" s="9" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D146" s="9" t="s">
         <v>568</v>
       </c>
-      <c r="E146" s="2" t="s">
+      <c r="E146" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="F146" s="2" t="s">
+      <c r="F146" s="8" t="s">
         <v>570</v>
       </c>
     </row>
@@ -5293,205 +5308,205 @@
       <c r="A147" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="B147" s="8" t="s">
+      <c r="B147" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E147" s="8" t="s">
+      <c r="C147" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D147" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="F147" s="9" t="s">
+      <c r="E147" s="2" t="s">
         <v>574</v>
       </c>
+      <c r="F147" s="2" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="10" t="s">
-        <v>575</v>
+      <c r="A148" s="1" t="s">
+        <v>576</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="C148" s="8" t="s">
         <v>577</v>
       </c>
-      <c r="D148" s="8" t="s">
+      <c r="E148" s="8" t="s">
         <v>578</v>
       </c>
-      <c r="E148" s="8" t="s">
+      <c r="F148" s="9" t="s">
         <v>579</v>
-      </c>
-      <c r="F148" s="8" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
+        <v>580</v>
+      </c>
+      <c r="B149" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="B149" s="8" t="s">
+      <c r="C149" s="8" t="s">
         <v>582</v>
       </c>
-      <c r="C149" s="11" t="s">
+      <c r="D149" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="D149" s="11" t="s">
+      <c r="E149" s="8" t="s">
         <v>584</v>
       </c>
-      <c r="E149" s="8" t="s">
+      <c r="F149" s="8" t="s">
         <v>585</v>
-      </c>
-      <c r="F149" s="8" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="B150" s="8" t="s">
         <v>587</v>
       </c>
-      <c r="B150" s="8" t="s">
+      <c r="C150" s="11" t="s">
         <v>588</v>
       </c>
-      <c r="C150" s="8" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D150" s="8"/>
+      <c r="D150" s="11" t="s">
+        <v>589</v>
+      </c>
       <c r="E150" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C151" s="11"/>
-      <c r="D151" s="11" t="s">
-        <v>592</v>
-      </c>
+        <v>593</v>
+      </c>
+      <c r="C151" s="8" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D151" s="8"/>
       <c r="E151" s="8" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C152" s="8" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D152" s="8" t="s">
-        <v>596</v>
+        <v>206</v>
+      </c>
+      <c r="C152" s="11"/>
+      <c r="D152" s="11" t="s">
+        <v>597</v>
       </c>
       <c r="E152" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C153" s="11"/>
-      <c r="D153" s="11"/>
+        <v>209</v>
+      </c>
+      <c r="C153" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D153" s="8" t="s">
+        <v>601</v>
+      </c>
       <c r="E153" s="8" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>602</v>
+        <v>264</v>
       </c>
       <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="8" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
       <c r="E156" s="8" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C157" s="11"/>
       <c r="D157" s="11"/>
       <c r="E157" s="8" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>616</v>
-      </c>
-      <c r="C158" s="8" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D158" s="8" t="s">
         <v>617</v>
       </c>
+      <c r="C158" s="11"/>
+      <c r="D158" s="11"/>
       <c r="E158" s="8" t="s">
         <v>618</v>
       </c>
@@ -5507,7 +5522,7 @@
         <v>621</v>
       </c>
       <c r="C159" s="8" t="n">
-        <v>7800</v>
+        <v>7700</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>622</v>
@@ -5516,90 +5531,92 @@
         <v>623</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="160" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="B160" s="17" t="s">
+    </row>
+    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="C160" s="14" t="n">
+      <c r="B160" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="C160" s="8" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D160" s="8" t="s">
+        <v>627</v>
+      </c>
+      <c r="E160" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="F160" s="8" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="161" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B161" s="17" t="s">
+        <v>630</v>
+      </c>
+      <c r="C161" s="14" t="n">
         <v>10300</v>
       </c>
-      <c r="D160" s="3" t="s">
-        <v>626</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="10" t="s">
-        <v>629</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>630</v>
-      </c>
-      <c r="C161" s="11"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="8" t="s">
+      <c r="D161" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="F161" s="8" t="s">
+      <c r="E161" s="2" t="s">
         <v>632</v>
       </c>
+      <c r="F161" s="2" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="s">
-        <v>633</v>
+      <c r="A162" s="10" t="s">
+        <v>634</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>634</v>
-      </c>
-      <c r="C162" s="9" t="n">
+        <v>635</v>
+      </c>
+      <c r="C162" s="11"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="F162" s="8" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="C163" s="9" t="n">
         <v>8900</v>
       </c>
-      <c r="E162" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="G162" s="4" t="s">
+      <c r="E163" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="G163" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C163" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="D163" s="11" t="s">
-        <v>637</v>
-      </c>
-      <c r="E163" s="8" t="s">
-        <v>638</v>
-      </c>
-      <c r="F163" s="8" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>641</v>
-      </c>
-      <c r="C164" s="11"/>
+        <v>209</v>
+      </c>
+      <c r="C164" s="11" t="n">
+        <v>100</v>
+      </c>
       <c r="D164" s="11" t="s">
         <v>642</v>
       </c>
@@ -5610,157 +5627,155 @@
         <v>644</v>
       </c>
     </row>
-    <row r="165" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
         <v>645</v>
       </c>
       <c r="B165" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="C165" s="11"/>
+      <c r="D165" s="11" t="s">
+        <v>647</v>
+      </c>
+      <c r="E165" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="F165" s="8" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="166" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="10" t="s">
+        <v>650</v>
+      </c>
+      <c r="B166" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="C165" s="8" t="n">
+      <c r="C166" s="8" t="n">
         <v>101</v>
       </c>
-      <c r="D165" s="12" t="s">
+      <c r="D166" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="E165" s="8" t="s">
+      <c r="E166" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="F165" s="2" t="s">
+      <c r="F166" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="10" t="s">
-        <v>646</v>
-      </c>
-      <c r="B166" s="8" t="s">
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="10" t="s">
+        <v>651</v>
+      </c>
+      <c r="B167" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C166" s="11"/>
-      <c r="D166" s="11"/>
-      <c r="E166" s="8" t="s">
-        <v>647</v>
-      </c>
-      <c r="F166" s="8"/>
-      <c r="G166" s="4" t="s">
+      <c r="C167" s="11"/>
+      <c r="D167" s="11"/>
+      <c r="E167" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F167" s="8"/>
+      <c r="G167" s="4" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="10" t="s">
-        <v>648</v>
-      </c>
-      <c r="B167" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="C167" s="11"/>
-      <c r="D167" s="11" t="s">
-        <v>649</v>
-      </c>
-      <c r="E167" s="8" t="s">
-        <v>650</v>
-      </c>
-      <c r="F167" s="8" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="10" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B168" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C168" s="11"/>
+      <c r="D168" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="E168" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="F168" s="8" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="B169" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="C168" s="8" t="n">
+      <c r="C169" s="8" t="n">
         <v>1400</v>
       </c>
-      <c r="D168" s="8" t="s">
-        <v>653</v>
-      </c>
-      <c r="E168" s="8" t="s">
-        <v>654</v>
-      </c>
-      <c r="F168" s="8" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="B169" s="8" t="s">
+      <c r="D169" s="8" t="s">
+        <v>658</v>
+      </c>
+      <c r="E169" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="F169" s="8" t="s">
         <v>656</v>
       </c>
-      <c r="C169" s="8" t="n">
-        <v>7400</v>
-      </c>
-      <c r="D169" s="8" t="s">
-        <v>657</v>
-      </c>
-      <c r="E169" s="8" t="s">
-        <v>658</v>
-      </c>
-      <c r="F169" s="8" t="s">
-        <v>659</v>
-      </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="10" t="s">
+      <c r="A170" s="1" t="s">
         <v>660</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>661</v>
       </c>
-      <c r="C170" s="11"/>
-      <c r="D170" s="11" t="s">
+      <c r="C170" s="8" t="n">
+        <v>7400</v>
+      </c>
+      <c r="D170" s="8" t="s">
         <v>662</v>
       </c>
       <c r="E170" s="8" t="s">
         <v>663</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>651</v>
+        <v>664</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>605</v>
-      </c>
-      <c r="C171" s="8" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D171" s="8" t="s">
-        <v>665</v>
+        <v>666</v>
+      </c>
+      <c r="C171" s="11"/>
+      <c r="D171" s="11" t="s">
+        <v>667</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>668</v>
+        <v>610</v>
       </c>
       <c r="C172" s="8" t="n">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5768,366 +5783,368 @@
         <v>672</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>288</v>
+        <v>673</v>
+      </c>
+      <c r="C173" s="8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D173" s="8" t="s">
+        <v>674</v>
       </c>
       <c r="E173" s="8" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C174" s="11" t="s">
-        <v>676</v>
-      </c>
-      <c r="D174" s="11" t="s">
-        <v>677</v>
+        <v>288</v>
       </c>
       <c r="E174" s="8" t="s">
         <v>678</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C175" s="11" t="s">
+        <v>681</v>
+      </c>
+      <c r="D175" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="E175" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="F175" s="8" t="s">
         <v>679</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>661</v>
-      </c>
-      <c r="C175" s="11"/>
-      <c r="D175" s="11"/>
-      <c r="E175" s="8" t="s">
-        <v>680</v>
-      </c>
-      <c r="F175" s="8" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>605</v>
+        <v>666</v>
       </c>
       <c r="C176" s="11"/>
-      <c r="D176" s="11" t="s">
-        <v>682</v>
-      </c>
+      <c r="D176" s="11"/>
       <c r="E176" s="8" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="D177" s="3" t="s">
+      <c r="A177" s="10" t="s">
         <v>686</v>
       </c>
-      <c r="E177" s="2" t="s">
+      <c r="B177" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="C177" s="11"/>
+      <c r="D177" s="11" t="s">
         <v>687</v>
       </c>
-      <c r="F177" s="2" t="s">
+      <c r="E177" s="8" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="178" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F177" s="8" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
         <v>689</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="C178" s="14" t="n">
+      <c r="D178" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="179" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="C179" s="14" t="n">
         <v>10100</v>
       </c>
-      <c r="E178" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="F178" s="2" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="10" t="s">
-        <v>693</v>
-      </c>
-      <c r="B179" s="8" t="s">
-        <v>694</v>
-      </c>
-      <c r="C179" s="11"/>
-      <c r="D179" s="11"/>
-      <c r="E179" s="8" t="s">
-        <v>695</v>
-      </c>
-      <c r="F179" s="8" t="s">
+      <c r="E179" s="2" t="s">
         <v>696</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>661</v>
+        <v>699</v>
       </c>
       <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>605</v>
+        <v>666</v>
       </c>
       <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="8" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
+        <v>704</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="C182" s="11"/>
+      <c r="D182" s="11"/>
+      <c r="E182" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="F182" s="8" t="s">
         <v>701</v>
-      </c>
-      <c r="B182" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C182" s="11"/>
-      <c r="D182" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="E182" s="8" t="s">
-        <v>703</v>
-      </c>
-      <c r="F182" s="8" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>206</v>
+        <v>264</v>
       </c>
       <c r="C183" s="11"/>
-      <c r="D183" s="11"/>
+      <c r="D183" s="11" t="s">
+        <v>707</v>
+      </c>
       <c r="E183" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>288</v>
+        <v>209</v>
       </c>
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>605</v>
+        <v>288</v>
       </c>
       <c r="C186" s="11"/>
-      <c r="D186" s="11" t="s">
-        <v>711</v>
-      </c>
+      <c r="D186" s="11"/>
       <c r="E186" s="8" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>206</v>
+        <v>610</v>
       </c>
       <c r="C187" s="11"/>
-      <c r="D187" s="11"/>
+      <c r="D187" s="11" t="s">
+        <v>716</v>
+      </c>
       <c r="E187" s="8" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>288</v>
+        <v>209</v>
       </c>
       <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="8" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="C190" s="11"/>
       <c r="D190" s="11"/>
       <c r="E190" s="8" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>661</v>
+        <v>264</v>
       </c>
       <c r="C191" s="11"/>
       <c r="D191" s="11"/>
       <c r="E191" s="8" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="1" t="s">
-        <v>723</v>
+      <c r="A192" s="10" t="s">
+        <v>726</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>724</v>
-      </c>
-      <c r="C192" s="9" t="n">
+        <v>666</v>
+      </c>
+      <c r="C192" s="11"/>
+      <c r="D192" s="11"/>
+      <c r="E192" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="F192" s="8" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>729</v>
+      </c>
+      <c r="C193" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="E192" s="8" t="s">
-        <v>725</v>
-      </c>
-      <c r="F192" s="9" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="10" t="s">
-        <v>727</v>
-      </c>
-      <c r="B193" s="8" t="s">
-        <v>728</v>
-      </c>
-      <c r="C193" s="8" t="n">
-        <v>121</v>
-      </c>
-      <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>729</v>
-      </c>
-      <c r="G193" s="4" t="s">
-        <v>95</v>
+        <v>730</v>
+      </c>
+      <c r="F193" s="9" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>731</v>
-      </c>
-      <c r="C194" s="11"/>
-      <c r="D194" s="11" t="s">
-        <v>732</v>
-      </c>
+        <v>733</v>
+      </c>
+      <c r="C194" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="D194" s="8"/>
       <c r="E194" s="8" t="s">
-        <v>733</v>
-      </c>
-      <c r="F194" s="8" t="s">
         <v>734</v>
+      </c>
+      <c r="G194" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6145,78 +6162,76 @@
         <v>738</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
+        <v>740</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="C196" s="11"/>
+      <c r="D196" s="11" t="s">
+        <v>742</v>
+      </c>
+      <c r="E196" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="F196" s="8" t="s">
         <v>739</v>
-      </c>
-      <c r="B196" s="8" t="s">
-        <v>487</v>
-      </c>
-      <c r="C196" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D196" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="E196" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="F196" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c r="B197" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="C197" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D197" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="F197" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="B198" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="C197" s="8" t="n">
+      <c r="C198" s="8" t="n">
         <v>1711</v>
       </c>
-      <c r="D197" s="8" t="s">
+      <c r="D198" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="E197" s="8" t="s">
+      <c r="E198" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="F197" s="8" t="s">
+      <c r="F198" s="8" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="B198" s="8" t="s">
-        <v>742</v>
-      </c>
-      <c r="C198" s="8" t="n">
-        <v>3300</v>
-      </c>
-      <c r="D198" s="8" t="s">
-        <v>743</v>
-      </c>
-      <c r="E198" s="8" t="s">
-        <v>744</v>
-      </c>
-      <c r="F198" s="8" t="s">
-        <v>745</v>
-      </c>
-    </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="10" t="s">
+      <c r="A199" s="1" t="s">
         <v>746</v>
       </c>
       <c r="B199" s="8" t="s">
         <v>747</v>
       </c>
       <c r="C199" s="8" t="n">
-        <v>8000</v>
+        <v>3300</v>
       </c>
       <c r="D199" s="8" t="s">
         <v>748</v>
@@ -6233,140 +6248,142 @@
         <v>751</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C200" s="11"/>
-      <c r="D200" s="11"/>
+        <v>752</v>
+      </c>
+      <c r="C200" s="8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D200" s="8" t="s">
+        <v>753</v>
+      </c>
       <c r="E200" s="8" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C201" s="11"/>
       <c r="D201" s="11"/>
       <c r="E201" s="8" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="B202" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C202" s="11"/>
+      <c r="D202" s="11"/>
+      <c r="E202" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="F202" s="8" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="10" t="s">
+        <v>761</v>
+      </c>
+      <c r="B203" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="C202" s="11"/>
-      <c r="D202" s="11" t="s">
-        <v>757</v>
-      </c>
-      <c r="E202" s="8" t="s">
+      <c r="C203" s="11"/>
+      <c r="D203" s="11" t="s">
+        <v>762</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="F203" s="8" t="s">
         <v>758</v>
       </c>
-      <c r="F202" s="8" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="203" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="10" t="s">
-        <v>759</v>
-      </c>
-      <c r="B203" s="8" t="s">
+    </row>
+    <row r="204" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="10" t="s">
+        <v>764</v>
+      </c>
+      <c r="B204" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C203" s="8" t="n">
+      <c r="C204" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="D203" s="12" t="s">
+      <c r="D204" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="E203" s="8" t="s">
-        <v>760</v>
-      </c>
-      <c r="F203" s="8" t="s">
+      <c r="E204" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="F204" s="8" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="10" t="s">
-        <v>761</v>
-      </c>
-      <c r="B204" s="8" t="s">
-        <v>762</v>
-      </c>
-      <c r="C204" s="8" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D204" s="8"/>
-      <c r="E204" s="8" t="s">
-        <v>763</v>
-      </c>
-      <c r="G204" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C205" s="8" t="n">
-        <v>2711</v>
+        <v>2611</v>
       </c>
       <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="G205" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C206" s="11"/>
-      <c r="D206" s="11"/>
+        <v>770</v>
+      </c>
+      <c r="C206" s="8" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D206" s="8"/>
       <c r="E206" s="8" t="s">
-        <v>768</v>
-      </c>
-      <c r="F206" s="8"/>
+        <v>771</v>
+      </c>
       <c r="G206" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>770</v>
+        <v>264</v>
       </c>
       <c r="C207" s="11"/>
-      <c r="D207" s="11" t="s">
-        <v>771</v>
-      </c>
+      <c r="D207" s="11"/>
       <c r="E207" s="8" t="s">
-        <v>772</v>
-      </c>
-      <c r="F207" s="8" t="s">
         <v>773</v>
+      </c>
+      <c r="F207" s="8"/>
+      <c r="G207" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6376,48 +6393,46 @@
       <c r="B208" s="8" t="s">
         <v>775</v>
       </c>
-      <c r="C208" s="8" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D208" s="8"/>
+      <c r="C208" s="11"/>
+      <c r="D208" s="11" t="s">
+        <v>776</v>
+      </c>
       <c r="E208" s="8" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>605</v>
+        <v>780</v>
       </c>
       <c r="C209" s="8" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D209" s="8" t="s">
-        <v>779</v>
-      </c>
+        <v>3721</v>
+      </c>
+      <c r="D209" s="8"/>
       <c r="E209" s="8" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="F209" s="8" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="10" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>783</v>
-      </c>
-      <c r="C210" s="11" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D210" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="C210" s="8" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D210" s="8" t="s">
         <v>784</v>
       </c>
       <c r="E210" s="8" t="s">
@@ -6432,102 +6447,122 @@
         <v>787</v>
       </c>
       <c r="B211" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="C211" s="11" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D211" s="11" t="s">
+        <v>789</v>
+      </c>
+      <c r="E211" s="8" t="s">
+        <v>790</v>
+      </c>
+      <c r="F211" s="8" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="B212" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E211" s="8" t="s">
-        <v>788</v>
-      </c>
-      <c r="F211" s="8" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="B212" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C212" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D212" s="8" t="s">
-        <v>555</v>
-      </c>
       <c r="E212" s="8" t="s">
-        <v>791</v>
-      </c>
-      <c r="F212" s="8"/>
-      <c r="G212" s="4" t="s">
-        <v>95</v>
+        <v>793</v>
+      </c>
+      <c r="F212" s="8" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>559</v>
+        <v>325</v>
       </c>
       <c r="C213" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D213" s="8" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="F213" s="8"/>
       <c r="G213" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="10" t="s">
-        <v>794</v>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>797</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C214" s="11"/>
-      <c r="D214" s="11"/>
+        <v>564</v>
+      </c>
+      <c r="C214" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D214" s="8" t="s">
+        <v>560</v>
+      </c>
       <c r="E214" s="8" t="s">
-        <v>795</v>
-      </c>
-      <c r="F214" s="8" t="s">
-        <v>796</v>
+        <v>798</v>
+      </c>
+      <c r="F214" s="8"/>
+      <c r="G214" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="10" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B215" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C215" s="11"/>
+      <c r="D215" s="11"/>
+      <c r="E215" s="8" t="s">
+        <v>800</v>
+      </c>
+      <c r="F215" s="8" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="216" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="10" t="s">
+        <v>802</v>
+      </c>
+      <c r="B216" s="8" t="s">
         <v>507</v>
       </c>
-      <c r="C215" s="8" t="n">
+      <c r="C216" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="D215" s="8"/>
-      <c r="E215" s="8" t="s">
-        <v>798</v>
-      </c>
-      <c r="G215" s="4" t="s">
+      <c r="D216" s="8"/>
+      <c r="E216" s="8" t="s">
+        <v>803</v>
+      </c>
+      <c r="G216" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="B216" s="8" t="s">
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B217" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="E216" s="8" t="s">
-        <v>800</v>
-      </c>
-      <c r="F216" s="8"/>
+      <c r="E217" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="F217" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fix JtR format for Joomla ≥ v2.5.18
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="810">
   <si>
     <t>Hash</t>
   </si>
@@ -998,6 +998,9 @@
     <t>400</t>
   </si>
   <si>
+    <t>phpass</t>
+  </si>
+  <si>
     <t>$P$BnJQp8THhoquE07nb1MxS7NYupEuF4.</t>
   </si>
   <si>
@@ -1013,7 +1016,7 @@
     <t>md5ns</t>
   </si>
   <si>
-    <t>nNxKL2rOEkbBc9BFLsVGG6OtOUO/8n:user</t>
+    <t>hashid$nKKoGnruCt0AcmaOVskPnuNtkPKWEn</t>
   </si>
   <si>
     <t>http://www.juniper.net/techpubs/en_US/junos10.2/topics/task/configuration/snmpv3-encrypton-type-configuring-junos-nm.html</t>
@@ -1707,9 +1710,6 @@
   </si>
   <si>
     <t>PHPass' Portable Hash</t>
-  </si>
-  <si>
-    <t>phpass</t>
   </si>
   <si>
     <t>$P$8ohUJ.1sdFw09/bMaAQPTGDNi2BIUt1</t>
@@ -2632,8 +2632,8 @@
   </sheetPr>
   <dimension ref="A1:G218"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A136" activeCellId="0" sqref="A136"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E88" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4192,52 +4192,54 @@
       <c r="C86" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="D86" s="8"/>
+      <c r="D86" s="8" t="s">
+        <v>327</v>
+      </c>
       <c r="E86" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C87" s="8" t="n">
         <v>22</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C88" s="8" t="n">
         <v>7500</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>11</v>
@@ -4245,53 +4247,53 @@
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C89" s="8" t="n">
         <v>6800</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C90" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F91" s="8"/>
       <c r="G91" s="4" t="s">
@@ -4300,7 +4302,7 @@
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>209</v>
@@ -4309,18 +4311,18 @@
         <v>190</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>206</v>
@@ -4329,75 +4331,75 @@
         <v>3000</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>206</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C96" s="9" t="n">
         <v>9100</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>209</v>
@@ -4405,33 +4407,33 @@
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="11" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>206</v>
@@ -4440,38 +4442,38 @@
         <v>900</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>206</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>92</v>
@@ -4483,15 +4485,15 @@
         <v>93</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>46</v>
@@ -4509,7 +4511,7 @@
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>313</v>
@@ -4529,232 +4531,232 @@
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="10" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="12" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C106" s="9" t="n">
         <v>9700</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="12" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C107" s="9" t="n">
         <v>9800</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C108" s="9" t="n">
         <v>9400</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E108" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C109" s="9" t="n">
         <v>9500</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C110" s="9" t="n">
         <v>9600</v>
       </c>
       <c r="E110" s="9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
       <c r="E113" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C114" s="8" t="n">
         <v>131</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E114" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C115" s="8" t="n">
         <v>132</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C116" s="11" t="n">
         <v>132</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E116" s="8"/>
       <c r="G116" s="4" t="s">
@@ -4763,65 +4765,65 @@
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C117" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C119" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>132</v>
@@ -4830,166 +4832,166 @@
         <v>200</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="15" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F121" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C122" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C123" s="8" t="n">
         <v>5500</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C125" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C126" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C127" s="11"/>
       <c r="D127" s="11"/>
       <c r="E127" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>95</v>
@@ -4997,27 +4999,27 @@
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C129" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>132</v>
@@ -5027,33 +5029,33 @@
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C131" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D131" s="8"/>
       <c r="E131" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F131" s="8" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>285</v>
@@ -5062,48 +5064,48 @@
         <v>122</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E132" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C133" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C134" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D134" s="12"/>
       <c r="E134" s="8" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="G134" s="4" t="s">
         <v>95</v>
@@ -5111,170 +5113,170 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="10" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F135" s="8"/>
       <c r="G135" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C136" s="3" t="n">
         <v>10900</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="10" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C140" s="3"/>
       <c r="E140" s="8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C141" s="11"/>
       <c r="D141" s="11"/>
       <c r="E141" s="8" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="10" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C142" s="11"/>
       <c r="D142" s="11"/>
       <c r="E142" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F142" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="12" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C143" s="3" t="n">
         <v>10500</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C144" s="9" t="n">
         <v>133</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F144" s="9" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B145" s="8" t="s">
         <v>325</v>
@@ -5283,7 +5285,7 @@
         <v>400</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>564</v>
+        <v>327</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>565</v>
@@ -5303,7 +5305,7 @@
         <v>400</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>564</v>
+        <v>327</v>
       </c>
       <c r="E146" s="8" t="s">
         <v>569</v>
@@ -5679,19 +5681,19 @@
         <v>654</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C167" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D167" s="12" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E167" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6217,19 +6219,19 @@
         <v>748</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C198" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E198" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6237,19 +6239,19 @@
         <v>749</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C199" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E199" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6516,7 +6518,7 @@
         <v>400</v>
       </c>
       <c r="D214" s="8" t="s">
-        <v>564</v>
+        <v>327</v>
       </c>
       <c r="E214" s="8" t="s">
         <v>800</v>
@@ -6537,7 +6539,7 @@
         <v>400</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>564</v>
+        <v>327</v>
       </c>
       <c r="E215" s="8" t="s">
         <v>802</v>
@@ -6568,7 +6570,7 @@
         <v>806</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C217" s="8" t="n">
         <v>21</v>

</xml_diff>

<commit_message>
Add GOST CryptoPro S-Box
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="813">
   <si>
     <t>Hash</t>
   </si>
@@ -806,10 +806,19 @@
     <t>0036deca</t>
   </si>
   <si>
+    <t>GOST CryptoPro S-Box</t>
+  </si>
+  <si>
+    <t>^[a-f0-9]{64}$/i</t>
+  </si>
+  <si>
+    <t>152c92b3927adc73ec6e45b1a8410ffa8939d20b7a8f0a091d70d99e74d750c2</t>
+  </si>
+  <si>
+    <t>https://github.com/manuelm/php-src/commit/8ca43527e8b7e076779560f1472518bd1fe4d6ca</t>
+  </si>
+  <si>
     <t>GOST R 34.11-94</t>
-  </si>
-  <si>
-    <t>^[a-f0-9]{64}$/i</t>
   </si>
   <si>
     <t>gost</t>
@@ -2630,10 +2639,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G218"/>
+  <dimension ref="A1:G219"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E88" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3876,53 +3885,49 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10" t="s">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
         <v>263</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="C69" s="8" t="n">
-        <v>6900</v>
-      </c>
-      <c r="D69" s="8" t="s">
+      <c r="E69" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="F69" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C70" s="8" t="n">
+        <v>6900</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="C70" s="8" t="n">
-        <v>7200</v>
-      </c>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8" t="s">
+      <c r="F70" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B71" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="B71" s="8" t="s">
-        <v>132</v>
-      </c>
       <c r="C71" s="8" t="n">
-        <v>5100</v>
+        <v>7200</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="8" t="s">
@@ -3937,14 +3942,16 @@
         <v>275</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
+        <v>132</v>
+      </c>
+      <c r="C72" s="8" t="n">
+        <v>5100</v>
+      </c>
+      <c r="D72" s="8"/>
       <c r="E72" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F72" s="9" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3953,41 +3960,41 @@
         <v>278</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C73" s="11"/>
-      <c r="D73" s="11" t="s">
+      <c r="D73" s="11"/>
+      <c r="E73" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="F73" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="B74" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
       <c r="E74" s="8" t="s">
         <v>283</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>285</v>
+        <v>209</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -3995,7 +4002,7 @@
         <v>286</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4011,7 +4018,7 @@
         <v>289</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,148 +4026,148 @@
         <v>290</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="C77" s="11"/>
-      <c r="D77" s="11" t="s">
-        <v>291</v>
-      </c>
+      <c r="D77" s="11"/>
       <c r="E77" s="8" t="s">
         <v>292</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="10" t="s">
         <v>293</v>
       </c>
       <c r="B78" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="C78" s="11" t="n">
+      <c r="E78" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C79" s="11" t="n">
         <v>1421</v>
       </c>
-      <c r="D78" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="79" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="12" t="s">
+      <c r="D79" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="E79" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="C79" s="9" t="n">
-        <v>5300</v>
-      </c>
-      <c r="E79" s="8" t="s">
+      <c r="F79" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="80" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="C80" s="9" t="n">
+        <v>5300</v>
+      </c>
+      <c r="E80" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="C80" s="9" t="n">
-        <v>5400</v>
-      </c>
-      <c r="E80" s="8" t="s">
+      <c r="F80" s="9" t="s">
         <v>304</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>301</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="15" t="s">
+    <row r="81" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="12" t="s">
         <v>305</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="C81" s="8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D81" s="8"/>
+      <c r="C81" s="9" t="n">
+        <v>5400</v>
+      </c>
       <c r="E81" s="8" t="s">
         <v>307</v>
       </c>
+      <c r="F81" s="9" t="s">
+        <v>304</v>
+      </c>
       <c r="G81" s="4" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="15" t="s">
         <v>308</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="C82" s="11" t="n">
-        <v>7300</v>
-      </c>
-      <c r="D82" s="11"/>
+      <c r="C82" s="8" t="n">
+        <v>2811</v>
+      </c>
+      <c r="D82" s="8"/>
       <c r="E82" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="10" t="s">
+      <c r="B83" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="C83" s="11" t="n">
+        <v>7300</v>
+      </c>
+      <c r="D83" s="11"/>
+      <c r="E83" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="C83" s="8" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D83" s="8" t="s">
+      <c r="F83" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C84" s="8" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D84" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
       <c r="E84" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="8" t="s">
         <v>319</v>
       </c>
     </row>
@@ -4169,247 +4176,247 @@
         <v>320</v>
       </c>
       <c r="B85" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="C85" s="8" t="n">
-        <v>11</v>
-      </c>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8" t="s">
+      <c r="F85" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="C86" s="8" t="n">
+        <v>11</v>
+      </c>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="F86" s="8" t="s">
         <v>326</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="D87" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="E87" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="C87" s="8" t="n">
+      <c r="F87" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C88" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="D87" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="10" t="s">
+      <c r="D88" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="E88" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="C88" s="8" t="n">
+      <c r="F88" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="C89" s="8" t="n">
         <v>7500</v>
       </c>
-      <c r="D88" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>338</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="G88" s="4" t="s">
+      <c r="D89" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="G89" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="C89" s="8" t="n">
-        <v>6800</v>
-      </c>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="B90" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="C90" s="8" t="n">
+        <v>6800</v>
+      </c>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="C90" s="8" t="n">
+      <c r="F90" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C91" s="8" t="n">
         <v>1711</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="10" t="s">
+      <c r="D91" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="E91" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="8" t="s">
+      <c r="F91" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="F91" s="8"/>
-      <c r="G91" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
         <v>352</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C92" s="8" t="n">
-        <v>190</v>
-      </c>
-      <c r="D92" s="8" t="s">
         <v>353</v>
       </c>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
       <c r="E92" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="F92" s="8" t="s">
-        <v>355</v>
+      <c r="F92" s="8"/>
+      <c r="G92" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C93" s="8" t="n">
+        <v>190</v>
+      </c>
+      <c r="D93" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C93" s="8" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D93" s="8" t="s">
+      <c r="E93" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="E93" s="8" t="s">
+      <c r="F93" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="F93" s="8" t="s">
+    </row>
+    <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="10" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="94" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="10" t="s">
-        <v>360</v>
       </c>
       <c r="B94" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="8" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="E94" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="D94" s="14" t="s">
+      <c r="F94" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="E94" s="8" t="s">
+    </row>
+    <row r="95" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="10" t="s">
         <v>363</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="B95" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C95" s="11" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="10" t="s">
+      <c r="D95" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="E95" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="F95" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D95" s="11" t="s">
+    </row>
+    <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="E95" s="8" t="s">
+      <c r="B96" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="C96" s="11" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
+      <c r="D96" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="E96" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="C96" s="9" t="n">
+      <c r="F96" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="C97" s="9" t="n">
         <v>9100</v>
       </c>
-      <c r="E96" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
       <c r="E97" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="F97" s="8" t="s">
+      <c r="F97" s="9" t="s">
         <v>377</v>
       </c>
     </row>
@@ -4418,71 +4425,67 @@
         <v>378</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11" t="s">
+      <c r="F98" s="8" t="s">
         <v>380</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="F98" s="8" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="B99" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C99" s="8" t="n">
-        <v>900</v>
-      </c>
-      <c r="D99" s="8" t="s">
+      <c r="E99" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="E99" s="8" t="s">
+      <c r="F99" s="8" t="s">
         <v>385</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="8" t="n">
+        <v>900</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="D100" s="8" t="s">
+      <c r="F100" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="E100" s="8" t="s">
+    </row>
+    <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="F100" s="8" t="s">
+      <c r="B101" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="101" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="10" t="s">
+      <c r="D101" s="8" t="s">
         <v>392</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C101" s="8" t="n">
-        <v>500</v>
-      </c>
-      <c r="D101" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>393</v>
@@ -4491,152 +4494,155 @@
         <v>394</v>
       </c>
     </row>
-    <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
         <v>395</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="C102" s="8" t="n">
-        <v>1600</v>
-      </c>
-      <c r="D102" s="8"/>
+        <v>500</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="E102" s="8" t="s">
-        <v>47</v>
+        <v>396</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>48</v>
+        <v>397</v>
       </c>
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>313</v>
+        <v>46</v>
       </c>
       <c r="C103" s="8" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>314</v>
-      </c>
+        <v>1600</v>
+      </c>
+      <c r="D103" s="8"/>
       <c r="E103" s="8" t="s">
-        <v>315</v>
+        <v>47</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>316</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="C104" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>400</v>
+        <v>316</v>
+      </c>
+      <c r="C104" s="8" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>317</v>
       </c>
       <c r="E104" s="8" t="s">
-        <v>401</v>
+        <v>318</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>402</v>
+        <v>319</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="D105" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="E105" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="8" t="s">
+      <c r="F105" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="F105" s="9" t="s">
+    </row>
+    <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="10" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="106" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="12" t="s">
+      <c r="B106" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="B106" s="8" t="s">
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="C106" s="9" t="n">
-        <v>9700</v>
-      </c>
-      <c r="D106" s="3" t="s">
+      <c r="F106" s="9" t="s">
         <v>409</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="B107" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="C107" s="9" t="n">
+        <v>9700</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="E107" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C107" s="9" t="n">
-        <v>9800</v>
-      </c>
-      <c r="E107" s="9" t="s">
+      <c r="F107" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="s">
+    </row>
+    <row r="108" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="12" t="s">
         <v>415</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>416</v>
       </c>
       <c r="C108" s="9" t="n">
-        <v>9400</v>
-      </c>
-      <c r="D108" s="3" t="s">
+        <v>9800</v>
+      </c>
+      <c r="E108" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="E108" s="8" t="s">
-        <v>418</v>
-      </c>
       <c r="F108" s="2" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="C109" s="9" t="n">
+        <v>9400</v>
+      </c>
+      <c r="D109" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="C109" s="9" t="n">
-        <v>9500</v>
-      </c>
-      <c r="E109" s="16" t="s">
+      <c r="E109" s="8" t="s">
         <v>421</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4647,159 +4653,156 @@
         <v>423</v>
       </c>
       <c r="C110" s="9" t="n">
-        <v>9600</v>
-      </c>
-      <c r="E110" s="9" t="s">
+        <v>9500</v>
+      </c>
+      <c r="E110" s="16" t="s">
         <v>424</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="C111" s="9" t="n">
+        <v>9600</v>
+      </c>
+      <c r="E111" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="F111" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="10" t="s">
+      <c r="D112" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B112" s="8" t="s">
+      <c r="E112" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="8" t="s">
+      <c r="F112" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="F112" s="8" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>434</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>435</v>
       </c>
       <c r="C113" s="11"/>
       <c r="D113" s="11"/>
       <c r="E113" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="F113" s="8" t="s">
         <v>436</v>
-      </c>
-      <c r="F113" s="8" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="B114" s="8" t="s">
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="C114" s="8" t="n">
-        <v>131</v>
-      </c>
-      <c r="D114" s="8" t="s">
+      <c r="F114" s="8" t="s">
         <v>440</v>
-      </c>
-      <c r="E114" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="C115" s="8" t="n">
+        <v>131</v>
+      </c>
+      <c r="D115" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="E115" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="C115" s="8" t="n">
+      <c r="F115" s="8" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="C116" s="8" t="n">
         <v>132</v>
       </c>
-      <c r="D115" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>446</v>
-      </c>
-      <c r="F115" s="8" t="s">
+      <c r="D116" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="E116" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="F116" s="8" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="117" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="116" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="10" t="s">
+      <c r="C117" s="11" t="n">
+        <v>132</v>
+      </c>
+      <c r="D117" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="B116" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="C116" s="11" t="n">
-        <v>132</v>
-      </c>
-      <c r="D116" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="E116" s="8"/>
-      <c r="G116" s="4" t="s">
+      <c r="E117" s="8"/>
+      <c r="G117" s="4" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>450</v>
-      </c>
-      <c r="C117" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D117" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="E118" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="F118" s="8" t="s">
+      <c r="F118" s="2" t="s">
         <v>456</v>
       </c>
     </row>
@@ -4808,193 +4811,193 @@
         <v>457</v>
       </c>
       <c r="B119" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C119" s="8" t="n">
+        <v>1731</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="E119" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="C119" s="8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8" t="s">
+      <c r="F119" s="8" t="s">
         <v>459</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="B120" s="8" t="s">
+      <c r="C120" s="8" t="n">
+        <v>2811</v>
+      </c>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B121" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C120" s="8" t="n">
+      <c r="C121" s="8" t="n">
         <v>200</v>
       </c>
-      <c r="D120" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="E120" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="F120" s="8" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="15" t="s">
+      <c r="D121" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="B121" s="8" t="s">
+      <c r="E121" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="C121" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="D121" s="8" t="s">
+      <c r="F121" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="E121" s="8" t="s">
+    </row>
+    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="15" t="s">
         <v>468</v>
       </c>
-      <c r="F121" s="8" t="s">
+      <c r="B122" s="8" t="s">
         <v>469</v>
-      </c>
-    </row>
-    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="B122" s="8" t="s">
-        <v>466</v>
       </c>
       <c r="C122" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="E122" s="8" t="s">
         <v>471</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>469</v>
+      </c>
+      <c r="C123" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="F123" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="B123" s="8" t="s">
-        <v>473</v>
-      </c>
-      <c r="C123" s="8" t="n">
+    </row>
+    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="C124" s="8" t="n">
         <v>5500</v>
       </c>
-      <c r="D123" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="E123" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="124" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="10" t="s">
+      <c r="D124" s="8" t="s">
         <v>477</v>
       </c>
-      <c r="B124" s="8" t="s">
+      <c r="E124" s="8" t="s">
         <v>478</v>
       </c>
-      <c r="C124" s="8" t="n">
+      <c r="F124" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="125" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C125" s="8" t="n">
         <v>5600</v>
       </c>
-      <c r="D124" s="12" t="s">
-        <v>479</v>
-      </c>
-      <c r="E124" s="8" t="s">
-        <v>480</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="10" t="s">
+      <c r="D125" s="12" t="s">
         <v>482</v>
       </c>
-      <c r="B125" s="8" t="s">
+      <c r="E125" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="C125" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D125" s="8" t="s">
+      <c r="F125" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="E125" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="C126" s="8" t="n">
+        <v>101</v>
+      </c>
+      <c r="D126" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="E126" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="C126" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D126" s="8" t="s">
+      <c r="F126" s="2" t="s">
         <v>489</v>
-      </c>
-      <c r="E126" s="8" t="s">
-        <v>490</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C127" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D127" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="B127" s="8" t="s">
+      <c r="E127" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="8" t="s">
+      <c r="F127" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="F127" s="8" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
+        <v>495</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="C128" s="11"/>
+      <c r="D128" s="11"/>
+      <c r="E128" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="C128" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D128" s="8" t="s">
+      <c r="F128" s="8" t="s">
         <v>498</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="G128" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5005,29 +5008,31 @@
         <v>500</v>
       </c>
       <c r="C129" s="8" t="n">
-        <v>112</v>
+        <v>1000</v>
       </c>
       <c r="D129" s="8" t="s">
         <v>501</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="F129" s="8" t="s">
-        <v>503</v>
+        <v>388</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="C130" s="8" t="n">
+        <v>112</v>
+      </c>
+      <c r="D130" s="8" t="s">
         <v>504</v>
       </c>
-      <c r="B130" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C130" s="8" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D130" s="8"/>
       <c r="E130" s="8" t="s">
         <v>505</v>
       </c>
@@ -5040,453 +5045,455 @@
         <v>507</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>508</v>
+        <v>132</v>
       </c>
       <c r="C131" s="8" t="n">
-        <v>21</v>
+        <v>3100</v>
       </c>
       <c r="D131" s="8"/>
       <c r="E131" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="F131" s="8" t="s">
         <v>509</v>
-      </c>
-      <c r="F131" s="8" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="B132" s="8" t="s">
         <v>511</v>
       </c>
-      <c r="B132" s="8" t="s">
-        <v>285</v>
-      </c>
       <c r="C132" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="F132" s="8" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C133" s="8" t="n">
         <v>122</v>
       </c>
-      <c r="D132" s="8" t="s">
-        <v>512</v>
-      </c>
-      <c r="E132" s="8" t="s">
-        <v>513</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="133" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="10" t="s">
+      <c r="D133" s="8" t="s">
         <v>515</v>
       </c>
-      <c r="B133" s="8" t="s">
+      <c r="E133" s="8" t="s">
         <v>516</v>
       </c>
-      <c r="C133" s="8" t="n">
+      <c r="F133" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="134" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B134" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="C134" s="8" t="n">
         <v>1722</v>
       </c>
-      <c r="D133" s="12" t="s">
-        <v>517</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>518</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="10" t="s">
+      <c r="D134" s="12" t="s">
         <v>520</v>
       </c>
-      <c r="B134" s="8" t="s">
+      <c r="E134" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="C134" s="8" t="n">
-        <v>7100</v>
-      </c>
-      <c r="D134" s="12"/>
-      <c r="E134" s="8" t="s">
+      <c r="F134" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="G134" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="10" t="s">
         <v>523</v>
       </c>
       <c r="B135" s="8" t="s">
         <v>524</v>
       </c>
-      <c r="C135" s="11"/>
-      <c r="D135" s="11"/>
+      <c r="C135" s="8" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D135" s="12"/>
       <c r="E135" s="8" t="s">
         <v>525</v>
       </c>
-      <c r="F135" s="8"/>
       <c r="G135" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="s">
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="10" t="s">
         <v>526</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="C136" s="3" t="n">
-        <v>10900</v>
-      </c>
-      <c r="E136" s="2" t="s">
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="8" t="s">
         <v>528</v>
       </c>
-      <c r="F136" s="2" t="s">
-        <v>529</v>
+      <c r="F136" s="8"/>
+      <c r="G136" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="C137" s="3" t="n">
+        <v>10900</v>
+      </c>
+      <c r="E137" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="E137" s="2" t="s">
+      <c r="F137" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="F137" s="8" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="E138" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="F138" s="8" t="s">
         <v>536</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="F138" s="8" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="D139" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="E139" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="E139" s="2" t="s">
+      <c r="F139" s="8" t="s">
         <v>541</v>
       </c>
-      <c r="F139" s="8" t="s">
+    </row>
+    <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="10" t="s">
+      <c r="B140" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="B140" s="8" t="s">
+      <c r="E140" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="C140" s="3"/>
-      <c r="E140" s="8" t="s">
+      <c r="F140" s="8" t="s">
         <v>545</v>
-      </c>
-      <c r="F140" s="9" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="B141" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B141" s="8" t="s">
+      <c r="C141" s="3"/>
+      <c r="E141" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="8" t="s">
+      <c r="F141" s="9" t="s">
         <v>549</v>
-      </c>
-      <c r="F141" s="8" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="B142" s="8" t="s">
         <v>551</v>
-      </c>
-      <c r="B142" s="8" t="s">
-        <v>552</v>
       </c>
       <c r="C142" s="11"/>
       <c r="D142" s="11"/>
       <c r="E142" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="F142" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="F142" s="8" t="s">
+    </row>
+    <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="10" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="143" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="12" t="s">
+      <c r="B143" s="8" t="s">
         <v>555</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
+      <c r="E143" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="C143" s="3" t="n">
+      <c r="F143" s="8" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="144" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C144" s="3" t="n">
         <v>10500</v>
       </c>
-      <c r="D143" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="s">
+      <c r="D144" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="B144" s="8" t="s">
+      <c r="E144" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="C144" s="9" t="n">
+      <c r="F144" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="C145" s="9" t="n">
         <v>133</v>
-      </c>
-      <c r="E144" s="8" t="s">
-        <v>562</v>
-      </c>
-      <c r="F144" s="9" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C145" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D145" s="8" t="s">
-        <v>327</v>
       </c>
       <c r="E145" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="F145" s="8" t="s">
+      <c r="F145" s="9" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
+    <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="10" t="s">
         <v>567</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>568</v>
+        <v>328</v>
       </c>
       <c r="C146" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E146" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="F146" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="F146" s="8"/>
-      <c r="G146" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
         <v>570</v>
       </c>
       <c r="B147" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="C147" s="9" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D147" s="9" t="s">
+      <c r="C147" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D147" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E147" s="8" t="s">
         <v>572</v>
       </c>
-      <c r="E147" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="F147" s="8" t="s">
-        <v>574</v>
+      <c r="F147" s="8"/>
+      <c r="G147" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="C148" s="9" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D148" s="9" t="s">
         <v>575</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="E148" s="8" t="s">
         <v>576</v>
       </c>
-      <c r="C148" s="3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D148" s="3" t="s">
+      <c r="F148" s="8" t="s">
         <v>577</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="F148" s="2" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="C149" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="D149" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="B149" s="8" t="s">
+      <c r="E149" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="E149" s="8" t="s">
+      <c r="F149" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="F149" s="9" t="s">
+    </row>
+    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="10" t="s">
+      <c r="B150" s="8" t="s">
         <v>584</v>
       </c>
-      <c r="B150" s="8" t="s">
+      <c r="E150" s="8" t="s">
         <v>585</v>
       </c>
-      <c r="C150" s="8" t="s">
+      <c r="F150" s="9" t="s">
         <v>586</v>
-      </c>
-      <c r="D150" s="8" t="s">
-        <v>587</v>
-      </c>
-      <c r="E150" s="8" t="s">
-        <v>588</v>
-      </c>
-      <c r="F150" s="8" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>588</v>
+      </c>
+      <c r="C151" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="D151" s="8" t="s">
         <v>590</v>
       </c>
-      <c r="B151" s="8" t="s">
+      <c r="E151" s="8" t="s">
         <v>591</v>
       </c>
-      <c r="C151" s="11" t="s">
+      <c r="F151" s="8" t="s">
         <v>592</v>
-      </c>
-      <c r="D151" s="11" t="s">
-        <v>593</v>
-      </c>
-      <c r="E151" s="8" t="s">
-        <v>594</v>
-      </c>
-      <c r="F151" s="8" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
+        <v>593</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>594</v>
+      </c>
+      <c r="C152" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="D152" s="11" t="s">
         <v>596</v>
       </c>
-      <c r="B152" s="8" t="s">
+      <c r="E152" s="8" t="s">
         <v>597</v>
       </c>
-      <c r="C152" s="8" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D152" s="8"/>
-      <c r="E152" s="8" t="s">
+      <c r="F152" s="8" t="s">
         <v>598</v>
-      </c>
-      <c r="F152" s="8" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
+        <v>599</v>
+      </c>
+      <c r="B153" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="B153" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C153" s="11"/>
-      <c r="D153" s="11" t="s">
+      <c r="C153" s="8" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D153" s="8"/>
+      <c r="E153" s="8" t="s">
         <v>601</v>
       </c>
-      <c r="E153" s="8" t="s">
+      <c r="F153" s="8" t="s">
         <v>602</v>
-      </c>
-      <c r="F153" s="8" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C154" s="11"/>
+      <c r="D154" s="11" t="s">
         <v>604</v>
       </c>
-      <c r="B154" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C154" s="8" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D154" s="8" t="s">
+      <c r="E154" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="E154" s="8" t="s">
+      <c r="F154" s="8" t="s">
         <v>606</v>
-      </c>
-      <c r="F154" s="8" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
+        <v>607</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C155" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D155" s="8" t="s">
         <v>608</v>
       </c>
-      <c r="B155" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11"/>
       <c r="E155" s="8" t="s">
         <v>609</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>611</v>
+        <v>264</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
@@ -5494,7 +5501,7 @@
         <v>612</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5510,15 +5517,15 @@
         <v>615</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
+        <v>616</v>
+      </c>
+      <c r="B158" s="8" t="s">
         <v>617</v>
-      </c>
-      <c r="B158" s="8" t="s">
-        <v>614</v>
       </c>
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
@@ -5534,279 +5541,275 @@
         <v>620</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C159" s="11"/>
       <c r="D159" s="11"/>
       <c r="E159" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="F159" s="8" t="s">
         <v>622</v>
-      </c>
-      <c r="F159" s="8" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
+        <v>623</v>
+      </c>
+      <c r="B160" s="8" t="s">
         <v>624</v>
       </c>
-      <c r="B160" s="8" t="s">
+      <c r="C160" s="11"/>
+      <c r="D160" s="11"/>
+      <c r="E160" s="8" t="s">
         <v>625</v>
       </c>
-      <c r="C160" s="8" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D160" s="8" t="s">
+      <c r="F160" s="8" t="s">
         <v>626</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>627</v>
-      </c>
-      <c r="F160" s="8" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
+        <v>627</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="C161" s="8" t="n">
+        <v>7700</v>
+      </c>
+      <c r="D161" s="8" t="s">
         <v>629</v>
       </c>
-      <c r="B161" s="8" t="s">
+      <c r="E161" s="8" t="s">
         <v>630</v>
       </c>
-      <c r="C161" s="8" t="n">
+      <c r="F161" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="C162" s="8" t="n">
         <v>7800</v>
       </c>
-      <c r="D161" s="8" t="s">
+      <c r="D162" s="8" t="s">
+        <v>634</v>
+      </c>
+      <c r="E162" s="8" t="s">
+        <v>635</v>
+      </c>
+      <c r="F162" s="8" t="s">
         <v>631</v>
       </c>
-      <c r="E161" s="8" t="s">
-        <v>632</v>
-      </c>
-      <c r="F161" s="8" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="162" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="B162" s="17" t="s">
-        <v>634</v>
-      </c>
-      <c r="C162" s="14" t="n">
+    </row>
+    <row r="163" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B163" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="C163" s="14" t="n">
         <v>10300</v>
       </c>
-      <c r="D162" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="F162" s="2" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="10" t="s">
+      <c r="D163" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="E163" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="C163" s="11"/>
-      <c r="D163" s="11"/>
-      <c r="E163" s="8" t="s">
+      <c r="F163" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="F163" s="8" t="s">
+    </row>
+    <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="10" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="s">
+      <c r="B164" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="B164" s="8" t="s">
+      <c r="C164" s="11"/>
+      <c r="D164" s="11"/>
+      <c r="E164" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="C164" s="9" t="n">
+      <c r="F164" s="8" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="C165" s="9" t="n">
         <v>8900</v>
       </c>
-      <c r="E164" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="G164" s="4" t="s">
+      <c r="E165" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="G165" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="10" t="s">
-        <v>645</v>
-      </c>
-      <c r="B165" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C165" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="D165" s="11" t="s">
-        <v>646</v>
-      </c>
-      <c r="E165" s="8" t="s">
-        <v>647</v>
-      </c>
-      <c r="F165" s="8" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
+        <v>648</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C166" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D166" s="11" t="s">
         <v>649</v>
       </c>
-      <c r="B166" s="8" t="s">
+      <c r="E166" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="C166" s="11"/>
-      <c r="D166" s="11" t="s">
+      <c r="F166" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="E166" s="8" t="s">
+    </row>
+    <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="10" t="s">
         <v>652</v>
       </c>
-      <c r="F166" s="8" t="s">
+      <c r="B167" s="8" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="167" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="10" t="s">
+      <c r="C167" s="11"/>
+      <c r="D167" s="11" t="s">
         <v>654</v>
       </c>
-      <c r="B167" s="8" t="s">
-        <v>483</v>
-      </c>
-      <c r="C167" s="8" t="n">
+      <c r="E167" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="F167" s="8" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="168" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="C168" s="8" t="n">
         <v>101</v>
       </c>
-      <c r="D167" s="12" t="s">
-        <v>484</v>
-      </c>
-      <c r="E167" s="8" t="s">
-        <v>485</v>
-      </c>
-      <c r="F167" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="10" t="s">
-        <v>655</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="C168" s="11"/>
-      <c r="D168" s="11"/>
+      <c r="D168" s="12" t="s">
+        <v>487</v>
+      </c>
       <c r="E168" s="8" t="s">
-        <v>656</v>
-      </c>
-      <c r="F168" s="8"/>
-      <c r="G168" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>488</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>288</v>
       </c>
       <c r="C169" s="11"/>
-      <c r="D169" s="11" t="s">
-        <v>658</v>
-      </c>
+      <c r="D169" s="11"/>
       <c r="E169" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="F169" s="8" t="s">
-        <v>660</v>
+      <c r="F169" s="8"/>
+      <c r="G169" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
+        <v>660</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C170" s="11"/>
+      <c r="D170" s="11" t="s">
         <v>661</v>
       </c>
-      <c r="B170" s="8" t="s">
+      <c r="E170" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="F170" s="8" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="B171" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="C170" s="8" t="n">
+      <c r="C171" s="8" t="n">
         <v>1400</v>
       </c>
-      <c r="D170" s="8" t="s">
-        <v>662</v>
-      </c>
-      <c r="E170" s="8" t="s">
+      <c r="D171" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="E171" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="F171" s="8" t="s">
         <v>663</v>
       </c>
-      <c r="F170" s="8" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="B171" s="8" t="s">
-        <v>665</v>
-      </c>
-      <c r="C171" s="8" t="n">
+    </row>
+    <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C172" s="8" t="n">
         <v>7400</v>
       </c>
-      <c r="D171" s="8" t="s">
-        <v>666</v>
-      </c>
-      <c r="E171" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="F171" s="8" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="10" t="s">
+      <c r="D172" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="B172" s="8" t="s">
+      <c r="E172" s="8" t="s">
         <v>670</v>
       </c>
-      <c r="C172" s="11"/>
-      <c r="D172" s="11" t="s">
+      <c r="F172" s="8" t="s">
         <v>671</v>
-      </c>
-      <c r="E172" s="8" t="s">
-        <v>672</v>
-      </c>
-      <c r="F172" s="8" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="B173" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="B173" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="C173" s="8" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D173" s="8" t="s">
+      <c r="C173" s="11"/>
+      <c r="D173" s="11" t="s">
         <v>674</v>
       </c>
       <c r="E173" s="8" t="s">
         <v>675</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5814,27 +5817,33 @@
         <v>676</v>
       </c>
       <c r="B174" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="C174" s="8" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D174" s="8" t="s">
         <v>677</v>
       </c>
-      <c r="C174" s="8" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D174" s="8" t="s">
+      <c r="E174" s="8" t="s">
         <v>678</v>
       </c>
-      <c r="E174" s="8" t="s">
-        <v>679</v>
-      </c>
       <c r="F174" s="8" t="s">
-        <v>680</v>
+        <v>663</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="C175" s="8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D175" s="8" t="s">
         <v>681</v>
-      </c>
-      <c r="B175" s="8" t="s">
-        <v>288</v>
       </c>
       <c r="E175" s="8" t="s">
         <v>682</v>
@@ -5848,111 +5857,109 @@
         <v>684</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C176" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="E176" s="8" t="s">
         <v>685</v>
       </c>
-      <c r="D176" s="11" t="s">
+      <c r="F176" s="8" t="s">
         <v>686</v>
-      </c>
-      <c r="E176" s="8" t="s">
-        <v>687</v>
-      </c>
-      <c r="F176" s="8" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C177" s="11" t="s">
         <v>688</v>
       </c>
-      <c r="B177" s="8" t="s">
-        <v>670</v>
-      </c>
-      <c r="C177" s="11"/>
-      <c r="D177" s="11"/>
+      <c r="D177" s="11" t="s">
+        <v>689</v>
+      </c>
       <c r="E177" s="8" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>614</v>
+        <v>673</v>
       </c>
       <c r="C178" s="11"/>
-      <c r="D178" s="11" t="s">
-        <v>691</v>
-      </c>
+      <c r="D178" s="11"/>
       <c r="E178" s="8" t="s">
         <v>692</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
+      <c r="A179" s="10" t="s">
         <v>693</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="C179" s="11"/>
+      <c r="D179" s="11" t="s">
         <v>694</v>
       </c>
-      <c r="D179" s="3" t="s">
+      <c r="E179" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="E179" s="2" t="s">
+      <c r="F179" s="8" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="F179" s="2" t="s">
+      <c r="B180" s="2" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="180" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="s">
+      <c r="D180" s="3" t="s">
         <v>698</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="E180" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="C180" s="14" t="n">
+      <c r="F180" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="181" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C181" s="14" t="n">
         <v>10100</v>
       </c>
-      <c r="E180" s="2" t="s">
-        <v>700</v>
-      </c>
-      <c r="F180" s="2" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="10" t="s">
-        <v>702</v>
-      </c>
-      <c r="B181" s="8" t="s">
+      <c r="E181" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="C181" s="11"/>
-      <c r="D181" s="11"/>
-      <c r="E181" s="8" t="s">
+      <c r="F181" s="2" t="s">
         <v>704</v>
-      </c>
-      <c r="F181" s="8" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
+        <v>705</v>
+      </c>
+      <c r="B182" s="8" t="s">
         <v>706</v>
-      </c>
-      <c r="B182" s="8" t="s">
-        <v>670</v>
       </c>
       <c r="C182" s="11"/>
       <c r="D182" s="11"/>
@@ -5960,41 +5967,39 @@
         <v>707</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>614</v>
+        <v>673</v>
       </c>
       <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="8" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>264</v>
+        <v>617</v>
       </c>
       <c r="C184" s="11"/>
-      <c r="D184" s="11" t="s">
-        <v>711</v>
-      </c>
+      <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
         <v>712</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6002,65 +6007,65 @@
         <v>713</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>206</v>
+        <v>264</v>
       </c>
       <c r="C185" s="11"/>
-      <c r="D185" s="11"/>
+      <c r="D185" s="11" t="s">
+        <v>714</v>
+      </c>
       <c r="E185" s="8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C186" s="11"/>
       <c r="D186" s="11"/>
       <c r="E186" s="8" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>288</v>
+        <v>209</v>
       </c>
       <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>614</v>
+        <v>291</v>
       </c>
       <c r="C188" s="11"/>
-      <c r="D188" s="11" t="s">
-        <v>720</v>
-      </c>
+      <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
         <v>721</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6068,114 +6073,114 @@
         <v>722</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>206</v>
+        <v>617</v>
       </c>
       <c r="C189" s="11"/>
-      <c r="D189" s="11"/>
+      <c r="D189" s="11" t="s">
+        <v>723</v>
+      </c>
       <c r="E189" s="8" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C190" s="11"/>
       <c r="D190" s="11"/>
       <c r="E190" s="8" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>288</v>
+        <v>209</v>
       </c>
       <c r="C191" s="11"/>
       <c r="D191" s="11"/>
       <c r="E191" s="8" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="C192" s="11"/>
       <c r="D192" s="11"/>
       <c r="E192" s="8" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>670</v>
+        <v>264</v>
       </c>
       <c r="C193" s="11"/>
       <c r="D193" s="11"/>
       <c r="E193" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="1" t="s">
-        <v>732</v>
+      <c r="A194" s="10" t="s">
+        <v>733</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>733</v>
-      </c>
-      <c r="C194" s="9" t="n">
-        <v>23</v>
-      </c>
+        <v>673</v>
+      </c>
+      <c r="C194" s="11"/>
+      <c r="D194" s="11"/>
       <c r="E194" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="F194" s="9" t="s">
+      <c r="F194" s="8" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="10" t="s">
+      <c r="B195" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="B195" s="8" t="s">
+      <c r="C195" s="9" t="n">
+        <v>23</v>
+      </c>
+      <c r="E195" s="8" t="s">
         <v>737</v>
       </c>
-      <c r="C195" s="8" t="n">
-        <v>121</v>
-      </c>
-      <c r="D195" s="8"/>
-      <c r="E195" s="8" t="s">
+      <c r="F195" s="9" t="s">
         <v>738</v>
-      </c>
-      <c r="G195" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6185,124 +6190,126 @@
       <c r="B196" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="C196" s="11"/>
-      <c r="D196" s="11" t="s">
+      <c r="C196" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="D196" s="8"/>
+      <c r="E196" s="8" t="s">
         <v>741</v>
       </c>
-      <c r="E196" s="8" t="s">
-        <v>742</v>
-      </c>
-      <c r="F196" s="8" t="s">
-        <v>743</v>
+      <c r="G196" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C197" s="11"/>
       <c r="D197" s="11" t="s">
+        <v>744</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>745</v>
+      </c>
+      <c r="F197" s="8" t="s">
         <v>746</v>
-      </c>
-      <c r="E197" s="8" t="s">
-        <v>747</v>
-      </c>
-      <c r="F197" s="8" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
+        <v>747</v>
+      </c>
+      <c r="B198" s="8" t="s">
         <v>748</v>
       </c>
-      <c r="B198" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="C198" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D198" s="8" t="s">
-        <v>489</v>
+      <c r="C198" s="11"/>
+      <c r="D198" s="11" t="s">
+        <v>749</v>
       </c>
       <c r="E198" s="8" t="s">
-        <v>490</v>
-      </c>
-      <c r="F198" s="2" t="s">
-        <v>491</v>
+        <v>750</v>
+      </c>
+      <c r="F198" s="8" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>345</v>
+        <v>491</v>
       </c>
       <c r="C199" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D199" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="E199" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C200" s="8" t="n">
         <v>1711</v>
       </c>
-      <c r="D199" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="E199" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="F199" s="8" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="B200" s="8" t="s">
-        <v>751</v>
-      </c>
-      <c r="C200" s="8" t="n">
+      <c r="D200" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="E200" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="F200" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>754</v>
+      </c>
+      <c r="C201" s="8" t="n">
         <v>3300</v>
       </c>
-      <c r="D200" s="8" t="s">
-        <v>752</v>
-      </c>
-      <c r="E200" s="8" t="s">
-        <v>753</v>
-      </c>
-      <c r="F200" s="8" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="10" t="s">
+      <c r="D201" s="8" t="s">
         <v>755</v>
       </c>
-      <c r="B201" s="8" t="s">
+      <c r="E201" s="8" t="s">
         <v>756</v>
       </c>
-      <c r="C201" s="8" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D201" s="8" t="s">
+      <c r="F201" s="8" t="s">
         <v>757</v>
-      </c>
-      <c r="E201" s="8" t="s">
-        <v>758</v>
-      </c>
-      <c r="F201" s="8" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="C202" s="8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D202" s="8" t="s">
         <v>760</v>
       </c>
-      <c r="B202" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C202" s="11"/>
-      <c r="D202" s="11"/>
       <c r="E202" s="8" t="s">
         <v>761</v>
       </c>
@@ -6315,7 +6322,7 @@
         <v>763</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C203" s="11"/>
       <c r="D203" s="11"/>
@@ -6323,63 +6330,61 @@
         <v>764</v>
       </c>
       <c r="F203" s="8" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>285</v>
+        <v>209</v>
       </c>
       <c r="C204" s="11"/>
-      <c r="D204" s="11" t="s">
-        <v>766</v>
-      </c>
+      <c r="D204" s="11"/>
       <c r="E204" s="8" t="s">
         <v>767</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="205" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
         <v>768</v>
       </c>
       <c r="B205" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C205" s="11"/>
+      <c r="D205" s="11" t="s">
+        <v>769</v>
+      </c>
+      <c r="E205" s="8" t="s">
+        <v>770</v>
+      </c>
+      <c r="F205" s="8" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="206" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="10" t="s">
+        <v>771</v>
+      </c>
+      <c r="B206" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C205" s="8" t="n">
+      <c r="C206" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="D205" s="12" t="s">
+      <c r="D206" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="E205" s="8" t="s">
-        <v>769</v>
-      </c>
-      <c r="F205" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="10" t="s">
-        <v>770</v>
-      </c>
-      <c r="B206" s="8" t="s">
-        <v>771</v>
-      </c>
-      <c r="C206" s="8" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D206" s="8"/>
       <c r="E206" s="8" t="s">
         <v>772</v>
       </c>
-      <c r="G206" s="4" t="s">
-        <v>95</v>
+      <c r="F206" s="8" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,7 +6395,7 @@
         <v>774</v>
       </c>
       <c r="C207" s="8" t="n">
-        <v>2711</v>
+        <v>2611</v>
       </c>
       <c r="D207" s="8"/>
       <c r="E207" s="8" t="s">
@@ -6400,105 +6405,109 @@
         <v>95</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
         <v>776</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C208" s="11"/>
-      <c r="D208" s="11"/>
+        <v>777</v>
+      </c>
+      <c r="C208" s="8" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D208" s="8"/>
       <c r="E208" s="8" t="s">
-        <v>777</v>
-      </c>
-      <c r="F208" s="8"/>
+        <v>778</v>
+      </c>
       <c r="G208" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>779</v>
+        <v>264</v>
       </c>
       <c r="C209" s="11"/>
-      <c r="D209" s="11" t="s">
+      <c r="D209" s="11"/>
+      <c r="E209" s="8" t="s">
         <v>780</v>
       </c>
-      <c r="E209" s="8" t="s">
-        <v>781</v>
-      </c>
-      <c r="F209" s="8" t="s">
-        <v>782</v>
+      <c r="F209" s="8"/>
+      <c r="G209" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="10" t="s">
+        <v>781</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>782</v>
+      </c>
+      <c r="C210" s="11"/>
+      <c r="D210" s="11" t="s">
         <v>783</v>
       </c>
-      <c r="B210" s="8" t="s">
+      <c r="E210" s="8" t="s">
         <v>784</v>
       </c>
-      <c r="C210" s="8" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D210" s="8"/>
-      <c r="E210" s="8" t="s">
+      <c r="F210" s="8" t="s">
         <v>785</v>
-      </c>
-      <c r="F210" s="8" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="B211" s="8" t="s">
         <v>787</v>
       </c>
-      <c r="B211" s="8" t="s">
-        <v>614</v>
-      </c>
       <c r="C211" s="8" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D211" s="8" t="s">
+        <v>3721</v>
+      </c>
+      <c r="D211" s="8"/>
+      <c r="E211" s="8" t="s">
         <v>788</v>
       </c>
-      <c r="E211" s="8" t="s">
+      <c r="F211" s="8" t="s">
         <v>789</v>
-      </c>
-      <c r="F211" s="8" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="C212" s="8" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D212" s="8" t="s">
         <v>791</v>
       </c>
-      <c r="B212" s="8" t="s">
+      <c r="E212" s="8" t="s">
         <v>792</v>
       </c>
-      <c r="C212" s="11" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D212" s="11" t="s">
+      <c r="F212" s="8" t="s">
         <v>793</v>
-      </c>
-      <c r="E212" s="8" t="s">
-        <v>794</v>
-      </c>
-      <c r="F212" s="8" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="C213" s="11" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D213" s="11" t="s">
         <v>796</v>
-      </c>
-      <c r="B213" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="E213" s="8" t="s">
         <v>797</v>
@@ -6507,62 +6516,60 @@
         <v>798</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="1" t="s">
+    <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="10" t="s">
         <v>799</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="C214" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D214" s="8" t="s">
-        <v>327</v>
+        <v>59</v>
       </c>
       <c r="E214" s="8" t="s">
         <v>800</v>
       </c>
-      <c r="F214" s="8"/>
-      <c r="G214" s="4" t="s">
-        <v>95</v>
+      <c r="F214" s="8" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>568</v>
+        <v>328</v>
       </c>
       <c r="C215" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D215" s="8" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E215" s="8" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F215" s="8"/>
       <c r="G215" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="216" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="10" t="s">
-        <v>803</v>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>804</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C216" s="11"/>
-      <c r="D216" s="11"/>
+        <v>571</v>
+      </c>
+      <c r="C216" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D216" s="8" t="s">
+        <v>330</v>
+      </c>
       <c r="E216" s="8" t="s">
-        <v>804</v>
-      </c>
-      <c r="F216" s="8" t="s">
         <v>805</v>
+      </c>
+      <c r="F216" s="8"/>
+      <c r="G216" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="217" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6570,30 +6577,46 @@
         <v>806</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="C217" s="8" t="n">
-        <v>21</v>
-      </c>
-      <c r="D217" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C217" s="11"/>
+      <c r="D217" s="11"/>
       <c r="E217" s="8" t="s">
         <v>807</v>
       </c>
-      <c r="G217" s="4" t="s">
+      <c r="F217" s="8" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="218" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="10" t="s">
+        <v>809</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="C218" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="D218" s="8"/>
+      <c r="E218" s="8" t="s">
+        <v>810</v>
+      </c>
+      <c r="G218" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="B218" s="8" t="s">
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B219" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="E218" s="8" t="s">
-        <v>809</v>
-      </c>
-      <c r="F218" s="8"/>
+      <c r="E219" s="8" t="s">
+        <v>812</v>
+      </c>
+      <c r="F219" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed PDF 1.4 - 1.6 (Acrobat 5 - 8) regex (#25)
https://hashcat.net/trac/ticket/594
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -1709,7 +1709,7 @@
     <t>PDF 1.4 - 1.6 (Acrobat 5 - 8)</t>
   </si>
   <si>
-    <t>^\$pdf\$2\*3\*128\*[0-9-]{1,5}\*1\*16\*[a-f0-9]{32}\*32\*[a-f0-9]{64}\*(8|16|32)\*[a-f0-9]{16,64}$/i</t>
+    <t>^\$pdf\$[24]\*[34]\*128\*[0-9-]{1,5}\*1\*(16|32)\*[a-f0-9]{32,64}\*32\*[a-f0-9]{64}\*(8|16|32)\*[a-f0-9]{16,64}$/i</t>
   </si>
   <si>
     <t>pdf</t>
@@ -2656,8 +2656,8 @@
   </sheetPr>
   <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3340,7 +3340,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Fixed PostgreSQL regex & hashcat mode
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -1766,10 +1766,10 @@
     <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/PHPS_fmt_plug.c</t>
   </si>
   <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>^(\$postgres\$.[^\*]+[*:])?[a-f0-9]{1,32}[*:][a-f0-9]{32}$/i</t>
+    <t>PostgreSQL Challenge-Response Auth</t>
+  </si>
+  <si>
+    <t>^\$postgres\$.[^\*]+[*:][a-f0-9]{1,32}[*:][a-f0-9]{32}$/i</t>
   </si>
   <si>
     <t>postgres</t>
@@ -2656,8 +2656,8 @@
   </sheetPr>
   <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A123" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2918,7 +2918,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
@@ -2934,6 +2934,7 @@
       <c r="F13" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
@@ -2973,7 +2974,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
@@ -2989,6 +2990,7 @@
       <c r="F16" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -3340,7 +3342,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
@@ -3356,6 +3358,7 @@
       <c r="F37" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="G37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
@@ -3403,6 +3406,7 @@
       <c r="B40" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="C40" s="3"/>
       <c r="E40" s="2" t="s">
         <v>162</v>
       </c>
@@ -3417,6 +3421,7 @@
       <c r="B41" s="8" t="s">
         <v>165</v>
       </c>
+      <c r="C41" s="3"/>
       <c r="E41" s="8" t="s">
         <v>166</v>
       </c>
@@ -3431,6 +3436,7 @@
       <c r="B42" s="8" t="s">
         <v>169</v>
       </c>
+      <c r="C42" s="3"/>
       <c r="E42" s="8" t="s">
         <v>170</v>
       </c>
@@ -3445,6 +3451,7 @@
       <c r="B43" s="8" t="s">
         <v>173</v>
       </c>
+      <c r="C43" s="3"/>
       <c r="E43" s="8" t="s">
         <v>174</v>
       </c>
@@ -3459,6 +3466,7 @@
       <c r="B44" s="8" t="s">
         <v>177</v>
       </c>
+      <c r="C44" s="3"/>
       <c r="E44" s="8" t="s">
         <v>178</v>
       </c>
@@ -3924,6 +3932,7 @@
       <c r="B70" s="8" t="s">
         <v>269</v>
       </c>
+      <c r="C70" s="3"/>
       <c r="E70" s="2" t="s">
         <v>270</v>
       </c>
@@ -4711,7 +4720,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
         <v>433</v>
       </c>
@@ -4727,6 +4736,7 @@
       <c r="F113" s="2" t="s">
         <v>437</v>
       </c>
+      <c r="G113" s="1"/>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
@@ -5207,6 +5217,7 @@
       <c r="B139" s="2" t="s">
         <v>539</v>
       </c>
+      <c r="C139" s="3"/>
       <c r="E139" s="2" t="s">
         <v>540</v>
       </c>
@@ -5214,7 +5225,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>542</v>
       </c>
@@ -5230,6 +5241,7 @@
       <c r="F140" s="8" t="s">
         <v>546</v>
       </c>
+      <c r="G140" s="1"/>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
@@ -5238,6 +5250,7 @@
       <c r="B141" s="2" t="s">
         <v>548</v>
       </c>
+      <c r="C141" s="3"/>
       <c r="E141" s="2" t="s">
         <v>549</v>
       </c>
@@ -5390,15 +5403,15 @@
         <v>582</v>
       </c>
     </row>
-    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
         <v>583</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="C150" s="3" t="n">
-        <v>12</v>
+      <c r="C150" s="14" t="n">
+        <v>11100</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>585</v>
@@ -5417,6 +5430,7 @@
       <c r="B151" s="8" t="s">
         <v>589</v>
       </c>
+      <c r="C151" s="3"/>
       <c r="E151" s="8" t="s">
         <v>590</v>
       </c>
@@ -5891,6 +5905,7 @@
       <c r="B177" s="8" t="s">
         <v>296</v>
       </c>
+      <c r="C177" s="3"/>
       <c r="E177" s="8" t="s">
         <v>690</v>
       </c>
@@ -5952,7 +5967,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
         <v>701</v>
       </c>
@@ -5968,6 +5983,7 @@
       <c r="F181" s="2" t="s">
         <v>705</v>
       </c>
+      <c r="G181" s="1"/>
     </row>
     <row r="182" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
@@ -6555,6 +6571,7 @@
       <c r="B215" s="8" t="s">
         <v>59</v>
       </c>
+      <c r="C215" s="3"/>
       <c r="E215" s="8" t="s">
         <v>805</v>
       </c>

</xml_diff>

<commit_message>
Added MySQL Challenge-Response Authentication
</commit_message>
<xml_diff>
--- a/doc/hashinfo.xlsx
+++ b/doc/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="822">
   <si>
     <t>Hash</t>
   </si>
@@ -1424,6 +1424,18 @@
     <t>http://community.mybb.com/post-555267.html</t>
   </si>
   <si>
+    <t>MySQL Challenge-Response Auth (SHA1)</t>
+  </si>
+  <si>
+    <t>^\$mysqlna\$[a-f0-9]{40}[:*][a-f0-9]{40}$/i</t>
+  </si>
+  <si>
+    <t>$mysqlna$1c24ab8d0ee94d70ab1f2e814d8f0948a14d10b9*437e93572f18ae44d9e779160c2505271f85821d</t>
+  </si>
+  <si>
+    <t>https://hashcat.net/trac/ticket/541</t>
+  </si>
+  <si>
     <t>MySQL323</t>
   </si>
   <si>
@@ -1766,7 +1778,7 @@
     <t>https://github.com/magnumripper/JohnTheRipper/blob/bleeding-jumbo/src/PHPS_fmt_plug.c</t>
   </si>
   <si>
-    <t>PostgreSQL Challenge-Response Auth</t>
+    <t>PostgreSQL Challenge-Response Auth (MD5)</t>
   </si>
   <si>
     <t>^\$postgres\$.[^\*]+[*:][a-f0-9]{1,32}[*:][a-f0-9]{32}$/i</t>
@@ -2654,10 +2666,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G220"/>
+  <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A114" activeCellId="0" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2918,7 +2930,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
@@ -2934,7 +2946,6 @@
       <c r="F13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="1"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
@@ -2974,7 +2985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
@@ -2990,7 +3001,6 @@
       <c r="F16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="1"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -3342,7 +3352,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
@@ -3358,7 +3368,6 @@
       <c r="F37" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
@@ -4720,7 +4729,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
         <v>433</v>
       </c>
@@ -4736,7 +4745,6 @@
       <c r="F113" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="G113" s="1"/>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
@@ -4886,159 +4894,160 @@
         <v>468</v>
       </c>
     </row>
-    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="10" t="s">
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C122" s="3" t="n">
+        <v>11200</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="B123" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C122" s="8" t="n">
+      <c r="C123" s="8" t="n">
         <v>200</v>
       </c>
-      <c r="D122" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="E122" s="8" t="s">
-        <v>471</v>
-      </c>
-      <c r="F122" s="8" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="15" t="s">
-        <v>473</v>
-      </c>
-      <c r="B123" s="8" t="s">
+      <c r="D123" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="C123" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="D123" s="8" t="s">
+      <c r="E123" s="8" t="s">
         <v>475</v>
       </c>
-      <c r="E123" s="8" t="s">
+      <c r="F123" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="F123" s="8" t="s">
+    </row>
+    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="15" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="10" t="s">
+      <c r="B124" s="8" t="s">
         <v>478</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>474</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C125" s="8" t="n">
-        <v>5500</v>
+        <v>300</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E125" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="F125" s="2" t="s">
+      <c r="F125" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="10" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="126" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="10" t="s">
+      <c r="B126" s="8" t="s">
         <v>485</v>
       </c>
-      <c r="B126" s="8" t="s">
+      <c r="C126" s="8" t="n">
+        <v>5500</v>
+      </c>
+      <c r="D126" s="8" t="s">
         <v>486</v>
       </c>
-      <c r="C126" s="8" t="n">
+      <c r="E126" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="127" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="C127" s="8" t="n">
         <v>5600</v>
       </c>
-      <c r="D126" s="12" t="s">
-        <v>487</v>
-      </c>
-      <c r="E126" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="B127" s="8" t="s">
+      <c r="D127" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="C127" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D127" s="8" t="s">
+      <c r="E127" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="E127" s="8" t="s">
+      <c r="F127" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="B128" s="8" t="s">
+      <c r="C128" s="8" t="n">
+        <v>101</v>
+      </c>
+      <c r="D128" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="C128" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D128" s="8" t="s">
+      <c r="E128" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="E128" s="8" t="s">
+      <c r="F128" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="C129" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D129" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
       <c r="E129" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="F129" s="8" t="s">
+      <c r="F129" s="2" t="s">
         <v>503</v>
       </c>
     </row>
@@ -5049,66 +5058,64 @@
       <c r="B130" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="C130" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D130" s="8" t="s">
+      <c r="C130" s="11"/>
+      <c r="D130" s="11"/>
+      <c r="E130" s="8" t="s">
         <v>506</v>
       </c>
-      <c r="E130" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="G130" s="4" t="s">
-        <v>95</v>
+      <c r="F130" s="8" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C131" s="8" t="n">
-        <v>112</v>
+        <v>1000</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E131" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="F131" s="8" t="s">
-        <v>511</v>
+        <v>393</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="B132" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="B132" s="8" t="s">
-        <v>132</v>
-      </c>
       <c r="C132" s="8" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D132" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="D132" s="8" t="s">
+        <v>513</v>
+      </c>
       <c r="E132" s="8" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="F132" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>516</v>
+        <v>132</v>
       </c>
       <c r="C133" s="8" t="n">
-        <v>21</v>
+        <v>3100</v>
       </c>
       <c r="D133" s="8"/>
       <c r="E133" s="8" t="s">
@@ -5123,91 +5130,92 @@
         <v>519</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>293</v>
+        <v>520</v>
       </c>
       <c r="C134" s="8" t="n">
-        <v>122</v>
-      </c>
-      <c r="D134" s="8" t="s">
-        <v>520</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D134" s="8"/>
       <c r="E134" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="F134" s="2" t="s">
+      <c r="F134" s="8" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="135" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="10" t="s">
         <v>523</v>
       </c>
       <c r="B135" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C135" s="8" t="n">
+        <v>122</v>
+      </c>
+      <c r="D135" s="8" t="s">
         <v>524</v>
       </c>
-      <c r="C135" s="8" t="n">
+      <c r="E135" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="136" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="C136" s="8" t="n">
         <v>1722</v>
       </c>
-      <c r="D135" s="12" t="s">
-        <v>525</v>
-      </c>
-      <c r="E135" s="8" t="s">
-        <v>526</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="10" t="s">
-        <v>528</v>
-      </c>
-      <c r="B136" s="8" t="s">
+      <c r="D136" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="C136" s="8" t="n">
-        <v>7100</v>
-      </c>
-      <c r="D136" s="12"/>
       <c r="E136" s="8" t="s">
         <v>530</v>
       </c>
-      <c r="G136" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F136" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="10" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="C137" s="11"/>
-      <c r="D137" s="11"/>
+        <v>533</v>
+      </c>
+      <c r="C137" s="8" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D137" s="12"/>
       <c r="E137" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="F137" s="8"/>
+        <v>534</v>
+      </c>
       <c r="G137" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="B138" s="2" t="s">
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="C138" s="3" t="n">
-        <v>10900</v>
-      </c>
-      <c r="E138" s="2" t="s">
+      <c r="B138" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="F138" s="2" t="s">
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
+      <c r="E138" s="8" t="s">
         <v>537</v>
+      </c>
+      <c r="F138" s="8"/>
+      <c r="G138" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5217,40 +5225,41 @@
       <c r="B139" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="C139" s="3"/>
+      <c r="C139" s="3" t="n">
+        <v>10900</v>
+      </c>
       <c r="E139" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="F139" s="8" t="s">
+      <c r="F139" s="2" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>542</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="C140" s="3"/>
+      <c r="E140" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="E140" s="2" t="s">
+      <c r="F140" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="F140" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="G140" s="1"/>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="D141" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="C141" s="3"/>
       <c r="E141" s="2" t="s">
         <v>549</v>
       </c>
@@ -5259,17 +5268,17 @@
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="10" t="s">
+      <c r="A142" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="B142" s="8" t="s">
+      <c r="B142" s="2" t="s">
         <v>552</v>
       </c>
       <c r="C142" s="3"/>
-      <c r="E142" s="8" t="s">
+      <c r="E142" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="F142" s="9" t="s">
+      <c r="F142" s="8" t="s">
         <v>554</v>
       </c>
     </row>
@@ -5280,12 +5289,11 @@
       <c r="B143" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
+      <c r="C143" s="3"/>
       <c r="E143" s="8" t="s">
         <v>557</v>
       </c>
-      <c r="F143" s="8" t="s">
+      <c r="F143" s="9" t="s">
         <v>558</v>
       </c>
     </row>
@@ -5305,69 +5313,65 @@
         <v>562</v>
       </c>
     </row>
-    <row r="145" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="12" t="s">
+    <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="C145" s="3" t="n">
+      <c r="C145" s="11"/>
+      <c r="D145" s="11"/>
+      <c r="E145" s="8" t="s">
+        <v>565</v>
+      </c>
+      <c r="F145" s="8" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="146" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="C146" s="3" t="n">
         <v>10500</v>
       </c>
-      <c r="D145" s="3" t="s">
-        <v>565</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="F145" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="B146" s="8" t="s">
+      <c r="D146" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="C146" s="9" t="n">
+      <c r="E146" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B147" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="C147" s="9" t="n">
         <v>133</v>
       </c>
-      <c r="E146" s="8" t="s">
-        <v>570</v>
-      </c>
-      <c r="F146" s="9" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="10" t="s">
-        <v>572</v>
-      </c>
-      <c r="B147" s="8" t="s">
+      <c r="E147" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="F147" s="9" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="B148" s="8" t="s">
         <v>333</v>
-      </c>
-      <c r="C147" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D147" s="8" t="s">
-        <v>335</v>
-      </c>
-      <c r="E147" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="F147" s="8" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="B148" s="8" t="s">
-        <v>576</v>
       </c>
       <c r="C148" s="8" t="n">
         <v>400</v>
@@ -5378,117 +5382,119 @@
       <c r="E148" s="8" t="s">
         <v>577</v>
       </c>
-      <c r="F148" s="8"/>
-      <c r="G148" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F148" s="8" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="C149" s="9" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D149" s="9" t="s">
         <v>580</v>
+      </c>
+      <c r="C149" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D149" s="8" t="s">
+        <v>335</v>
       </c>
       <c r="E149" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="F149" s="8" t="s">
+      <c r="F149" s="8"/>
+      <c r="G149" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="150" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
+      <c r="B150" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="C150" s="9" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D150" s="9" t="s">
         <v>584</v>
       </c>
-      <c r="C150" s="14" t="n">
+      <c r="E150" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="F150" s="8" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="151" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="C151" s="14" t="n">
         <v>11100</v>
       </c>
-      <c r="D150" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="B151" s="8" t="s">
+      <c r="D151" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="C151" s="3"/>
-      <c r="E151" s="8" t="s">
+      <c r="E151" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="F151" s="9" t="s">
+      <c r="F151" s="2" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="10" t="s">
+      <c r="A152" s="1" t="s">
         <v>592</v>
       </c>
       <c r="B152" s="8" t="s">
         <v>593</v>
       </c>
-      <c r="C152" s="8" t="s">
+      <c r="C152" s="3"/>
+      <c r="E152" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="D152" s="8" t="s">
+      <c r="F152" s="9" t="s">
         <v>595</v>
-      </c>
-      <c r="E152" s="8" t="s">
-        <v>596</v>
-      </c>
-      <c r="F152" s="8" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
+        <v>596</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="C153" s="8" t="s">
         <v>598</v>
       </c>
-      <c r="B153" s="8" t="s">
+      <c r="D153" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="C153" s="11" t="s">
+      <c r="E153" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="D153" s="11" t="s">
+      <c r="F153" s="8" t="s">
         <v>601</v>
-      </c>
-      <c r="E153" s="8" t="s">
-        <v>602</v>
-      </c>
-      <c r="F153" s="8" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="C154" s="11" t="s">
         <v>604</v>
       </c>
-      <c r="B154" s="8" t="s">
+      <c r="D154" s="11" t="s">
         <v>605</v>
       </c>
-      <c r="C154" s="8" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D154" s="8"/>
       <c r="E154" s="8" t="s">
         <v>606</v>
       </c>
@@ -5501,12 +5507,12 @@
         <v>608</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C155" s="11"/>
-      <c r="D155" s="11" t="s">
         <v>609</v>
       </c>
+      <c r="C155" s="8" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D155" s="8"/>
       <c r="E155" s="8" t="s">
         <v>610</v>
       </c>
@@ -5519,12 +5525,10 @@
         <v>612</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C156" s="8" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D156" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11" t="s">
         <v>613</v>
       </c>
       <c r="E156" s="8" t="s">
@@ -5539,47 +5543,51 @@
         <v>616</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="C157" s="11"/>
-      <c r="D157" s="11"/>
+        <v>214</v>
+      </c>
+      <c r="C157" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D157" s="8" t="s">
+        <v>617</v>
+      </c>
       <c r="E157" s="8" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>619</v>
+        <v>269</v>
       </c>
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
       <c r="E158" s="8" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C159" s="11"/>
       <c r="D159" s="11"/>
       <c r="E159" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5587,23 +5595,23 @@
         <v>625</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="C160" s="11"/>
       <c r="D160" s="11"/>
       <c r="E160" s="8" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C161" s="11"/>
       <c r="D161" s="11"/>
@@ -5621,110 +5629,106 @@
       <c r="B162" s="8" t="s">
         <v>633</v>
       </c>
-      <c r="C162" s="8" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D162" s="8" t="s">
+      <c r="C162" s="11"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="8" t="s">
         <v>634</v>
       </c>
-      <c r="E162" s="8" t="s">
+      <c r="F162" s="8" t="s">
         <v>635</v>
-      </c>
-      <c r="F162" s="8" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
+        <v>636</v>
+      </c>
+      <c r="B163" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="C163" s="8" t="n">
+        <v>7700</v>
+      </c>
+      <c r="D163" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="C163" s="8" t="n">
+      <c r="E163" s="8" t="s">
+        <v>639</v>
+      </c>
+      <c r="F163" s="8" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="10" t="s">
+        <v>641</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C164" s="8" t="n">
         <v>7800</v>
       </c>
-      <c r="D163" s="8" t="s">
-        <v>639</v>
-      </c>
-      <c r="E163" s="8" t="s">
+      <c r="D164" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="E164" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="F164" s="8" t="s">
         <v>640</v>
       </c>
-      <c r="F163" s="8" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="164" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="B164" s="17" t="s">
-        <v>642</v>
-      </c>
-      <c r="C164" s="14" t="n">
+    </row>
+    <row r="165" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B165" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="C165" s="14" t="n">
         <v>10300</v>
       </c>
-      <c r="D164" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="E164" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="F164" s="2" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="10" t="s">
-        <v>646</v>
-      </c>
-      <c r="B165" s="8" t="s">
+      <c r="D165" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="C165" s="11"/>
-      <c r="D165" s="11"/>
-      <c r="E165" s="8" t="s">
+      <c r="E165" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="F165" s="8" t="s">
+      <c r="F165" s="2" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="s">
+      <c r="A166" s="10" t="s">
         <v>650</v>
       </c>
       <c r="B166" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="C166" s="9" t="n">
+      <c r="C166" s="11"/>
+      <c r="D166" s="11"/>
+      <c r="E166" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="F166" s="8" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="C167" s="9" t="n">
         <v>8900</v>
       </c>
-      <c r="E166" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="G166" s="4" t="s">
+      <c r="E167" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="G167" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="10" t="s">
-        <v>653</v>
-      </c>
-      <c r="B167" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C167" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="D167" s="11" t="s">
-        <v>654</v>
-      </c>
-      <c r="E167" s="8" t="s">
-        <v>655</v>
-      </c>
-      <c r="F167" s="8" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5732,72 +5736,74 @@
         <v>657</v>
       </c>
       <c r="B168" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C168" s="11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D168" s="11" t="s">
         <v>658</v>
       </c>
-      <c r="C168" s="11"/>
-      <c r="D168" s="11" t="s">
+      <c r="E168" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="E168" s="8" t="s">
+      <c r="F168" s="8" t="s">
         <v>660</v>
       </c>
-      <c r="F168" s="8" t="s">
+    </row>
+    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="10" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="169" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="10" t="s">
+      <c r="B169" s="8" t="s">
         <v>662</v>
       </c>
-      <c r="B169" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="C169" s="8" t="n">
+      <c r="C169" s="11"/>
+      <c r="D169" s="11" t="s">
+        <v>663</v>
+      </c>
+      <c r="E169" s="8" t="s">
+        <v>664</v>
+      </c>
+      <c r="F169" s="8" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="170" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="C170" s="8" t="n">
         <v>101</v>
       </c>
-      <c r="D169" s="12" t="s">
-        <v>492</v>
-      </c>
-      <c r="E169" s="8" t="s">
-        <v>493</v>
-      </c>
-      <c r="F169" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="10" t="s">
-        <v>663</v>
-      </c>
-      <c r="B170" s="8" t="s">
+      <c r="D170" s="12" t="s">
+        <v>496</v>
+      </c>
+      <c r="E170" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="B171" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="C170" s="11"/>
-      <c r="D170" s="11"/>
-      <c r="E170" s="8" t="s">
-        <v>664</v>
-      </c>
-      <c r="F170" s="8"/>
-      <c r="G170" s="4" t="s">
+      <c r="C171" s="11"/>
+      <c r="D171" s="11"/>
+      <c r="E171" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="F171" s="8"/>
+      <c r="G171" s="4" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="10" t="s">
-        <v>665</v>
-      </c>
-      <c r="B171" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C171" s="11"/>
-      <c r="D171" s="11" t="s">
-        <v>666</v>
-      </c>
-      <c r="E171" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="F171" s="8" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,30 +5811,28 @@
         <v>669</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="C172" s="8" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D172" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="C172" s="11"/>
+      <c r="D172" s="11" t="s">
         <v>670</v>
       </c>
       <c r="E172" s="8" t="s">
         <v>671</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="s">
-        <v>672</v>
+      <c r="A173" s="10" t="s">
+        <v>673</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>673</v>
+        <v>269</v>
       </c>
       <c r="C173" s="8" t="n">
-        <v>7400</v>
+        <v>1400</v>
       </c>
       <c r="D173" s="8" t="s">
         <v>674</v>
@@ -5837,25 +5841,27 @@
         <v>675</v>
       </c>
       <c r="F173" s="8" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="10" t="s">
+      <c r="B174" s="8" t="s">
         <v>677</v>
       </c>
-      <c r="B174" s="8" t="s">
+      <c r="C174" s="8" t="n">
+        <v>7400</v>
+      </c>
+      <c r="D174" s="8" t="s">
         <v>678</v>
       </c>
-      <c r="C174" s="11"/>
-      <c r="D174" s="11" t="s">
+      <c r="E174" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="E174" s="8" t="s">
+      <c r="F174" s="8" t="s">
         <v>680</v>
-      </c>
-      <c r="F174" s="8" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5863,30 +5869,28 @@
         <v>681</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>622</v>
-      </c>
-      <c r="C175" s="8" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D175" s="8" t="s">
         <v>682</v>
       </c>
+      <c r="C175" s="11"/>
+      <c r="D175" s="11" t="s">
+        <v>683</v>
+      </c>
       <c r="E175" s="8" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>685</v>
+        <v>626</v>
       </c>
       <c r="C176" s="8" t="n">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="D176" s="8" t="s">
         <v>686</v>
@@ -5895,42 +5899,42 @@
         <v>687</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>688</v>
+        <v>672</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
+        <v>688</v>
+      </c>
+      <c r="B177" s="8" t="s">
         <v>689</v>
       </c>
-      <c r="B177" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="C177" s="3"/>
+      <c r="C177" s="8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D177" s="8" t="s">
+        <v>690</v>
+      </c>
       <c r="E177" s="8" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="C178" s="11" t="s">
-        <v>693</v>
-      </c>
-      <c r="D178" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C178" s="3"/>
+      <c r="E178" s="8" t="s">
         <v>694</v>
       </c>
-      <c r="E178" s="8" t="s">
+      <c r="F178" s="8" t="s">
         <v>695</v>
-      </c>
-      <c r="F178" s="8" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5938,62 +5942,64 @@
         <v>696</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>678</v>
-      </c>
-      <c r="C179" s="11"/>
-      <c r="D179" s="11"/>
+        <v>269</v>
+      </c>
+      <c r="C179" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="D179" s="11" t="s">
+        <v>698</v>
+      </c>
       <c r="E179" s="8" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>622</v>
+        <v>682</v>
       </c>
       <c r="C180" s="11"/>
-      <c r="D180" s="11" t="s">
-        <v>699</v>
-      </c>
+      <c r="D180" s="11"/>
       <c r="E180" s="8" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="B181" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="10" t="s">
         <v>702</v>
       </c>
-      <c r="D181" s="3" t="s">
+      <c r="B181" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="C181" s="11"/>
+      <c r="D181" s="11" t="s">
         <v>703</v>
       </c>
-      <c r="E181" s="2" t="s">
+      <c r="E181" s="8" t="s">
         <v>704</v>
       </c>
-      <c r="F181" s="2" t="s">
+      <c r="F181" s="8" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="G181" s="1"/>
-    </row>
-    <row r="182" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="s">
+      <c r="B182" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="D182" s="3" t="s">
         <v>707</v>
-      </c>
-      <c r="C182" s="14" t="n">
-        <v>10100</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>708</v>
@@ -6002,19 +6008,20 @@
         <v>709</v>
       </c>
     </row>
-    <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="10" t="s">
+    <row r="183" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="B183" s="8" t="s">
+      <c r="B183" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="C183" s="11"/>
-      <c r="D183" s="11"/>
-      <c r="E183" s="8" t="s">
+      <c r="C183" s="14" t="n">
+        <v>10100</v>
+      </c>
+      <c r="E183" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="F183" s="8" t="s">
+      <c r="F183" s="2" t="s">
         <v>713</v>
       </c>
     </row>
@@ -6023,266 +6030,264 @@
         <v>714</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>678</v>
+        <v>715</v>
       </c>
       <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="8" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>622</v>
+        <v>682</v>
       </c>
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="F185" s="8" t="s">
         <v>717</v>
-      </c>
-      <c r="F185" s="8" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>269</v>
+        <v>626</v>
       </c>
       <c r="C186" s="11"/>
-      <c r="D186" s="11" t="s">
-        <v>719</v>
-      </c>
+      <c r="D186" s="11"/>
       <c r="E186" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>211</v>
+        <v>269</v>
       </c>
       <c r="C187" s="11"/>
-      <c r="D187" s="11"/>
+      <c r="D187" s="11" t="s">
+        <v>723</v>
+      </c>
       <c r="E187" s="8" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="8" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>296</v>
+        <v>214</v>
       </c>
       <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="8" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>622</v>
+        <v>296</v>
       </c>
       <c r="C190" s="11"/>
-      <c r="D190" s="11" t="s">
-        <v>728</v>
-      </c>
+      <c r="D190" s="11"/>
       <c r="E190" s="8" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>211</v>
+        <v>626</v>
       </c>
       <c r="C191" s="11"/>
-      <c r="D191" s="11"/>
+      <c r="D191" s="11" t="s">
+        <v>732</v>
+      </c>
       <c r="E191" s="8" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C192" s="11"/>
       <c r="D192" s="11"/>
       <c r="E192" s="8" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>296</v>
+        <v>214</v>
       </c>
       <c r="C193" s="11"/>
       <c r="D193" s="11"/>
       <c r="E193" s="8" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
       <c r="C194" s="11"/>
       <c r="D194" s="11"/>
       <c r="E194" s="8" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>678</v>
+        <v>269</v>
       </c>
       <c r="C195" s="11"/>
       <c r="D195" s="11"/>
       <c r="E195" s="8" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="1" t="s">
-        <v>740</v>
+      <c r="A196" s="10" t="s">
+        <v>742</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>741</v>
-      </c>
-      <c r="C196" s="9" t="n">
-        <v>23</v>
-      </c>
+        <v>682</v>
+      </c>
+      <c r="C196" s="11"/>
+      <c r="D196" s="11"/>
       <c r="E196" s="8" t="s">
-        <v>742</v>
-      </c>
-      <c r="F196" s="9" t="s">
         <v>743</v>
       </c>
+      <c r="F196" s="8" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="10" t="s">
+      <c r="A197" s="1" t="s">
         <v>744</v>
       </c>
       <c r="B197" s="8" t="s">
         <v>745</v>
       </c>
-      <c r="C197" s="8" t="n">
-        <v>121</v>
-      </c>
-      <c r="D197" s="8"/>
+      <c r="C197" s="9" t="n">
+        <v>23</v>
+      </c>
       <c r="E197" s="8" t="s">
         <v>746</v>
       </c>
-      <c r="G197" s="4" t="s">
-        <v>95</v>
+      <c r="F197" s="9" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>748</v>
-      </c>
-      <c r="C198" s="11"/>
-      <c r="D198" s="11" t="s">
         <v>749</v>
       </c>
+      <c r="C198" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="D198" s="8"/>
       <c r="E198" s="8" t="s">
         <v>750</v>
       </c>
-      <c r="F198" s="8" t="s">
-        <v>751</v>
+      <c r="G198" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
+        <v>751</v>
+      </c>
+      <c r="B199" s="8" t="s">
         <v>752</v>
-      </c>
-      <c r="B199" s="8" t="s">
-        <v>753</v>
       </c>
       <c r="C199" s="11"/>
       <c r="D199" s="11" t="s">
+        <v>753</v>
+      </c>
+      <c r="E199" s="8" t="s">
         <v>754</v>
       </c>
-      <c r="E199" s="8" t="s">
+      <c r="F199" s="8" t="s">
         <v>755</v>
-      </c>
-      <c r="F199" s="8" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6290,233 +6295,233 @@
         <v>756</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>496</v>
-      </c>
-      <c r="C200" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D200" s="8" t="s">
-        <v>497</v>
+        <v>757</v>
+      </c>
+      <c r="C200" s="11"/>
+      <c r="D200" s="11" t="s">
+        <v>758</v>
       </c>
       <c r="E200" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="F200" s="2" t="s">
-        <v>499</v>
+        <v>759</v>
+      </c>
+      <c r="F200" s="8" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
       <c r="B201" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="C201" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D201" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="E201" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="10" t="s">
+        <v>761</v>
+      </c>
+      <c r="B202" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="C201" s="8" t="n">
+      <c r="C202" s="8" t="n">
         <v>1711</v>
       </c>
-      <c r="D201" s="8" t="s">
+      <c r="D202" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="E201" s="8" t="s">
+      <c r="E202" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="F201" s="8" t="s">
+      <c r="F202" s="8" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="B202" s="8" t="s">
-        <v>759</v>
-      </c>
-      <c r="C202" s="8" t="n">
+    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>763</v>
+      </c>
+      <c r="C203" s="8" t="n">
         <v>3300</v>
       </c>
-      <c r="D202" s="8" t="s">
-        <v>760</v>
-      </c>
-      <c r="E202" s="8" t="s">
-        <v>761</v>
-      </c>
-      <c r="F202" s="8" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="10" t="s">
-        <v>763</v>
-      </c>
-      <c r="B203" s="8" t="s">
+      <c r="D203" s="8" t="s">
         <v>764</v>
       </c>
-      <c r="C203" s="8" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D203" s="8" t="s">
+      <c r="E203" s="8" t="s">
         <v>765</v>
       </c>
-      <c r="E203" s="8" t="s">
+      <c r="F203" s="8" t="s">
         <v>766</v>
-      </c>
-      <c r="F203" s="8" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="B204" s="8" t="s">
         <v>768</v>
       </c>
-      <c r="B204" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C204" s="11"/>
-      <c r="D204" s="11"/>
+      <c r="C204" s="8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D204" s="8" t="s">
+        <v>769</v>
+      </c>
       <c r="E204" s="8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C205" s="11"/>
       <c r="D205" s="11"/>
       <c r="E205" s="8" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
     </row>
     <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B206" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C206" s="11"/>
+      <c r="D206" s="11"/>
+      <c r="E206" s="8" t="s">
+        <v>776</v>
+      </c>
+      <c r="F206" s="8" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="B207" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="C206" s="11"/>
-      <c r="D206" s="11" t="s">
+      <c r="C207" s="11"/>
+      <c r="D207" s="11" t="s">
+        <v>778</v>
+      </c>
+      <c r="E207" s="8" t="s">
+        <v>779</v>
+      </c>
+      <c r="F207" s="8" t="s">
         <v>774</v>
       </c>
-      <c r="E206" s="8" t="s">
-        <v>775</v>
-      </c>
-      <c r="F206" s="8" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="207" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="10" t="s">
-        <v>776</v>
-      </c>
-      <c r="B207" s="8" t="s">
+    </row>
+    <row r="208" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="B208" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="C207" s="8" t="n">
+      <c r="C208" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="D207" s="12" t="s">
+      <c r="D208" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="E207" s="8" t="s">
-        <v>777</v>
-      </c>
-      <c r="F207" s="8" t="s">
+      <c r="E208" s="8" t="s">
+        <v>781</v>
+      </c>
+      <c r="F208" s="8" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="10" t="s">
-        <v>778</v>
-      </c>
-      <c r="B208" s="8" t="s">
-        <v>779</v>
-      </c>
-      <c r="C208" s="8" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D208" s="8"/>
-      <c r="E208" s="8" t="s">
-        <v>780</v>
-      </c>
-      <c r="G208" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C209" s="8" t="n">
-        <v>2711</v>
+        <v>2611</v>
       </c>
       <c r="D209" s="8"/>
       <c r="E209" s="8" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="G209" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="10" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="C210" s="11"/>
-      <c r="D210" s="11"/>
+        <v>786</v>
+      </c>
+      <c r="C210" s="8" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D210" s="8"/>
       <c r="E210" s="8" t="s">
-        <v>785</v>
-      </c>
-      <c r="F210" s="8"/>
+        <v>787</v>
+      </c>
       <c r="G210" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="10" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>787</v>
+        <v>269</v>
       </c>
       <c r="C211" s="11"/>
-      <c r="D211" s="11" t="s">
-        <v>788</v>
-      </c>
+      <c r="D211" s="11"/>
       <c r="E211" s="8" t="s">
         <v>789</v>
       </c>
-      <c r="F211" s="8" t="s">
-        <v>790</v>
+      <c r="F211" s="8"/>
+      <c r="G211" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="B212" s="8" t="s">
         <v>791</v>
       </c>
-      <c r="B212" s="8" t="s">
+      <c r="C212" s="11"/>
+      <c r="D212" s="11" t="s">
         <v>792</v>
       </c>
-      <c r="C212" s="8" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D212" s="8"/>
       <c r="E212" s="8" t="s">
         <v>793</v>
       </c>
@@ -6529,14 +6534,12 @@
         <v>795</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>622</v>
+        <v>796</v>
       </c>
       <c r="C213" s="8" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D213" s="8" t="s">
-        <v>796</v>
-      </c>
+        <v>3721</v>
+      </c>
+      <c r="D213" s="8"/>
       <c r="E213" s="8" t="s">
         <v>797</v>
       </c>
@@ -6549,63 +6552,62 @@
         <v>799</v>
       </c>
       <c r="B214" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="C214" s="8" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D214" s="8" t="s">
         <v>800</v>
       </c>
-      <c r="C214" s="11" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D214" s="11" t="s">
+      <c r="E214" s="8" t="s">
         <v>801</v>
       </c>
-      <c r="E214" s="8" t="s">
+      <c r="F214" s="8" t="s">
         <v>802</v>
-      </c>
-      <c r="F214" s="8" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="10" t="s">
+        <v>803</v>
+      </c>
+      <c r="B215" s="8" t="s">
         <v>804</v>
       </c>
-      <c r="B215" s="8" t="s">
+      <c r="C215" s="11" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D215" s="11" t="s">
+        <v>805</v>
+      </c>
+      <c r="E215" s="8" t="s">
+        <v>806</v>
+      </c>
+      <c r="F215" s="8" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="216" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="10" t="s">
+        <v>808</v>
+      </c>
+      <c r="B216" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C215" s="3"/>
-      <c r="E215" s="8" t="s">
-        <v>805</v>
-      </c>
-      <c r="F215" s="8" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="B216" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="C216" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D216" s="8" t="s">
-        <v>335</v>
-      </c>
+      <c r="C216" s="3"/>
       <c r="E216" s="8" t="s">
-        <v>808</v>
-      </c>
-      <c r="F216" s="8"/>
-      <c r="G216" s="4" t="s">
-        <v>95</v>
+        <v>809</v>
+      </c>
+      <c r="F216" s="8" t="s">
+        <v>810</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>576</v>
+        <v>333</v>
       </c>
       <c r="C217" s="8" t="n">
         <v>400</v>
@@ -6614,58 +6616,79 @@
         <v>335</v>
       </c>
       <c r="E217" s="8" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="F217" s="8"/>
       <c r="G217" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="218" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="10" t="s">
-        <v>811</v>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>813</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C218" s="11"/>
-      <c r="D218" s="11"/>
+        <v>580</v>
+      </c>
+      <c r="C218" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D218" s="8" t="s">
+        <v>335</v>
+      </c>
       <c r="E218" s="8" t="s">
-        <v>812</v>
-      </c>
-      <c r="F218" s="8" t="s">
-        <v>813</v>
+        <v>814</v>
+      </c>
+      <c r="F218" s="8"/>
+      <c r="G218" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="219" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="10" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="C219" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="C219" s="11"/>
+      <c r="D219" s="11"/>
+      <c r="E219" s="8" t="s">
+        <v>816</v>
+      </c>
+      <c r="F219" s="8" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="220" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="C220" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="D219" s="8"/>
-      <c r="E219" s="8" t="s">
-        <v>815</v>
-      </c>
-      <c r="G219" s="4" t="s">
+      <c r="D220" s="8"/>
+      <c r="E220" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="G220" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="B220" s="8" t="s">
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B221" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="E220" s="8" t="s">
-        <v>817</v>
-      </c>
-      <c r="F220" s="8"/>
+      <c r="E221" s="8" t="s">
+        <v>821</v>
+      </c>
+      <c r="F221" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>